<commit_message>
get rid of pounds
</commit_message>
<xml_diff>
--- a/data/tech_guidance.xlsx
+++ b/data/tech_guidance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/sarah_wong_education_gov_uk/Documents/Documents/RAP/la_scorecards/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/sarah_wong_education_gov_uk/Documents/Documents/RAP/la-school-places-scorecards/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="8_{9B79E267-60E7-4A31-9325-0F758DA50D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{057813C6-65ED-4111-BE3E-1985EC36376F}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="8_{9B79E267-60E7-4A31-9325-0F758DA50D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D75B0836-A6EA-4BAD-92E1-C1AE37C741F0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{9CCC1F63-2262-45DD-B4CA-7C937E5C8E7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9CCC1F63-2262-45DD-B4CA-7C937E5C8E7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="1" r:id="rId1"/>
@@ -422,224 +422,6 @@
 &lt;br&gt; and the average cost per place of new school projects delivered by the selected local authority;</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">1. No cost data was collected in 2019 as the Capital Spend data collection was removed from the SCAP survey pending the introduction of the Capital Spend Survey. The most recent cost data available is the 2018 Capital Spend data as used in the 2018 Scorecard. For the 2019 Scorecard, this data has been adjusted for inflation (rebased to 1st Quarter 2020 prices). </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">You can use this data to establish developer contributions per school place by adjusting the national average (for a chosen project type/phase) for region, and adjusting for further inflation if needed </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(see examples below).
-&lt;br&gt;2. Projects which do not create additional mainstream places or where the project's additional place funding is zero are removed. After further investigation, three projects were removed from the 2018 Scorecards cost data for use in the 2019 Scorecards as the projects' additional place funding was zero.
-&lt;br&gt;3. Projects were identified as primary phase or secondary phase based on additional mainstream place year group breakdown. Where a project created places across the primary and secondary phases, the project was assigned a phase corresponding to the phase of the school it affected (i.e. if its school was middle-deemed primary - the project was assigned to primary).
-&lt;br&gt;4. Average cost per place figures for all-through, middle-deemed primary and middle-deemed secondary schools have not been calculated separately due to low sample sizes for these project types. </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>To estimate average cost per place for middle-deemed primary schools, we recommend using primary average cost per place</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> as the middle school provides education equivalent to the education a primary school provides for all year groups. </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>To estimate average cost per place for middle-deemed secondary schools, we recommend using secondary average cost per place</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> for the same reason. </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>For new middle schools or whole school expansions for middle schools not ‘deemed’ primary or secondary, we recommend taking a mid-point of the primary and secondary costs if the project covers both primary- and secondary-equivalent year groups equally</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (e.g. 2 classes per Year 5 &amp; 6 and 2 classes per Year 7 &amp; 8). </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>If the project only covers certain year groups, we recommend using primary cost data if only primary-equivalent years groups are expanding</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (e.g. Years 5 &amp; 6) and </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>secondary data if only secondary-equivalent year groups are expanding</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (e.g. Years 7 &amp; 8).
-&lt;br&gt;5. The average cost does not include costs associated with land acquisition.
-&lt;br&gt;6. The average cost includes costs associated with maintenance and building condition or enhancement works.
-&lt;br&gt;7. The measure does not include places in special schools or units attached to mainstream schools, or new places which were funded through central programmes (including free schools). Where a project creates additional mainstream places and also creates SEN places or re-provides places, an adjustment has been applied to apportion out those costs. 
-&lt;br&gt;8. All costs have been normalised to a common UK average price level using regional location factors published by Building Cost Information Service (BCIS), December 2015, 1 is the base weight.
-&lt;br&gt;9. All costs have been adjusted for inflation using the latest Building Cost Information Service (BCIS) All-In Tender Price of Index (TPI), published March 2020.  Costs have been rebased from the start of construction (or time of place provision if construction start date unavailable) to 1st Quarter (Jan – Mar) 2020 prices using this index (Q1 2020 index value = 335).
-&lt;br&gt;10. </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>To adjust the national average to the region of interest, divide the national average cost by the weight for the region, given in the Scorecard underlying data</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (the regional weight has been calculated using the regional location factors mentioned above).
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Example: New primary school in Outer London.  
-National average for primary new schools = £20,508
-Outer London weight = 0.820 (Base weight of 1.00/Outer London location factor of 1.22).
-Average primary New School cost that applies to Outer London in Q1 2020 prices =  £20,508 ÷ 0.820 = £25,000 (rounded to nearest £100).
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-11. </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>To adjust the national average to current or future prices, you need to uprate or downrate the prices in this scorecard relative to the change that has happened since Q1 2020</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.  If you have access to the BCIS indices via a subscription to BCIS Online (https://www.rics.org/uk/products/data-products/bcis-construction/bcis-online/) you can use the latest inflation index to re-base (weight to apply = latest index/335).  If not, you can apply a known change to the published cost (e.g. up or down x%).
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Example: New primary school in Outer London Q3 (Jul - Sep) 2021.  
-National average for primary new schools = £20,508.  
-Outer London weight = 0.820.  
-Inflation weight = 342/335 = 1.021 (taken from BCIS All-In TPI published March 2020). 
-Average primary New School cost that applies to Outer London in Q3 2021 prices = £20,508 ÷ 0.820 x 1.021 = £25,500 (rounded to nearest £100).  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-If you do not have access the BCIS index, but sources say TPI inflation is set to increase by 4% per annum, then approximate inflation weight = 6% (18 months’ worth of inflation) = 1.06.
-12. Some additional but limited benchmark information for similar capital programme schemes carried out by the DfE is available in the National School Delivery Cost Benchmarking study (https://ebdog.org.uk/wp-content/uploads/2019/06/F07125-National-School-Delivery-Cost-Benchmarking-Primary-Secondary-and--SEN-Schools-Final-June-2019-v6.7a.pdf).</t>
-    </r>
-  </si>
-  <si>
     <t>The total number of new places planned for delivery from 2019/20 to 2021/22;
 &lt;br&gt;The number of places planned for delivery contains four elements: 
 &lt;br&gt;1) local authority firm plans for  new permanent additional places and new temporary bulge places’,
@@ -756,6 +538,30 @@
     <t>1. The quality rating of the places created is either the Ofsted judgment, the key stage 2 reading or maths progress measures (primary only) or the key stage 4 progress 8 score category (secondary only).
 &lt;br&gt;2. The quality of new places amongst the relevant quality categories for the selected authority is presented.
 &lt;br&gt;3. The quality rating of the places present in the school capacity collection 2019 that were also present in the school capacity collection 2018 is presented as the existing places.</t>
+  </si>
+  <si>
+    <t>1. No cost data was collected in 2019 as the Capital Spend data collection was removed from the SCAP survey pending the introduction of the Capital Spend Survey. The most recent cost data available is the 2018 Capital Spend data as used in the 2018 Scorecard. For the 2019 Scorecard, this data has been adjusted for inflation (rebased to 1st Quarter 2020 prices). You can use this data to establish developer contributions per school place by adjusting the national average (for a chosen project type/phase) for region, and adjusting for further inflation if needed (see examples below).
+&lt;br&gt;2. Projects which do not create additional mainstream places or where the project's additional place funding is zero are removed. After further investigation, three projects were removed from the 2018 Scorecards cost data for use in the 2019 Scorecards as the projects' additional place funding was zero.
+&lt;br&gt;3. Projects were identified as primary phase or secondary phase based on additional mainstream place year group breakdown. Where a project created places across the primary and secondary phases, the project was assigned a phase corresponding to the phase of the school it affected (i.e. if its school was middle-deemed primary - the project was assigned to primary).
+&lt;br&gt;4. Average cost per place figures for all-through, middle-deemed primary and middle-deemed secondary schools have not been calculated separately due to low sample sizes for these project types. To estimate average cost per place for middle-deemed primary schools, we recommend using primary average cost per place as the middle school provides education equivalent to the education a primary school provides for all year groups. To estimate average cost per place for middle-deemed secondary schools, we recommend using secondary average cost per place for the same reason. For new middle schools or whole school expansions for middle schools not ‘deemed’ primary or secondary, we recommend taking a mid-point of the primary and secondary costs if the project covers both primary- and secondary-equivalent year groups equally (e.g. 2 classes per Year 5 &amp; 6 and 2 classes per Year 7 &amp; 8). If the project only covers certain year groups, we recommend using primary cost data if only primary-equivalent years groups are expanding (e.g. Years 5 &amp; 6) and secondary data if only secondary-equivalent year groups are expanding (e.g. Years 7 &amp; 8).
+&lt;br&gt;5. The average cost does not include costs associated with land acquisition.
+&lt;br&gt;6. The average cost includes costs associated with maintenance and building condition or enhancement works.
+&lt;br&gt;7. The measure does not include places in special schools or units attached to mainstream schools, or new places which were funded through central programmes (including free schools). Where a project creates additional mainstream places and also creates SEN places or re-provides places, an adjustment has been applied to apportion out those costs. 
+&lt;br&gt;8. All costs have been normalised to a common UK average price level using regional location factors published by Building Cost Information Service (BCIS), December 2015, 1 is the base weight.
+&lt;br&gt;9. All costs have been adjusted for inflation using the latest Building Cost Information Service (BCIS) All-In Tender Price of Index (TPI), published March 2020.  Costs have been rebased from the start of construction (or time of place provision if construction start date unavailable) to 1st Quarter (Jan – Mar) 2020 prices using this index (Q1 2020 index value = 335).
+&lt;br&gt;10. To adjust the national average to the region of interest, divide the national average cost by the weight for the region, given in the Scorecard underlying data (the regional weight has been calculated using the regional location factors mentioned above).
+Example: New primary school in Outer London.  
+National average for primary new schools = 20,508
+Outer London weight = 0.820 (Base weight of 1.00/Outer London location factor of 1.22).
+Average primary New School cost that applies to Outer London in Q1 2020 prices =  20,508 ÷ 0.820 = 25,000 (rounded to nearest 100).
+11. To adjust the national average to current or future prices, you need to uprate or downrate the prices in this scorecard relative to the change that has happened since Q1 2020.  If you have access to the BCIS indices via a subscription to BCIS Online (https://www.rics.org/uk/products/data-products/bcis-construction/bcis-online/) you can use the latest inflation index to re-base (weight to apply = latest index/335).  If not, you can apply a known change to the published cost (e.g. up or down x%).
+Example: New primary school in Outer London Q3 (Jul - Sep) 2021.  
+National average for primary new schools = 20,508.  
+Outer London weight = 0.820.  
+Inflation weight = 342/335 = 1.021 (taken from BCIS All-In TPI published March 2020). 
+Average primary New School cost that applies to Outer London in Q3 2021 prices = 20,508 ÷ 0.820 x 1.021 = 25,500 (rounded to nearest 100).  
+If you do not have access the BCIS index, but sources say TPI inflation is set to increase by 4% per annum, then approximate inflation weight = 6% (18 months’ worth of inflation) = 1.06.
+12. Some additional but limited benchmark information for similar capital programme schemes carried out by the DfE is available in the National School Delivery Cost Benchmarking study (https://ebdog.org.uk/wp-content/uploads/2019/06/F07125-National-School-Delivery-Cost-Benchmarking-Primary-Secondary-and--SEN-Schools-Final-June-2019-v6.7a.pdf).</t>
   </si>
 </sst>
 </file>
@@ -1557,8 +1363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C67D23D-5B13-4F00-9F83-043839CEFFD1}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1690,7 +1496,7 @@
         <v>14</v>
       </c>
       <c r="E2" s="48" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1709,7 +1515,7 @@
         <v>74</v>
       </c>
       <c r="B4" s="45" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>17</v>
@@ -1718,7 +1524,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="38" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1744,7 +1550,7 @@
         <v>20</v>
       </c>
       <c r="E6" s="38" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1768,7 +1574,7 @@
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1785,7 +1591,7 @@
         <v>27</v>
       </c>
       <c r="E9" s="45" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1813,7 +1619,7 @@
         <v>30</v>
       </c>
       <c r="E11" s="45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1839,7 +1645,7 @@
         <v>35</v>
       </c>
       <c r="E13" s="45" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1939,7 +1745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{172A91E8-EE08-4774-802F-E9F4C78EAB63}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A10" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -1982,7 +1788,7 @@
         <v>42</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2010,7 +1816,7 @@
         <v>47</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2121,7 +1927,7 @@
       </c>
       <c r="D13" s="30"/>
       <c r="E13" s="30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2220,7 +2026,7 @@
         <v>69</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add pounds back in, csv as utf-8
</commit_message>
<xml_diff>
--- a/data/tech_guidance.xlsx
+++ b/data/tech_guidance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/sarah_wong_education_gov_uk/Documents/Documents/RAP/la-school-places-scorecards/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="70" documentId="8_{9B79E267-60E7-4A31-9325-0F758DA50D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D75B0836-A6EA-4BAD-92E1-C1AE37C741F0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA473C83-A5B5-41C2-BF57-9EB551CBA1C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9CCC1F63-2262-45DD-B4CA-7C937E5C8E7F}"/>
   </bookViews>
@@ -422,6 +422,224 @@
 &lt;br&gt; and the average cost per place of new school projects delivered by the selected local authority;</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">1. No cost data was collected in 2019 as the Capital Spend data collection was removed from the SCAP survey pending the introduction of the Capital Spend Survey. The most recent cost data available is the 2018 Capital Spend data as used in the 2018 Scorecard. For the 2019 Scorecard, this data has been adjusted for inflation (rebased to 1st Quarter 2020 prices). </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">You can use this data to establish developer contributions per school place by adjusting the national average (for a chosen project type/phase) for region, and adjusting for further inflation if needed </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(see examples below).
+&lt;br&gt;2. Projects which do not create additional mainstream places or where the project's additional place funding is zero are removed. After further investigation, three projects were removed from the 2018 Scorecards cost data for use in the 2019 Scorecards as the projects' additional place funding was zero.
+&lt;br&gt;3. Projects were identified as primary phase or secondary phase based on additional mainstream place year group breakdown. Where a project created places across the primary and secondary phases, the project was assigned a phase corresponding to the phase of the school it affected (i.e. if its school was middle-deemed primary - the project was assigned to primary).
+&lt;br&gt;4. Average cost per place figures for all-through, middle-deemed primary and middle-deemed secondary schools have not been calculated separately due to low sample sizes for these project types. </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>To estimate average cost per place for middle-deemed primary schools, we recommend using primary average cost per place</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> as the middle school provides education equivalent to the education a primary school provides for all year groups. </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>To estimate average cost per place for middle-deemed secondary schools, we recommend using secondary average cost per place</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for the same reason. </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>For new middle schools or whole school expansions for middle schools not ‘deemed’ primary or secondary, we recommend taking a mid-point of the primary and secondary costs if the project covers both primary- and secondary-equivalent year groups equally</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (e.g. 2 classes per Year 5 &amp; 6 and 2 classes per Year 7 &amp; 8). </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If the project only covers certain year groups, we recommend using primary cost data if only primary-equivalent years groups are expanding</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (e.g. Years 5 &amp; 6) and </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>secondary data if only secondary-equivalent year groups are expanding</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (e.g. Years 7 &amp; 8).
+&lt;br&gt;5. The average cost does not include costs associated with land acquisition.
+&lt;br&gt;6. The average cost includes costs associated with maintenance and building condition or enhancement works.
+&lt;br&gt;7. The measure does not include places in special schools or units attached to mainstream schools, or new places which were funded through central programmes (including free schools). Where a project creates additional mainstream places and also creates SEN places or re-provides places, an adjustment has been applied to apportion out those costs. 
+&lt;br&gt;8. All costs have been normalised to a common UK average price level using regional location factors published by Building Cost Information Service (BCIS), December 2015, 1 is the base weight.
+&lt;br&gt;9. All costs have been adjusted for inflation using the latest Building Cost Information Service (BCIS) All-In Tender Price of Index (TPI), published March 2020.  Costs have been rebased from the start of construction (or time of place provision if construction start date unavailable) to 1st Quarter (Jan – Mar) 2020 prices using this index (Q1 2020 index value = 335).
+&lt;br&gt;10. </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>To adjust the national average to the region of interest, divide the national average cost by the weight for the region, given in the Scorecard underlying data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (the regional weight has been calculated using the regional location factors mentioned above).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Example: New primary school in Outer London.  
+National average for primary new schools = £20,508
+Outer London weight = 0.820 (Base weight of 1.00/Outer London location factor of 1.22).
+Average primary New School cost that applies to Outer London in Q1 2020 prices =  £20,508 ÷ 0.820 = £25,000 (rounded to nearest £100).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+11. </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>To adjust the national average to current or future prices, you need to uprate or downrate the prices in this scorecard relative to the change that has happened since Q1 2020</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.  If you have access to the BCIS indices via a subscription to BCIS Online (https://www.rics.org/uk/products/data-products/bcis-construction/bcis-online/) you can use the latest inflation index to re-base (weight to apply = latest index/335).  If not, you can apply a known change to the published cost (e.g. up or down x%).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Example: New primary school in Outer London Q3 (Jul - Sep) 2021.  
+National average for primary new schools = £20,508.  
+Outer London weight = 0.820.  
+Inflation weight = 342/335 = 1.021 (taken from BCIS All-In TPI published March 2020). 
+Average primary New School cost that applies to Outer London in Q3 2021 prices = £20,508 ÷ 0.820 x 1.021 = £25,500 (rounded to nearest £100).  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+If you do not have access the BCIS index, but sources say TPI inflation is set to increase by 4% per annum, then approximate inflation weight = 6% (18 months’ worth of inflation) = 1.06.
+12. Some additional but limited benchmark information for similar capital programme schemes carried out by the DfE is available in the National School Delivery Cost Benchmarking study (https://ebdog.org.uk/wp-content/uploads/2019/06/F07125-National-School-Delivery-Cost-Benchmarking-Primary-Secondary-and--SEN-Schools-Final-June-2019-v6.7a.pdf).</t>
+    </r>
+  </si>
+  <si>
     <t>The total number of new places planned for delivery from 2019/20 to 2021/22;
 &lt;br&gt;The number of places planned for delivery contains four elements: 
 &lt;br&gt;1) local authority firm plans for  new permanent additional places and new temporary bulge places’,
@@ -538,30 +756,6 @@
     <t>1. The quality rating of the places created is either the Ofsted judgment, the key stage 2 reading or maths progress measures (primary only) or the key stage 4 progress 8 score category (secondary only).
 &lt;br&gt;2. The quality of new places amongst the relevant quality categories for the selected authority is presented.
 &lt;br&gt;3. The quality rating of the places present in the school capacity collection 2019 that were also present in the school capacity collection 2018 is presented as the existing places.</t>
-  </si>
-  <si>
-    <t>1. No cost data was collected in 2019 as the Capital Spend data collection was removed from the SCAP survey pending the introduction of the Capital Spend Survey. The most recent cost data available is the 2018 Capital Spend data as used in the 2018 Scorecard. For the 2019 Scorecard, this data has been adjusted for inflation (rebased to 1st Quarter 2020 prices). You can use this data to establish developer contributions per school place by adjusting the national average (for a chosen project type/phase) for region, and adjusting for further inflation if needed (see examples below).
-&lt;br&gt;2. Projects which do not create additional mainstream places or where the project's additional place funding is zero are removed. After further investigation, three projects were removed from the 2018 Scorecards cost data for use in the 2019 Scorecards as the projects' additional place funding was zero.
-&lt;br&gt;3. Projects were identified as primary phase or secondary phase based on additional mainstream place year group breakdown. Where a project created places across the primary and secondary phases, the project was assigned a phase corresponding to the phase of the school it affected (i.e. if its school was middle-deemed primary - the project was assigned to primary).
-&lt;br&gt;4. Average cost per place figures for all-through, middle-deemed primary and middle-deemed secondary schools have not been calculated separately due to low sample sizes for these project types. To estimate average cost per place for middle-deemed primary schools, we recommend using primary average cost per place as the middle school provides education equivalent to the education a primary school provides for all year groups. To estimate average cost per place for middle-deemed secondary schools, we recommend using secondary average cost per place for the same reason. For new middle schools or whole school expansions for middle schools not ‘deemed’ primary or secondary, we recommend taking a mid-point of the primary and secondary costs if the project covers both primary- and secondary-equivalent year groups equally (e.g. 2 classes per Year 5 &amp; 6 and 2 classes per Year 7 &amp; 8). If the project only covers certain year groups, we recommend using primary cost data if only primary-equivalent years groups are expanding (e.g. Years 5 &amp; 6) and secondary data if only secondary-equivalent year groups are expanding (e.g. Years 7 &amp; 8).
-&lt;br&gt;5. The average cost does not include costs associated with land acquisition.
-&lt;br&gt;6. The average cost includes costs associated with maintenance and building condition or enhancement works.
-&lt;br&gt;7. The measure does not include places in special schools or units attached to mainstream schools, or new places which were funded through central programmes (including free schools). Where a project creates additional mainstream places and also creates SEN places or re-provides places, an adjustment has been applied to apportion out those costs. 
-&lt;br&gt;8. All costs have been normalised to a common UK average price level using regional location factors published by Building Cost Information Service (BCIS), December 2015, 1 is the base weight.
-&lt;br&gt;9. All costs have been adjusted for inflation using the latest Building Cost Information Service (BCIS) All-In Tender Price of Index (TPI), published March 2020.  Costs have been rebased from the start of construction (or time of place provision if construction start date unavailable) to 1st Quarter (Jan – Mar) 2020 prices using this index (Q1 2020 index value = 335).
-&lt;br&gt;10. To adjust the national average to the region of interest, divide the national average cost by the weight for the region, given in the Scorecard underlying data (the regional weight has been calculated using the regional location factors mentioned above).
-Example: New primary school in Outer London.  
-National average for primary new schools = 20,508
-Outer London weight = 0.820 (Base weight of 1.00/Outer London location factor of 1.22).
-Average primary New School cost that applies to Outer London in Q1 2020 prices =  20,508 ÷ 0.820 = 25,000 (rounded to nearest 100).
-11. To adjust the national average to current or future prices, you need to uprate or downrate the prices in this scorecard relative to the change that has happened since Q1 2020.  If you have access to the BCIS indices via a subscription to BCIS Online (https://www.rics.org/uk/products/data-products/bcis-construction/bcis-online/) you can use the latest inflation index to re-base (weight to apply = latest index/335).  If not, you can apply a known change to the published cost (e.g. up or down x%).
-Example: New primary school in Outer London Q3 (Jul - Sep) 2021.  
-National average for primary new schools = 20,508.  
-Outer London weight = 0.820.  
-Inflation weight = 342/335 = 1.021 (taken from BCIS All-In TPI published March 2020). 
-Average primary New School cost that applies to Outer London in Q3 2021 prices = 20,508 ÷ 0.820 x 1.021 = 25,500 (rounded to nearest 100).  
-If you do not have access the BCIS index, but sources say TPI inflation is set to increase by 4% per annum, then approximate inflation weight = 6% (18 months’ worth of inflation) = 1.06.
-12. Some additional but limited benchmark information for similar capital programme schemes carried out by the DfE is available in the National School Delivery Cost Benchmarking study (https://ebdog.org.uk/wp-content/uploads/2019/06/F07125-National-School-Delivery-Cost-Benchmarking-Primary-Secondary-and--SEN-Schools-Final-June-2019-v6.7a.pdf).</t>
   </si>
 </sst>
 </file>
@@ -1364,7 +1558,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1496,7 +1690,7 @@
         <v>14</v>
       </c>
       <c r="E2" s="48" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1515,7 +1709,7 @@
         <v>74</v>
       </c>
       <c r="B4" s="45" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>17</v>
@@ -1524,7 +1718,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="38" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1550,7 +1744,7 @@
         <v>20</v>
       </c>
       <c r="E6" s="38" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1574,7 +1768,7 @@
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="38" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1591,7 +1785,7 @@
         <v>27</v>
       </c>
       <c r="E9" s="45" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1619,7 +1813,7 @@
         <v>30</v>
       </c>
       <c r="E11" s="45" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1645,7 +1839,7 @@
         <v>35</v>
       </c>
       <c r="E13" s="45" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1788,7 +1982,7 @@
         <v>42</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1816,7 +2010,7 @@
         <v>47</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1927,7 +2121,7 @@
       </c>
       <c r="D13" s="30"/>
       <c r="E13" s="30" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2026,7 +2220,7 @@
         <v>69</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added new data for new release.
</commit_message>
<xml_diff>
--- a/data/tech_guidance.xlsx
+++ b/data/tech_guidance.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\r projects\R shiny scorecard dev\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Scorecards\Scorecards 2021\Scorecard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE36E96C-27EB-4347-836C-26626107BB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64378A66-F5FB-496C-8AE6-4C6A847247BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{9CCC1F63-2262-45DD-B4CA-7C937E5C8E7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9CCC1F63-2262-45DD-B4CA-7C937E5C8E7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Quantity" sheetId="2" r:id="rId1"/>
@@ -256,9 +256,81 @@
 &lt;br&gt;2. Most local authorities will have further developed their plans since this data was reported in Summer 2021, and so although it allows for comparisons between local authorities, the figure is likely to be an understatement of the current position. </t>
   </si>
   <si>
+    <t>The anticipated percentage increase in pupil numbers in primary or secondary provision between the 2009/10 and 2023/24 academic years.</t>
+  </si>
+  <si>
+    <t>1. This is the local authority's forecast of pupil numbers for the academic year 2023/24 as provided in SCAP 2021.
+2. These forecasts cover pupils that local authorities anticipate will attend primary schools (or primary provision in middle or all-through schools i.e. years R-6) and secondary schools (or secondary provision in middle or all-through schools i.e. years 7-11)
+3. These forecasts focus on local authorities expectations about new school places and do not include pupils who are expected to attend independent schools or special/non-mainstream provision.</t>
+  </si>
+  <si>
+    <t>1. Forecasts of academic year 2021/22 pupil numbers made in 2020/21.</t>
+  </si>
+  <si>
+    <t>1. The proportions of applicants who received an offer of a place in their first, second and third preferences.
+&lt;br&gt;2. The blank section represents the proportion made an offer of a lower preference (where a local authority allows 4 or more preferences) and the proportion not made a preferred offer (including applicants who were made an alternative offer and those who were not made any offer).</t>
+  </si>
+  <si>
+    <t>The proportion of applicants who received an offer of a place in one of their top three preference schools for September 2021 on national offer day</t>
+  </si>
+  <si>
+    <t>Percentage of new places created in good and outstanding schools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LA Rank
+</t>
+  </si>
+  <si>
+    <t>Ranks local authorities on their proportion of new school places which are in good and outstanding schools</t>
+  </si>
+  <si>
+    <t>Total amount of basic need capital funding allocated to each local authority to create new places from 2011 to 2024. This covers places needed at both primary and secondary.</t>
+  </si>
+  <si>
+    <t>Estimated percentage of spare places in 2023/24.</t>
+  </si>
+  <si>
+    <t>Estimated number of additional places needed to meet demand in 2023/24;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. The calculation mirrors the approach taken for basic need funding allocations published in March 2022. It includes mainstream primary and secondary free schools which opened in September 2021 and those with a high degree of certainty of opening in September 2022, and counts the total number of places which will be in use by September 2023.
+&lt;br&gt;2. The data does not include free schools which opened before September 2021, as they will be included in the SCAP2021. It does not include free schools which are planned to open in academic year 2022/23 where it is likely the opening will be delayed, or those planned to open in the academic year 2023/24 and beyond. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. This refers to the amount of basic need capital funding that the Department for Education (DfE) has allocated to each local authority to create new places from 2011 to 2024.
+&lt;br&gt;2. The figure includes formula-based funding allocations and funding provided through the Targeted Basic Need Programme. Basic Need funding is not ring-fenced, but Targeted Basic Need funding must be spent by agreed deadlines and on specific projects.
+&lt;br&gt;3. The figure only includes funding allocated to local authorities, and does not include centrally funded capital programmes such as free schools. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The national average has been adjusted to the relevant region for each local authority, using the Building Cost Information Service (BCIS) Dec 2021 published regional location factors. The England national average has been multiplied by the relevant regional location factor:  East Midlands: 1.05, East of England 1.01, Inner London: 1.26, North East: 0.93, North West: 0.99, Outer London: 1.19, South East: 1.08, South West: 1.02, West Midlands: 0.95, Yorkshire &amp; the Humber: 0.94. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Forecasts of academic year 2021/22 pupil numbers made in 2018/19.
+</t>
+  </si>
+  <si>
+    <t>The number of new places created between academic year 2018/19 and academic year 2020/21</t>
+  </si>
+  <si>
+    <t>1. Ranking of proportions of new places created in 'good' or 'outstanding' schools for each local authority, amongst all local authorities with new places. Local authorities with the same proportion are given an equal ranking. Ranking is only applied to local authorities where new places have been created.
+&lt;br&gt;2. The higher the rank the higher the proportion of new school places in good and outstanding schools compared to other local authorities. &lt;br&gt;3. Ranks can be tied and there will many local authorities with a rank of 1 due to 100% of new places in good and outstanding schools.</t>
+  </si>
+  <si>
+    <t>Forecast accuracy of pupil projections for 2021/22</t>
+  </si>
+  <si>
+    <t>School place offers by preference for September 2021 entry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The national average cost per place of permanent expansion, temporary expansion and new school projects in England. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average cost per additional mainstream place, based on local authority reported projects for 2015/16, 2016/17 and 2017/18, adjusted for inflation and regional variation. </t>
+  </si>
+  <si>
     <t>1.This relates to the academic year 2023/24 and is the difference between local authority pupil forecasts and future capacity, taking account of planned future additions.
      places needed = forecast demand - (existing capacity + additional capacity).  
-For further information on the methodology used, see the School Place Planning Tables 2021: technical note (https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/874771/School_place_planning_2021_Technical_Guidance.pdf)
+For further information on the methodology used, see the School Place Planning 2021: technical note found on the School Capacity 21 publication on Explore Education Statistics.
 &lt;br&gt;2. Where demand is greater than capacity a need for additional places results; where capacity is greater than demand spare places result. 
 &lt;br&gt;3. Local authority pupil forecasts for 2023/24 are collected through the SCAP 2021 and include pupils who will attend places created by housing developer contributions (HDC).
 &lt;br&gt;4. Additional capacity as at 2023/24 includes places that the local authority plans to add between May 2021 and before the start of the 2023/24 academic year and places from programmes centrally funded by the department, as described above. 
@@ -268,24 +340,18 @@
 &lt;br&gt;8. Estimates for spare places are presented as a percentage of total future capacity.</t>
   </si>
   <si>
-    <t>The anticipated percentage increase in pupil numbers in primary or secondary provision between the 2009/10 and 2023/24 academic years.</t>
-  </si>
-  <si>
-    <t>1. This is the local authority's forecast of pupil numbers for the academic year 2023/24 as provided in SCAP 2021.
-2. These forecasts cover pupils that local authorities anticipate will attend primary schools (or primary provision in middle or all-through schools i.e. years R-6) and secondary schools (or secondary provision in middle or all-through schools i.e. years 7-11)
-3. These forecasts focus on local authorities expectations about new school places and do not include pupils who are expected to attend independent schools or special/non-mainstream provision.</t>
-  </si>
-  <si>
-    <t>The one year ahead local authority forecast accuracy. It compares actual numbers on roll in 2021/22 with forecasts of pupil numbers for 2021/22 made one year previously (in SCAP21)</t>
-  </si>
-  <si>
-    <t>The three year ahead forecast accuracy compares forecasts of pupil numbers on roll for 2021/22 made three years previously (in SCAP19) by local authority).</t>
-  </si>
-  <si>
-    <t>1. Forecasts of academic year 2021/22 pupil numbers made in 2020/21.</t>
-  </si>
-  <si>
-    <t>1. Forecasts, submitted by local authorities for SCAP21 , at planning area level  2021/22 pupil numbers are made for each year group and aggregated to local authority level. Forecasts include pupils expected to be educated in new schools (or expanded schools) funded through Housing Developer Contributions and Housing Infrastructure Fund agreements.
+    <t>Total places created between 2009/10 and 2020/21</t>
+  </si>
+  <si>
+    <t>Total number of new places planned for delivery from 2021/22 to 2023/24;
+&lt;br&gt;This contains four elements: 
+&lt;br&gt;1) local authority firm plans for new permanent additional places and new temporary bulge places’,
+&lt;br&gt;2) capacity changes through the Condition Improvement Fund (CIF), Priority School Building Programme (PSBP), Selective Schools Expansion Fund (SSEF), and Voluntary Aided Schools Fund (VA)
+&lt;br&gt;3) places from free schools opened in September 2021 and planned to open in September 2022, and
+&lt;br&gt;4) reduction in places from free school and academy closures.</t>
+  </si>
+  <si>
+    <t>1. Forecasts, submitted by local authorities for SCAP21 , at planning area level  2021/22 pupil numbers are made for each year group and aggregated to local authority level. Forecasts include pupils expected to be educated in new schools (or expanded schools) funded through Housing Developer Contributions (HDC) and Housing Infrastructure Fund (HIF) agreements.
 &lt;br&gt;2. Actual pupil numbers on roll for academic year 2021/22 are taken from the January school census.
 &lt;br&gt;3. Forecast accuracy is calculated by  subtracting the years R-6 actual numbers from the years R-6 forecasts to give the absolute inaccuracy. Absolute inaccuracy is then divided by the R-6 actual number to give the relative percentage inaccuracy. The same is done for secondary using years 7-11. 
 &lt;br&gt;4.  Scorecard figures may differ to those published in SCAP due to the exclusion of years 12 to 14 in the pupil numbers and forecasts used in the scorecard.</t>
@@ -311,20 +377,13 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>as part of the SCAP 2019, at planning area level  2021/22 pupil numbers are aggregated to local authority level. Forecasts include pupils expected to be educated in new schools (or expanded schools) funded through HDC agreements.
+      <t>as part of the SCAP 2019, at planning area level  2021/22 pupil numbers are aggregated to local authority level. Forecasts include pupils expected to be educated in new schools (or expanded schools) funded through HDC and HIF agreements.
 &lt;br&gt;2. Actual pupil numbers on roll for academic year 2021/22 are taken from the January school census.&lt;br&gt;3. Forecast accuracy is calculated by  subtracting the years R-6 actual numbers from the years R-6 forecasts to give the absolute inaccuracy. Absolute inaccuracy is then divided by the R-6 actual number to give the relative percentage inaccuracy. The same is done for secondary using years 7-11. 
 &lt;br&gt;4.  Scorecard figures may differ to those published in SCAP due to the exclusion of years 12 to 14 in the pupil numbers and forecasts used in the scorecard.</t>
     </r>
   </si>
   <si>
-    <t>1. The proportions of applicants who received an offer of a place in their first, second and third preferences.
-&lt;br&gt;2. The blank section represents the proportion made an offer of a lower preference (where a local authority allows 4 or more preferences) and the proportion not made a preferred offer (including applicants who were made an alternative offer and those who were not made any offer).</t>
-  </si>
-  <si>
-    <t>The proportion of applicants who received an offer of a place in one of their top three preference schools for September 2021 on national offer day</t>
-  </si>
-  <si>
-    <t>1. The following school types, identified using Get Information About Schools (https://get-information-schools.service.gov.uk), have been excluded:
+    <t>1. The following school types, identified using Get Information About Schools, have been excluded:
 &lt;br&gt;- former independent schools which have not had an inspection since opening;
 &lt;br&gt;- sponsored academies which have not had an Ofsted inspection since opening as an academy.
 &lt;br&gt;- schools that have amalgamated and have not been inspected since amalgamation.
@@ -339,43 +398,7 @@
 &lt;br&gt;10. The quality measures represent the window in time when places were added and this is not necessarily the same quality outcome as when the decision to add places was taken.</t>
   </si>
   <si>
-    <t>Percentage of new places created in good and outstanding schools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LA Rank
-</t>
-  </si>
-  <si>
-    <t>Ranks local authorities on their proportion of new school places which are in good and outstanding schools</t>
-  </si>
-  <si>
-    <t>Total number of new places planned for delivery from 2021/22 to 2023/24;
-&lt;br&gt;This contains four elements: 
-&lt;br&gt;1) local authority firm plans for new permanent additional places and new temporary bulge places’,
-&lt;br&gt;2) capacity changes through the Condition Improvement Fund (CIF), Priority School Building Programme (PSBP), Selective Schools Expansion Fund (SSEF), and Voluntary aided Schools fund (VA)
-&lt;br&gt;3) places from free schools opened in September 2021 and planned to open in September 2022, and
-&lt;br&gt;4) reduction in places from free school and academy closures.</t>
-  </si>
-  <si>
-    <t>Total amount of basic need capital funding allocated to each local authority to create new places from 2011 to 2024. This covers places needed at both primary and secondary.</t>
-  </si>
-  <si>
-    <t>Estimated percentage of spare places in 2023/24.</t>
-  </si>
-  <si>
-    <t>Estimated number of additional places needed to meet demand in 2023/24;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. The calculation mirrors the approach taken for basic need funding allocations published in March 2022. It includes mainstream primary and secondary free schools which opened in September 2021 and those with a high degree of certainty of opening in September 2022, and counts the total number of places which will be in use by September 2023.
-&lt;br&gt;2. The data does not include free schools which opened before September 2021, as they will be included in the SCAP2021. It does not include free schools which are planned to open in academic year 2022/23 where it is likely the opening will be delayed, or those planned to open in the academic year 2023/24 and beyond. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. This refers to the amount of basic need capital funding that the Department for Education (DfE) has allocated to each local authority to create new places from 2011 to 2024.
-&lt;br&gt;2. The figure includes formula-based funding allocations and funding provided through the Targeted Basic Need Programme. Basic Need funding is not ring-fenced, but Targeted Basic Need funding must be spent by agreed deadlines and on specific projects.
-&lt;br&gt;3. The figure only includes funding allocated to local authorities, and does not include centrally funded capital programmes such as free schools. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The national average has been adjusted to the relevant region for each local authority, using the Building Cost Information Service (BCIS) Dec 2021 published regional location factors. The England national average has been multiplied by the relevant regional location factor:  East Midlands: 1.05, East of England 1.01, Inner London: 1.26, North East: 0.93, North West: 0.99, Outer London: 1.19, South East: 1.08, South West: 1.02, West Midlands: 0.95, Yorkshire &amp; the Humber: 0.94. </t>
+    <t>The one year ahead local authority forecast accuracy. It compares actual numbers on roll in 2021/22 with forecasts of pupil numbers for 2021/22 made one year previously (in SCAP 2021)</t>
   </si>
   <si>
     <r>
@@ -534,10 +557,10 @@
       </rPr>
       <t xml:space="preserve">
 Example: New primary school in Outer London Q3 (Jul - Sep) 2022.  
-National average for primary new schools = £xxx.  
-Outer London weight = 0.840.  
+National average for primary new schools = £21,559.  
+Outer London location factor = 1.19 (taken from published BCIS regional location factors Dec 2021)
 Inflation weight = 367/349 = 1.052(taken from BCIS All-In TPI published March 2022). 
-Average primary New School cost that applies to Outer London in Q3 2022 prices = £21,599 ÷ 0.840 x 1.052 = £xxx (rounded to nearest £100).  </t>
+Average primary New School cost that applies to Outer London in Q3 2022 prices = £21,559 x 1.19 x 1.052 = £27,000 (rounded to nearest £100).  </t>
     </r>
     <r>
       <rPr>
@@ -548,52 +571,29 @@
       </rPr>
       <t xml:space="preserve">
 If you do not have access the BCIS index, but sources say TPI inflation is set to increase by 4% per annum, then approximate inflation weight = 6% (18 months’ worth of inflation) = 1.06.
-11. Some additional but limited benchmark information for similar capital programme schemes carried out by the DfE is available in the National School Delivery Cost Benchmarking study (https://ebdog.org.uk/wp-content/uploads/2019/06/F07125-National-School-Delivery-Cost-Benchmarking-Primary-Secondary-and--SEN-Schools-Final-June-2019-v6.7a.pdf).</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Forecasts of academic year 2021/22 pupil numbers made in 2018/19.
-</t>
-  </si>
-  <si>
-    <t>Percentage of new places created in good and outstanding schools between academic year 2018/19 and academic year 2021/22.</t>
-  </si>
-  <si>
-    <t>The number of new places created between academic year 2018/19 and academic year 2020/21</t>
-  </si>
-  <si>
-    <t>1. Ranking of proportions of new places created in 'good' or 'outstanding' schools for each local authority, amongst all local authorities with new places. Local authorities with the same proportion are given an equal ranking. Ranking is only applied to local authorities where new places have been created.
-&lt;br&gt;2. The higher the rank the higher the proportion of new school places in good and outstanding schools compared to other local authorities. &lt;br&gt;3. Ranks can be tied and there will many local authorities with a rank of 1 due to 100% of new places in good and outstanding schools.</t>
+11. Some additional but limited benchmark information for similar capital programme schemes carried out by the DfE is available in the National School Delivery Cost Benchmarking study: https://ebdog.org.uk/wp-content/uploads/2019/06/F07125-National-School-Delivery-Cost-Benchmarking-Primary-Secondary-and--SEN-Schools-Final-June-2019-v6.7a.pdf.</t>
+    </r>
+  </si>
+  <si>
+    <t>Quality of new school places created between academic year 2018/19 and 2020/21, based on Ofsted rating</t>
+  </si>
+  <si>
+    <t>Percentage of new places created in good and outstanding schools between academic year 2018/19 and academic year 2020/21.</t>
+  </si>
+  <si>
+    <t>The three year ahead forecast accuracy compares actual pupil numbers on roll with forecasts of pupil numbers for 2021/22 made three years previously (in SCAP 2019) by local authority).</t>
+  </si>
+  <si>
+    <t>Quality of school places created between academic year 2018/19 and academic year 2020/21, based on Ofsted rating. The quality of existing school places (places in 2020/21 which were also present in 2018/19) is shown for context.</t>
   </si>
   <si>
     <t>1. Each school has been matched with the Ofsted judgement of 'Overall effectiveness: how good is the school." as at 31 August 2021 (published November 2021).
 &lt;br&gt;2. There are four Ofsted categories: 'Outstanding', 'Good', 'Requires improvement' and 'Inadequate'.
-&lt;br&gt;3. The calculation counts the number of exisiting and new places that have been created in schools of each category. &lt;br&gt;4. Note that many schools will have been inspected some time before August 2021, and some will have been inspected since this date. &lt;br&gt;5. There are school places with no rating, as the school has yet to be inspected so do not have an Ofsted judgement.</t>
-  </si>
-  <si>
-    <t>Total primary places and total secondary places created between 2009/10 and 2020/21</t>
-  </si>
-  <si>
-    <t>Forecast accuracy of pupil projections for 2021/22</t>
-  </si>
-  <si>
-    <t>School place offers by preference for September 2021 entry</t>
-  </si>
-  <si>
-    <t>Quality of new school places created between academic year 2018/19 and 2021/22, based on Ofsted rating</t>
-  </si>
-  <si>
-    <t>Quality of school places created between academic year 2018/19 and academic year 2020/21, based on ofsted rating. The quality of existing school places (places in 2020/21 which were also present in 2018/19) is shown for context.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The national average cost per place of permanent expansion, temporary expansion and new school projects in England. </t>
+&lt;br&gt;3. The calculation counts the number of existing and new places that have been created in schools of each category. &lt;br&gt;4. Note that many schools will have been inspected some time before August 2021, and some will have been inspected since this date. &lt;br&gt;5. There are school places with no rating, as the school has yet to be inspected so do not have an Ofsted judgement.</t>
   </si>
   <si>
     <t>Local authority data provided through the 2018 Capital Spend return. 
-See Scorecard underlying data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average cost per additional mainstream place, based on local authority reported projects for 2015/16, 2016/17 and 2017/18, adjusted for inflation and regional variation. </t>
+See Scorecard underlying data on explore education statistics</t>
   </si>
 </sst>
 </file>
@@ -1055,6 +1055,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1092,9 +1095,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1414,7 +1414,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8372DA64-5E2C-41C1-8CF4-85BC1C2AFF86}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1445,8 +1447,8 @@
       <c r="A2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="44" t="s">
-        <v>76</v>
+      <c r="B2" s="45" t="s">
+        <v>71</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>3</v>
@@ -1454,27 +1456,27 @@
       <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="46" t="s">
+      <c r="E2" s="47" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
-      <c r="B3" s="45"/>
+      <c r="B3" s="46"/>
       <c r="C3" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="45"/>
+      <c r="E3" s="46"/>
     </row>
     <row r="4" spans="1:5" ht="285" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="47" t="s">
-        <v>63</v>
+      <c r="B4" s="48" t="s">
+        <v>72</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>25</v>
@@ -1488,7 +1490,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
-      <c r="B5" s="48"/>
+      <c r="B5" s="49"/>
       <c r="C5" s="6" t="s">
         <v>45</v>
       </c>
@@ -1501,7 +1503,7 @@
     </row>
     <row r="6" spans="1:5" ht="315" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
-      <c r="B6" s="48"/>
+      <c r="B6" s="49"/>
       <c r="C6" s="6" t="s">
         <v>38</v>
       </c>
@@ -1509,12 +1511,12 @@
         <v>5</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
-      <c r="B7" s="48"/>
+      <c r="B7" s="49"/>
       <c r="C7" s="6" t="s">
         <v>39</v>
       </c>
@@ -1527,7 +1529,7 @@
     </row>
     <row r="8" spans="1:5" ht="240" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
-      <c r="B8" s="45"/>
+      <c r="B8" s="46"/>
       <c r="C8" s="6" t="s">
         <v>22</v>
       </c>
@@ -1541,16 +1543,16 @@
         <v>26</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="50" t="s">
+      <c r="D9" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="47" t="s">
-        <v>49</v>
+      <c r="E9" s="48" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1558,33 +1560,33 @@
         <v>27</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="45"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="45"/>
+        <v>58</v>
+      </c>
+      <c r="C10" s="46"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="46"/>
     </row>
     <row r="11" spans="1:5" ht="270.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C11" s="27"/>
       <c r="D11" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="42" t="s">
-        <v>50</v>
+      <c r="B12" s="43" t="s">
+        <v>49</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>35</v>
@@ -1597,8 +1599,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="255.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="41"/>
-      <c r="B13" s="43"/>
+      <c r="A13" s="42"/>
+      <c r="B13" s="44"/>
       <c r="C13" s="26" t="s">
         <v>29</v>
       </c>
@@ -1606,7 +1608,7 @@
         <v>23</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1639,7 +1641,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E4" sqref="E4:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1668,57 +1670,57 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="B2" s="49" t="s">
-        <v>52</v>
+        <v>66</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>76</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D2" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="47" t="s">
-        <v>55</v>
+      <c r="E2" s="48" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
-      <c r="B3" s="45"/>
+      <c r="B3" s="46"/>
       <c r="C3" s="25" t="s">
         <v>30</v>
       </c>
       <c r="D3" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="45"/>
+      <c r="E3" s="46"/>
     </row>
     <row r="4" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
-      <c r="B4" s="49" t="s">
-        <v>53</v>
+      <c r="B4" s="50" t="s">
+        <v>80</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D4" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="47" t="s">
-        <v>56</v>
+      <c r="E4" s="48" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
-      <c r="B5" s="52"/>
+      <c r="B5" s="53"/>
       <c r="C5" s="38" t="s">
         <v>31</v>
       </c>
       <c r="D5" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="52"/>
+      <c r="E5" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1743,7 +1745,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1771,18 +1773,18 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="53" t="s">
-        <v>78</v>
+      <c r="A2" s="40" t="s">
+        <v>67</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="33" t="s">
         <v>41</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1797,8 +1799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{172A91E8-EE08-4774-802F-E9F4C78EAB63}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1828,10 +1830,10 @@
     </row>
     <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C2" s="24" t="s">
         <v>43</v>
@@ -1840,7 +1842,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1857,7 +1859,7 @@
     <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="21" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>9</v>
@@ -1866,15 +1868,15 @@
         <v>10</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>11</v>
@@ -1886,15 +1888,15 @@
     </row>
     <row r="6" spans="1:5" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B6" s="39" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C6" s="39"/>
       <c r="D6" s="39"/>
       <c r="E6" s="28" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1911,8 +1913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB73E146-A141-4797-B302-F0B3455C0C2E}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1941,19 +1943,19 @@
     </row>
     <row r="2" spans="1:5" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" s="28" t="s">
-        <v>82</v>
-      </c>
       <c r="E2" s="28" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated to latest technical notes
</commit_message>
<xml_diff>
--- a/data/tech_guidance.xlsx
+++ b/data/tech_guidance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/simone_cardin-stewart_education_gov_uk/Documents/Documents/R/la-school-places-scorecards/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\npaterson\repos\Scorecard dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{768E6869-B7D0-4989-8841-DD1BDA72AC58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{184480C5-5EF2-4935-B977-B9F95F76007B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BE2CE3C-E6C8-4C03-BCB6-726342E50CC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26964" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9CCC1F63-2262-45DD-B4CA-7C937E5C8E7F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9CCC1F63-2262-45DD-B4CA-7C937E5C8E7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Quantity" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="91">
   <si>
     <t>Notes</t>
   </si>
@@ -148,13 +148,6 @@
     <t>Local authority data provided through the School Capacity (SCAP) Collection 2021</t>
   </si>
   <si>
-    <t>Total basic need funding 2011-24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Pupil Numbers for the 2009/10 academic year taken as at the pupil census in January 2010
-</t>
-  </si>
-  <si>
     <t>School census Jan 2010 data</t>
   </si>
   <si>
@@ -185,24 +178,6 @@
     <t xml:space="preserve">Average cost per additional mainstream place, based on local authority reported projects for 2015/16, 2016/17 and 2017/18, adjusted for inflation and regional variation. </t>
   </si>
   <si>
-    <t>1. The following school types, identified using Get Information About Schools, have been excluded:
-&lt;br&gt;- former independent schools which have not had an inspection since opening;
-&lt;br&gt;- sponsored academies which have not had an Ofsted inspection since opening as an academy.
-&lt;br&gt;- schools that have amalgamated and have not been inspected since amalgamation.
-&lt;br&gt;2. We  compare the capacity of schools present in May 2021 with May 2019 capacity.
-&lt;br&gt;3. New places are identified as an increase in capacity between May 2019 and May 2021 at each school. For mergers and academy conversions where 2019 capacity is not available, the capacities of the ‘parent’ schools in 2019 have been used.
-&lt;br&gt;4. We define a school expansion to be an increase of 15 places or more. Schools where fewer than 15 places have been created between May 2019 and May 2021 have all of their capacity counted as existing places.
-&lt;br&gt;5. Existing places are the number of places present in May 2021 after subtracting the new places since May 2019 (if 15 or more) from the May 2021 capacity.
-&lt;br&gt;6. Places at schools which operate in both education phases have been assigned to years primary or secondary as notified in school capacity data in May 2019 or  2021. 
-&lt;br&gt;7. New places in schools which had not had an Ofsted judgment or key stage 2 or 4 result by August 2021 have been excluded from the relevant version of the measure. These places are included in the figure beneath the chart.
-&lt;br&gt;8. Because any decreases in capacity are not factored the number of places added for use in the quality measure may not be the same as the number of places added in the quantity measure.
-&lt;br&gt;9. From June 2019 the Ofsted grades of academy predecessor schools were factored into their data, even though it may have been some time since those schools converted and/or were inspected. 
-&lt;br&gt;10. The quality measures represent the window in time when places were added and this is not necessarily the same quality outcome as when the decision to add places was taken.</t>
-  </si>
-  <si>
-    <t>The one year ahead local authority forecast accuracy. It compares actual numbers on roll in 2021/22 with forecasts of pupil numbers for 2021/22 made one year previously (in SCAP 2021)</t>
-  </si>
-  <si>
     <t>Local authority data provided through the 2018 Capital Spend return. 
 See Scorecard underlying data on explore education statistics</t>
   </si>
@@ -216,125 +191,186 @@
     <t>Places planned to 2024/25</t>
   </si>
   <si>
-    <t>1. Local authority plans for places to be created between May 2022 and before the start of the 2024/25 academic year.</t>
-  </si>
-  <si>
     <t>Local authority data provided through the School Capacity (SCAP) Survey 2022.</t>
+  </si>
+  <si>
+    <t>2. Capacity changes through the CIF, SRP, SSEF, VA.</t>
+  </si>
+  <si>
+    <t>4. Reduction in places from free school and academy closures between May 2022 and January 2023, or identified/confirmed to close before August 2023.</t>
+  </si>
+  <si>
+    <t>1. Where an academy or free school closed after 1 May 2022 its capacity, as reported in the School Capacity data, is now no longer available. Their capacity has therefore been removed from the planned delivery total.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. This measure reports planned increases in capacity only. If there is a total net planned reduction in capacity (e.g. due to a free school closure), this is shown as zero places planned. Therefore the sum of local authority-level figures will not equal the national planned places figure.
+&lt;br&gt;2. Most local authorities will have further developed their plans since this data was reported in Summer 2022, and so although it allows for comparisons between local authorities, the figure is likely to be an understatement of the current position. </t>
+  </si>
+  <si>
+    <t>2021/22 school place planning published underlying data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total amount of basic need capital funding allocated to each local authority to support them to create new mainstream primary and secondary places from 2011 to 2024. </t>
+  </si>
+  <si>
+    <t>2. Forecast pupil numbers for the 2024/25 academic year</t>
+  </si>
+  <si>
+    <t>Local authority data provided through the  School Capacity (SCAP) Collection 2022</t>
+  </si>
+  <si>
+    <t>1. This is the local authority's forecast of pupil numbers for the academic year 2024/25 as provided in SCAP 2022.
+2. These forecasts cover pupils that local authorities anticipate will attend primary schools (or primary provision in middle or all-through schools i.e. years R-6) and secondary schools (or secondary provision in middle or all-through schools i.e. years 7-11)
+3. These forecasts focus on local authorities expectations about new school places and do not include pupils who are expected to attend independent schools or special/non-mainstream provision.</t>
+  </si>
+  <si>
+    <t>Forecast accuracy of pupil projections for 2022/23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Forecasts of academic year 2022/23 pupil numbers made in 2020/21.
+</t>
+  </si>
+  <si>
+    <t>2. Actual pupil numbers on roll in academic year 2022/23.</t>
+  </si>
+  <si>
+    <t>1. Forecasts of academic year 2022/23 pupil numbers made in 2021/22.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Actual pupil numbers on roll in academic year 2022/23.
+</t>
+  </si>
+  <si>
+    <t>Local authority data provided through the School Capacity (SCAP) Collection 2022</t>
+  </si>
+  <si>
+    <t>Pupils in school provided through the January 2023 School Census</t>
+  </si>
+  <si>
+    <t>School place offers by preference for September 2022 entry</t>
+  </si>
+  <si>
+    <t>The proportion of applicants who received an offer of a place in one of their top three preference schools for September 2022 on national offer day</t>
+  </si>
+  <si>
+    <t>Published School Applications and Offer data 2022/23 Academic Year</t>
+  </si>
+  <si>
+    <t>School place offers by preference for September 2023 entry</t>
+  </si>
+  <si>
+    <t>The proportion of applicants who received an offer of a place in one of their top three preference schools for September 2023 on national offer day</t>
+  </si>
+  <si>
+    <t>Published School Applications and Offer data 2023/24 Academic Year</t>
+  </si>
+  <si>
+    <t>The number of new places created between academic year 2020/21 and academic year 2021/22</t>
+  </si>
+  <si>
+    <t>Capacity of each school in May 2021</t>
+  </si>
+  <si>
+    <t>Capacity for each school in May 2022</t>
+  </si>
+  <si>
+    <t>Local authority data, provided through School Capacity collection 2022</t>
+  </si>
+  <si>
+    <t>Quality of school places created between academic year 2020/21 and academic year 2021/22, based on Ofsted rating. The quality of existing school places (places in 2021/22 which were also present in 2020/21) is shown for context.</t>
+  </si>
+  <si>
+    <t>1. Each school has been matched with the Ofsted judgement of 'Overall effectiveness: how good is the school." as at 31 August 2022 (published December 2022).
+&lt;br&gt;2. There are four Ofsted categories: 'Outstanding', 'Good', 'Requires improvement' and 'Inadequate'.
+&lt;br&gt;3. The calculation counts the number of existing and new places that have been created in schools of each category. &lt;br&gt;4. Note that many schools will have been inspected some time before August 2022, and some will have been inspected since this date. &lt;br&gt;5. There are school places with no rating, as the school has yet to be inspected so do not have an Ofsted judgement.</t>
+  </si>
+  <si>
+    <t>Percentage of new places created in good and outstanding schools between academic year 2020/21 and academic year 2021/22.</t>
+  </si>
+  <si>
+    <t>Unfilled places as a percentage of total places</t>
+  </si>
+  <si>
+    <t>Local authority data provided through School Capacity (SCAP) Survey 2022</t>
+  </si>
+  <si>
+    <t>Unfilled places in 2021/22</t>
   </si>
   <si>
     <t>1. The number of places that have been created since May 2010 in each local authority is taken as the difference between capacity as reported by local authorities, via SCAP, at May 2010 and May 2022.
 &lt;br&gt;2. The measure includes all primary and middle deemed primary school capacity in the primary phase, and all secondary, middle deemed secondary and all-through school capacity in the secondary phase.
-&lt;br&gt;3. The measure reports net increase in places only, if phase capacity in a local authority has reduced between May 2010 and May 2021, this is recorded as zero places created. Therefore the sum of the local authority-level figures will not equal the overall increase in places at national level.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Local authority data about new permanent additional places and new temporary bulge places (to accommodate large cohorts as they move through the school) available for the start of the academic years  2022/23, 2023/24 and 2024/25 is aggregated to local authority level.
-&lt;br&gt;2. The data was provided by local authorities in May 2022, and only includes projects they were confident would proceed. Local authorities were asked to include the total capacity of any new provision. 
+&lt;br&gt;3. The measure reports net increase in places only, if phase capacity in a local authority has reduced between May 2010 and May 2022, this is recorded as zero places created. Therefore the sum of the local authority-level figures will not equal the overall increase in places at national level.</t>
+  </si>
+  <si>
+    <t>1. Local authority plans for places to be created or removed between May 2022 and before the start of the 2024/25 academic year.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Local authority data about new permanent additional places, new temporary bulge places (to accommodate large cohorts as they move through the school) and permanent places to remove 2022/23, 2023/24 and 2024/25 is aggregated to local authority level.
+&lt;br&gt;2. The data was provided by local authorities in May 2022, and only includes projects they were confident would proceed. Local authorities were asked to include the total places of any new provision, even if spaces would fill gradually. 
 &lt;br&gt;3. Local authorities were asked not to include places created through free schools unless they were providing the funding for additional places themselves. </t>
   </si>
   <si>
-    <t>2. Capacity changes through the CIF, SRP, SSEF, VA.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Changes to school capacity (both increases and decreases) as a consequence of works delivered through the CIF, SRP, SSEF, VA between 2022-23 and 2024-25 inclusive, aggregated to local authority level. </t>
-  </si>
-  <si>
-    <t>3. Places from free schools opened in September 2022 and to be opened in September 2023.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. The calculation mirrors the approach taken for basic need funding allocations published in March 2023. It includes mainstream primary and secondary free schools which opened in September 2021 and those with a high degree of certainty of opening in September 2023, and counts the total number of places which will be in use by September 2024.
-&lt;br&gt;2. The data does not include free schools which opened before September 2022, as they will be included in the SCAP2022. It does not include free schools which are planned to open in academic year 2023/24 where it is likely the opening will be delayed, or those planned to open in the academic year 2024/25 and beyond. </t>
-  </si>
-  <si>
-    <t>4. Reduction in places from free school and academy closures between May 2022 and January 2023, or identified/confirmed to close before August 2023.</t>
-  </si>
-  <si>
-    <t>1. Where an academy or free school closed after 1 May 2022 its capacity, as reported in the School Capacity data, is now no longer available. Their capacity has therefore been removed from the planned delivery total.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. This measure reports planned increases in capacity only. If there is a total net planned reduction in capacity (e.g. due to a free school closure), this is shown as zero places planned. Therefore the sum of local authority-level figures will not equal the national planned places figure.
-&lt;br&gt;2. Most local authorities will have further developed their plans since this data was reported in Summer 2022, and so although it allows for comparisons between local authorities, the figure is likely to be an understatement of the current position. </t>
-  </si>
-  <si>
-    <t>Estimated number of additional places needed to meet demand in 2024/25;</t>
-  </si>
-  <si>
-    <t>2021/22 school place planning published underlying data</t>
-  </si>
-  <si>
-    <t>1.This relates to the academic year 2024/25 and is the difference between local authority pupil forecasts and future capacity, taking account of planned future additions.
-     places needed = forecast demand - (existing capacity + additional capacity).  
+    <t>3. Places from free schools opened in September 2022 and due to be opened in September 2023.</t>
+  </si>
+  <si>
+    <t>Estimated number of additional places needed to meet demand in 2024/25; estimated percentage of spare places in 2024/25.</t>
+  </si>
+  <si>
+    <t>Additional places needed in 2024/25; spare places in 2024/25</t>
+  </si>
+  <si>
+    <t>1.This relates to the academic year 2024/25 and is the difference between local authority pupil forecasts and future capacity, taking account of planned future additions and places to remove.
+     places needed = forecast demand - (existing capacity + additional capacity - places to remove).  
 For further information on the methodology used, see the School Place Planning 2022: technical note found on the School Capacity 22 publication on Explore Education Statistics.
 &lt;br&gt;2. Where demand is greater than capacity a need for additional places results; where capacity is greater than demand spare places result. 
-&lt;br&gt;3. Local authority pupil forecasts for 2024/25 are collected through the SCAP 2022 and include pupils who will attend places created by housing developer contributions (HDC).
-&lt;br&gt;4. Additional capacity as at 2024/25 includes places that the local authority plans to add between May 2022 and before the start of the 2024/25 academic year and places from programmes centrally funded by the department, as described above. 
+&lt;br&gt;3. Local authority pupil forecasts for 2024/25 are collected through SCAP 2022&lt;br&gt;4. Additional capacity as at 2024/25 includes places that the local authority plans to add or remove between May 2022 and before the start of the 2024/25 academic year and places from programmes centrally funded by the department, as described above. 
 &lt;br&gt;5. The comparison of demand and capacity takes place for each national curriculum year group within each planning area to estimate places needed in each. The estimates in the scorecard do not allow for spare capacity in one year group or planning area to be off-set against need in another, or vice-versa. This avoids the risk of spare places in one or more planning areas masking areas of need for additional places in planning areas elsewhere in the local authority. For further information see the School Place Planning Tables 2022: technical note.
 &lt;br&gt;6. The estimated need for additional places is aggregated to planning area level and then to local authority level. Similarly spare place estimates are aggregated to planning area and then local authority level. It is common for a local authority to have both a need for additional places and spare places, reflecting pockets of localised need for places or pockets of localised spare places.
 &lt;br&gt;7. Estimates for need are rounded to the nearest 10.
 &lt;br&gt;8. Estimates for spare places are presented as a percentage of total future capacity.</t>
   </si>
   <si>
-    <t>Additional places needed in 2024/25</t>
-  </si>
-  <si>
-    <t>Spare places needed in 2024/25</t>
-  </si>
-  <si>
-    <t>Estimated percentage of spare places in 2024/25.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total amount of basic need capital funding allocated to each local authority to support them to create new mainstream primary and secondary places from 2011 to 2024. </t>
-  </si>
-  <si>
-    <t>1. This refers to the amount of basic need capital funding that the Department for Education (DfE) has allocated to each local authority to create new places from the 2011-12 financial year to the 2023-24 financial year. Basic Need funding for the 2023-24 financial year is intended to support the creation of mainstream places for pupils aged 5 to 16 for the 2024/25 academic year. &lt;br&gt;2. The figure includes formula-based funding allocations and funding provided through the Targeted Basic Need Programme. Basic Need formula-based funding allocations cover the whole period and are not ring-fenced (although they can only be used for capital purposes).  Targeted Basic Need funding was provided between 2013 and 2015 and had to be spent by agreed deadlines and on specific projects. Both types of allocations are published here. &lt;br&gt;3. The figure only includes funding allocated to local authorities and does not include centrally-funded capital programmes such as the free schools programme.</t>
+    <t>1. This relates to the difference between number of pupils on roll and capacity, in schools where the number on roll is higher than a school's reported capacity, for each local authority.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Changes to school capacity (both increases and decreases) as a consequence of works delivered through the CIF, SRP, SSEF, VA between 2022/23 and 2024/25 inclusive, aggregated to local authority level. </t>
   </si>
   <si>
     <t>Growth in pupil numbers
-2009/10 - 2024/25</t>
-  </si>
-  <si>
-    <t>The anticipated percentage increase in pupil numbers in primary or secondary provision between the 2009/10 and 2024/25 academic years.</t>
-  </si>
-  <si>
-    <t>2. Forecast pupil numbers for the 2024/25 academic year</t>
-  </si>
-  <si>
-    <t>Local authority data provided through the  School Capacity (SCAP) Collection 2022</t>
-  </si>
-  <si>
-    <t>1. This is the local authority's forecast of pupil numbers for the academic year 2024/25 as provided in SCAP 2022.
-2. These forecasts cover pupils that local authorities anticipate will attend primary schools (or primary provision in middle or all-through schools i.e. years R-6) and secondary schools (or secondary provision in middle or all-through schools i.e. years 7-11)
-3. These forecasts focus on local authorities expectations about new school places and do not include pupils who are expected to attend independent schools or special/non-mainstream provision.</t>
-  </si>
-  <si>
-    <t>Forecast accuracy of pupil projections for 2022/23</t>
-  </si>
-  <si>
-    <t>The two year ahead forecast accuracy compares actual pupil numbers on roll with forecasts of pupil numbers for 2022/23 made three years previously (in SCAP 2021) by local authority).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Forecasts of academic year 2022/23 pupil numbers made in 2020/21.
+2009/10 to 2022/23, Anticipated growth in pupil numbers 2022/23 to 2024/25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. The calculation mirrors the approach taken for basic need funding allocations published in March 2023. It includes mainstream primary and secondary free schools which opened in September 2022 and those with a high degree of certainty of opening in September 2023, and counts the total number of places which will be in use by September 2024.
+&lt;br&gt;2. The data does not include free schools which opened before September 2022, as they will already be included in SCAP22 and are therefore existing places. It does not include free schools which are planned to open in the academic year 2024/25 and beyond. </t>
+  </si>
+  <si>
+    <t>The actual percentage increase between 2009/10 and 2023/24; the anticipated percentage increase in pupil numbers in primary or secondary state-funded mainstream provision between the 2009/10 and 2024/25 academic years.</t>
+  </si>
+  <si>
+    <t>School census Jan 2023 data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Pupil Numbers for the 2009/10 academic year taken from the pupil census in January 2010
 </t>
   </si>
   <si>
-    <t>2. Actual pupil numbers on roll in academic year 2022/23.</t>
-  </si>
-  <si>
-    <t>1. Forecasts of academic year 2022/23 pupil numbers made in 2021/22.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. Actual pupil numbers on roll in academic year 2022/23.
-</t>
-  </si>
-  <si>
-    <t>Local authority data provided through the School Capacity (SCAP) Collection 2022</t>
-  </si>
-  <si>
-    <t>Pupils in school provided through the January 2023 School Census</t>
-  </si>
-  <si>
-    <t>1. Forecasts, submitted by local authorities for SCAP22 , at planning area level  2022/23 pupil numbers are made for each year group and aggregated to local authority level. Forecasts include pupils expected to be educated in new schools (or expanded schools) funded through Housing Developer Contributions (HDC) and Housing Infrastructure Fund (HIF) agreements.
-&lt;br&gt;2. Actual pupil numbers on roll for academic year 2022/23 are taken from the January school census.
-&lt;br&gt;3. Forecast accuracy is calculated by  subtracting the years R-6 actual numbers from the years R-6 forecasts to give the absolute inaccuracy. Absolute inaccuracy is then divided by the R-6 actual number to give the relative percentage inaccuracy. The same is done for secondary using years 7-11. 
+    <t>2. Pupil Numbers for the 2009/10 academic year taken from the pupil census in January 2023</t>
+  </si>
+  <si>
+    <t>The one year ahead local authority forecast accuracy. It compares actual numbers on roll in 2022/23 with forecasts of pupil numbers for 2022/23 made one year previously (in SCAP 2022)</t>
+  </si>
+  <si>
+    <t>The two year ahead forecast accuracy compares actual pupil numbers on roll with forecasts of pupil numbers for 2022/23 made two years previously (in SCAP 2021) by local authority).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Number of pupils in roll, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Number of pupils in roll, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. 							</t>
+  </si>
+  <si>
+    <t>1. Forecasts, submitted by local authorities for SCAP22 , at planning area level and aggregated to local authority level. Forecasts include pupils expected to be educated in new schools (or expanded schools) funded through Housing Developer Contributions (HDC) and Housing Infrastructure Fund (HIF) agreements.
+&lt;br&gt;2. Actual pupil numbers on roll for academic year 2022/23 are taken from the January school census and aggregated to local authority level. They include pupils in roll, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. &lt;br&gt;3. Forecast accuracy is calculated by  subtracting the years R-6 actual numbers from the years R-6 forecasts to give the absolute inaccuracy. Absolute inaccuracy is then divided by the R-6 actual number to give the relative percentage inaccuracy. The same is done for secondary using years 7-11. 
 &lt;br&gt;4.  Scorecard figures may differ to those published in SCAP due to the exclusion of years 12 to 14 in the pupil numbers and forecasts used in the scorecard.</t>
   </si>
   <si>
@@ -358,58 +394,32 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>as part of the SCAP 2021, at planning area level  2022/23 pupil numbers are aggregated to local authority level. Forecasts include pupils expected to be educated in new schools (or expanded schools) funded through HDC and HIF agreements.
-&lt;br&gt;2. Actual pupil numbers on roll for academic year 2022/23 are taken from the January school census.&lt;br&gt;3. Forecast accuracy is calculated by  subtracting the years R-6 actual numbers from the years R-6 forecasts to give the absolute inaccuracy. Absolute inaccuracy is then divided by the R-6 actual number to give the relative percentage inaccuracy. The same is done for secondary using years 7-11. 
+      <t>as part of the SCAP 2021, at planning area level and aggregated to local authority level. Forecasts include pupils expected to be educated in new schools (or expanded schools) funded through HDC and HIF agreements.
+&lt;br&gt;2. Actual pupil numbers on roll for academic year 2022/23 are taken from the January school census and aggregated to local authority level. They include pupils in roll, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. 	&lt;br&gt;3. Forecast accuracy is calculated by subtracting the years R-6 actual numbers from the years R-6 forecasts to give the absolute inaccuracy. Absolute inaccuracy is then divided by the R-6 actual number to give the relative percentage inaccuracy. The same is done for secondary using years 7-11. 
 &lt;br&gt;4.  Scorecard figures may differ to those published in SCAP due to the exclusion of years 12 to 14 in the pupil numbers and forecasts used in the scorecard.</t>
     </r>
   </si>
   <si>
-    <t>School place offers by preference for September 2022 entry</t>
-  </si>
-  <si>
-    <t>The proportion of applicants who received an offer of a place in one of their top three preference schools for September 2022 on national offer day</t>
-  </si>
-  <si>
-    <t>Published School Applications and Offer data 2022/23 Academic Year</t>
-  </si>
-  <si>
-    <t>School place offers by preference for September 2023 entry</t>
-  </si>
-  <si>
-    <t>The proportion of applicants who received an offer of a place in one of their top three preference schools for September 2023 on national offer day</t>
-  </si>
-  <si>
-    <t>Published School Applications and Offer data 2023/24 Academic Year</t>
-  </si>
-  <si>
-    <t>Quality of new school places created between academic year 2018/19 and 2021/22, based on Ofsted rating</t>
-  </si>
-  <si>
-    <t>The number of new places created between academic year 2020/21 and academic year 2021/22</t>
-  </si>
-  <si>
-    <t>Capacity of each school in May 2021</t>
-  </si>
-  <si>
-    <t>Capacity for each school in May 2022</t>
-  </si>
-  <si>
-    <t>Local authority data, provided through School Capacity collection 2022</t>
-  </si>
-  <si>
-    <t>Quality of school places created between academic year 2020/21 and academic year 2021/22, based on Ofsted rating. The quality of existing school places (places in 2021/22 which were also present in 2020/21) is shown for context.</t>
-  </si>
-  <si>
-    <t>1. Each school has been matched with the Ofsted judgement of 'Overall effectiveness: how good is the school." as at 31 August 2022 (published December 2022).
-&lt;br&gt;2. There are four Ofsted categories: 'Outstanding', 'Good', 'Requires improvement' and 'Inadequate'.
-&lt;br&gt;3. The calculation counts the number of existing and new places that have been created in schools of each category. &lt;br&gt;4. Note that many schools will have been inspected some time before August 2022, and some will have been inspected since this date. &lt;br&gt;5. There are school places with no rating, as the school has yet to be inspected so do not have an Ofsted judgement.</t>
-  </si>
-  <si>
-    <t>Percentage of new places created in good and outstanding schools between academic year 2020/21 and academic year 2021/22.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. The cost data used in the scorecard is the 2018 Capital Spend data as used in the 2018, 2019 and 2021 Scorecards. For the 2022 Scorecard, this data has been adjusted for inflation (rebased to 1st Quarter 2023 prices). National averages adjusted for 2022 regional location factors are shown. </t>
+    <t>Quality of new school places created between academic year 2020/21 and 2021/22, based on Ofsted rating</t>
+  </si>
+  <si>
+    <t>1. The following school types, identified using Get Information About Schools, have been excluded:
+&lt;br&gt;- former independent schools which have not had an inspection since opening;
+&lt;br&gt;- sponsored academies which have not had an Ofsted inspection since opening as an academy.
+&lt;br&gt;- schools that have amalgamated and have not been inspected since amalgamation.
+&lt;br&gt;2.The capacity of schools present in May 2022 is compared with May 2021 capacity.
+&lt;br&gt;3. New places are identified as an increase in school capacity of 30 places or more between May 2021 and May 2022 at each school. For mergers and academy conversions where 2021 capacity is not available, the capacities of the ‘parent’ schools in 2021 have been used.
+&lt;br&gt;4. Schools where fewer than 30 places have been created between May 2021 and May 2022 have all of their capacity counted as existing places.
+&lt;br&gt;5. Existing places are the number of places present in May 2022 after subtracting the new places since May 2021 (if 30 or more) from the May 2021 capacity.
+&lt;br&gt;6. Places at schools which operate in both education phases have been assigned to years primary or secondary as notified in school capacity data in May 2021 or 2022. 
+&lt;br&gt;7. New places in schools which had not had an Ofsted judgment or key stage 2 or 4 result by August 2022 have been excluded from the relevant version of the measure. These places are included in the figure beneath the chart.
+&lt;br&gt;8. Because any decreases in capacity are not factored, the number of places added for use in the quality measure may not be the same as the number of places added in the quantity measure.
+&lt;br&gt;9. From June 2019 the Ofsted grades of academy predecessor schools were factored into their data, even though it may have been some time since those schools converted and/or were inspected. 
+&lt;br&gt;10. The quality measures represent the window in time when places were added and this is not necessarily the same quality outcome as when the decision to add places was taken.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. The cost data used in the scorecard is the 2018 Capital Spend data as used in the 2018, 2019 and 2021 Scorecards. For the 2022 Scorecard, this data has been adjusted for inflation (rebased to 1st Quarter 2023 prices). National averages adjusted for 2023 regional location factors are shown. </t>
     </r>
     <r>
       <rPr>
@@ -563,11 +573,11 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-Example: New primary school in Outer London Q3 (Jul - Sep) 2022.  
-National average for primary new schools = £23,501. 
+Example: New primary school in Outer London Q3 (Jul - Sep) 2023.  
+National average for primary new school place = £23,192. 
 Outer London location factor = 1.21 (taken from published BCIS regional location factors March 2023)
-Inflation weight = 371/379 = 0.979(taken from BCIS All-In TPI published March 2023). 
-Average primary New School cost that applies to Outer London in Q3 2022 prices = £23,501 x 1.21 x 0.979 = £25,800 (rounded to nearest £100).  </t>
+Inflation weight = 383/379 = 1.01 ( taken from BCIS All-In TPI published March 2023). 
+Average primary New School place cost that applies to Outer London in Q3 2023 prices = £23,192 x 1.21 x 1.01 = £28,300 (rounded to nearest £100).  </t>
     </r>
     <r>
       <rPr>
@@ -582,30 +592,25 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">The national average has been adjusted to the relevant region for each local authority, using the Building Cost Information Service (BCIS) Dec 2021 published regional location factors. The England national average has been multiplied by the relevant regional location factor:  East Midlands: 1.03, East of England 0.99, Inner London: 1.29, North East: 0.91, North West: 1, Outer London: 1.21, South East: 1.13, South West: 1.01, West Midlands: 0.96, Yorkshire &amp; the Humber: 0.91. </t>
-  </si>
-  <si>
-    <t>Unfilled places as a percentage of total places</t>
-  </si>
-  <si>
     <t>Total number of new places planned for delivery from 2022/23 to 2024/25;
-&lt;br&gt;This contains five elements: 
-&lt;br&gt;1) local authority firm plans for new permanent additional places and new temporary bulge places’,
+&lt;br&gt;This contains: 
+&lt;br&gt;1) local authority firm plans for new permanent additional places , new temporary bulge places and the removal of places,
 &lt;br&gt;2) capacity changes through the Condition Improvement Fund (CIF), School Rebuilding Programme (SRP), Selective Schools Expansion Fund (SSEF), and Voluntary Aided Schools Fund (VA)
 &lt;br&gt;3) places from free schools opened in September 2022 and planned to open in September 2023, and
-&lt;br&gt;4) reduction in places from free school and academy closures.&lt;br&gt;5) removed places</t>
-  </si>
-  <si>
-    <t>5. Total number of planned places (sum of 1, 2, 3, 4 and 5 above) September 2022 to August 2023</t>
-  </si>
-  <si>
-    <t>Local authority data provided through School Capacity (SCAP) Survey 2022</t>
-  </si>
-  <si>
-    <t>1. This relates to the difference between number of pupils on roll and capacity for each local authority.</t>
-  </si>
-  <si>
-    <t>Unfilled places in 2021/22</t>
+&lt;br&gt;4) reduction in places from free school and academy closures.</t>
+  </si>
+  <si>
+    <t>5. Total number of planned places (sum of 1, 2, 3, 4 and 5 above)</t>
+  </si>
+  <si>
+    <t>Total basic need funding 2011 to 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The national average has been adjusted to the relevant region for each local authority, using the Building Cost Information Service (BCIS) March 2023 published regional location factors. The England national average has been multiplied by the relevant regional location factor:  East Midlands: 1.03, East of England 0.99, Inner London: 1.29, North East: 0.91, North West: 1, Outer London: 1.21, South East: 1.13, South West: 1.01, West Midlands: 0.96, Yorkshire &amp; the Humber: 0.91. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. This refers to the amount of basic need capital funding that the Department for Education (DfE) has allocated to each local authority to create new places from the 2011-12 financial year to the 2023-24 financial year. Basic Need funding for the 2023-24 financial year is intended to support the creation of mainstream places for pupils aged 5 to 16 for the 2024/25 academic year. &lt;br&gt;2. The figure includes formula-based funding allocations and funding provided through the Targeted Basic Need Programme. Basic Need formula-based funding allocations cover the whole period and are not ring-fenced (although they can only be used for capital purposes).  Targeted Basic Need funding was provided between 2013 and 2015 and had to be spent by agreed deadlines and on specific projects. Both types of allocations are published here. &lt;br&gt;3. The figure only includes funding allocated to local authorities and does not include centrally-funded capital programmes such as the free schools programme. &lt;br&gt;4. The England total will not match the sum of allocations for all local authorities in the scorecard because the England total includes allocations to predecessor local authorities.
+</t>
   </si>
 </sst>
 </file>
@@ -943,7 +948,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1018,9 +1023,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1042,17 +1044,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1070,12 +1072,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1398,20 +1394,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8372DA64-5E2C-41C1-8CF4-85BC1C2AFF86}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B8"/>
+    <sheetView tabSelected="1" topLeftCell="B11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.53515625" customWidth="1"/>
-    <col min="2" max="2" width="84.15234375" customWidth="1"/>
-    <col min="3" max="3" width="54.15234375" customWidth="1"/>
-    <col min="4" max="4" width="28.921875" customWidth="1"/>
-    <col min="5" max="5" width="35.3828125" customWidth="1"/>
+    <col min="1" max="1" width="57.42578125" customWidth="1"/>
+    <col min="2" max="2" width="84.140625" customWidth="1"/>
+    <col min="3" max="3" width="54.140625" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" customWidth="1"/>
+    <col min="5" max="5" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1428,12 +1424,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="38" t="s">
-        <v>30</v>
+      <c r="B2" s="37" t="s">
+        <v>26</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>2</v>
@@ -1441,198 +1437,198 @@
       <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="40" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E2" s="39" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
-      <c r="B3" s="39"/>
+      <c r="B3" s="38"/>
       <c r="C3" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D3" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="38"/>
+    </row>
+    <row r="4" spans="1:5" ht="300" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="E3" s="39"/>
-    </row>
-    <row r="4" spans="1:5" ht="262.3" x14ac:dyDescent="0.4">
-      <c r="A4" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="41" t="s">
-        <v>84</v>
-      </c>
       <c r="C4" s="6" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
-      <c r="B5" s="42"/>
+      <c r="B5" s="41"/>
       <c r="C5" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="262.3" x14ac:dyDescent="0.4">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="285" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
-      <c r="B6" s="42"/>
+      <c r="B6" s="41"/>
       <c r="C6" s="6" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
-      <c r="B7" s="42"/>
+      <c r="B7" s="41"/>
       <c r="C7" s="6" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="219" thickBot="1" x14ac:dyDescent="0.45">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="240.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
-      <c r="B8" s="39"/>
+      <c r="B8" s="38"/>
       <c r="C8" s="6" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="32"/>
+      <c r="D9" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="E9" s="31" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A10" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10" s="41" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A11" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="39"/>
-    </row>
-    <row r="12" spans="1:5" ht="393.9" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="2" t="s">
+      <c r="B11" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="21"/>
+      <c r="D11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A13" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" s="36" t="s">
-        <v>53</v>
-      </c>
+      <c r="E12" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="8"/>
+      <c r="B13" s="31"/>
       <c r="C13" s="14" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="14"/>
-    </row>
-    <row r="14" spans="1:5" ht="233.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="35"/>
-      <c r="B14" s="37"/>
-      <c r="C14" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="22" t="s">
-        <v>56</v>
+        <v>74</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="255.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="12"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
+  <mergeCells count="3">
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="B4:B8"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{77149A54-01F0-45EA-8D19-CDE8AECFE598}"/>
-    <hyperlink ref="D10:D11" r:id="rId2" display="2021/22 school place planning published underlying data" xr:uid="{093B09C6-85AC-4B03-8BE4-078C82660B4C}"/>
+    <hyperlink ref="D10" r:id="rId2" xr:uid="{093B09C6-85AC-4B03-8BE4-078C82660B4C}"/>
     <hyperlink ref="D2" r:id="rId3" xr:uid="{8150C38D-D188-4C8E-86C3-B5575B8FFEE8}"/>
-    <hyperlink ref="D12" r:id="rId4" xr:uid="{84C17436-4B87-48EB-BAE5-31DBACCBDB31}"/>
-    <hyperlink ref="D14" r:id="rId5" xr:uid="{B4335ED1-45C2-43A8-BAE4-D6C4C7E179D0}"/>
-    <hyperlink ref="D13" r:id="rId6" xr:uid="{CCB6838D-DD36-44DD-BC08-5E652C942FA3}"/>
+    <hyperlink ref="D11" r:id="rId4" xr:uid="{84C17436-4B87-48EB-BAE5-31DBACCBDB31}"/>
+    <hyperlink ref="D13" r:id="rId5" xr:uid="{B4335ED1-45C2-43A8-BAE4-D6C4C7E179D0}"/>
+    <hyperlink ref="D12" r:id="rId6" xr:uid="{CCB6838D-DD36-44DD-BC08-5E652C942FA3}"/>
     <hyperlink ref="D3" r:id="rId7" display="Local authority data provided through School Capacity (SCAP) Survey 2021" xr:uid="{205D253B-3F70-4D79-B508-03F18A091E1F}"/>
     <hyperlink ref="D9" r:id="rId8" display="Local authority data provided through School Capacity (SCAP) Survey 2021" xr:uid="{F7517439-C801-46CD-8DC3-B6DD58F4289A}"/>
+    <hyperlink ref="D14" r:id="rId9" xr:uid="{2257ADC3-56E0-46AA-984A-65A14B6B91D4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 
@@ -1641,17 +1637,17 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B5"/>
+      <selection activeCell="E2" sqref="E2:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.53515625" customWidth="1"/>
-    <col min="2" max="2" width="84.15234375" customWidth="1"/>
-    <col min="3" max="3" width="54.15234375" customWidth="1"/>
+    <col min="1" max="1" width="50.5703125" customWidth="1"/>
+    <col min="2" max="2" width="84.140625" customWidth="1"/>
+    <col min="3" max="3" width="54.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1668,59 +1664,59 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="43" t="s">
-        <v>28</v>
+        <v>39</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>77</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" s="41" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>44</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
-      <c r="B3" s="39"/>
+      <c r="B3" s="38"/>
       <c r="C3" s="19" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" s="39"/>
-    </row>
-    <row r="4" spans="1:5" ht="44.15" thickBot="1" x14ac:dyDescent="0.45">
+        <v>45</v>
+      </c>
+      <c r="E3" s="38"/>
+    </row>
+    <row r="4" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
-      <c r="B4" s="43" t="s">
-        <v>58</v>
+      <c r="B4" s="42" t="s">
+        <v>78</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="D4" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="41" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="E4" s="40" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9"/>
-      <c r="B5" s="46"/>
+      <c r="B5" s="43"/>
       <c r="C5" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="E5" s="46"/>
+        <v>41</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1745,17 +1741,17 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.53515625" customWidth="1"/>
-    <col min="2" max="2" width="84.15234375" customWidth="1"/>
-    <col min="3" max="3" width="54.15234375" customWidth="1"/>
+    <col min="1" max="1" width="50.5703125" customWidth="1"/>
+    <col min="2" max="2" width="84.140625" customWidth="1"/>
+    <col min="3" max="3" width="54.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1772,34 +1768,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="409.6" x14ac:dyDescent="0.4">
-      <c r="A2" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" s="31" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="19" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1815,18 +1811,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{172A91E8-EE08-4774-802F-E9F4C78EAB63}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.53515625" customWidth="1"/>
-    <col min="2" max="2" width="84.15234375" customWidth="1"/>
-    <col min="3" max="3" width="54.15234375" customWidth="1"/>
+    <col min="1" max="1" width="50.5703125" customWidth="1"/>
+    <col min="2" max="2" width="84.140625" customWidth="1"/>
+    <col min="3" max="3" width="54.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1843,38 +1839,38 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="409.6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="15"/>
       <c r="C3" s="6" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="E3" s="15"/>
     </row>
-    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="16" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>6</v>
@@ -1883,15 +1879,15 @@
         <v>7</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>8</v>
@@ -1901,17 +1897,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="409.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" s="20"/>
       <c r="D6" s="20"/>
       <c r="E6" s="22" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1928,18 +1924,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB73E146-A141-4797-B302-F0B3455C0C2E}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.53515625" customWidth="1"/>
-    <col min="2" max="2" width="84.15234375" customWidth="1"/>
-    <col min="3" max="3" width="54.15234375" customWidth="1"/>
+    <col min="1" max="1" width="50.5703125" customWidth="1"/>
+    <col min="2" max="2" width="84.140625" customWidth="1"/>
+    <col min="3" max="3" width="54.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1956,67 +1952,67 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>29</v>
-      </c>
       <c r="E2" s="22" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B4" s="28"/>
-      <c r="C4" s="30"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B5" s="28"/>
-      <c r="C5" s="30"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B6" s="28"/>
-      <c r="C6" s="30"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B7" s="28"/>
-      <c r="C7" s="30"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B8" s="28"/>
-      <c r="C8" s="30"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B9" s="28"/>
-      <c r="C9" s="30"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B10" s="28"/>
-      <c r="C10" s="30"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B11" s="28"/>
-      <c r="C11" s="30"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B12" s="28"/>
-      <c r="C12" s="30"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B13" s="28"/>
-      <c r="C13" s="30"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="28"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="27"/>
+      <c r="C4" s="29"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="27"/>
+      <c r="C5" s="29"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="27"/>
+      <c r="C6" s="29"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="27"/>
+      <c r="C7" s="29"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="27"/>
+      <c r="C8" s="29"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="27"/>
+      <c r="C9" s="29"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="27"/>
+      <c r="C10" s="29"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="27"/>
+      <c r="C11" s="29"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="27"/>
+      <c r="C12" s="29"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="27"/>
+      <c r="C13" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2026,57 +2022,56 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="ec07c698-60f5-424f-b9af-f4c59398b511" ContentTypeId="0x010100545E941595ED5448BA61900FDDAFF313" PreviousValue="false"/>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
+      <Value>5</Value>
+      <Value>25</Value>
+      <Value>1</Value>
+      <Value>4</Value>
+    </TaxCatchAll>
+    <p6919dbb65844893b164c5f63a6f0eeb xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">DfE</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">a484111e-5b24-4ad9-9778-c536c8c88985</TermId>
+        </TermInfo>
+      </Terms>
+    </p6919dbb65844893b164c5f63a6f0eeb>
+    <c02f73938b5741d4934b358b31a1b80f xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Official</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">0884c477-2e62-47ea-b19c-5af6e91124c5</TermId>
+        </TermInfo>
+      </Terms>
+    </c02f73938b5741d4934b358b31a1b80f>
+    <f6ec388a6d534bab86a259abd1bfa088 xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">DfE</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">cc08a6d4-dfde-4d0f-bd85-069ebcef80d5</TermId>
+        </TermInfo>
+      </Terms>
+    </f6ec388a6d534bab86a259abd1bfa088>
+    <i98b064926ea4fbe8f5b88c394ff652b xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </i98b064926ea4fbe8f5b88c394ff652b>
+    <_dlc_DocIdUrl xmlns="2a6436df-3f7a-48ac-8ea6-44b411e24bbc">
+      <Url>https://educationgovuk.sharepoint.com/sites/efappp/_layouts/15/DocIdRedir.aspx?ID=FKMV6N5X2MYP-1953928680-73356</Url>
+      <Description>FKMV6N5X2MYP-1953928680-73356</Description>
+    </_dlc_DocIdUrl>
+    <_dlc_DocId xmlns="2a6436df-3f7a-48ac-8ea6-44b411e24bbc">FKMV6N5X2MYP-1953928680-73356</_dlc_DocId>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2286,71 +2281,81 @@
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
-      <Value>5</Value>
-      <Value>25</Value>
-      <Value>1</Value>
-      <Value>4</Value>
-    </TaxCatchAll>
-    <p6919dbb65844893b164c5f63a6f0eeb xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">DfE</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">a484111e-5b24-4ad9-9778-c536c8c88985</TermId>
-        </TermInfo>
-      </Terms>
-    </p6919dbb65844893b164c5f63a6f0eeb>
-    <c02f73938b5741d4934b358b31a1b80f xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Official</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">0884c477-2e62-47ea-b19c-5af6e91124c5</TermId>
-        </TermInfo>
-      </Terms>
-    </c02f73938b5741d4934b358b31a1b80f>
-    <f6ec388a6d534bab86a259abd1bfa088 xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">DfE</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">cc08a6d4-dfde-4d0f-bd85-069ebcef80d5</TermId>
-        </TermInfo>
-      </Terms>
-    </f6ec388a6d534bab86a259abd1bfa088>
-    <i98b064926ea4fbe8f5b88c394ff652b xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </i98b064926ea4fbe8f5b88c394ff652b>
-    <_dlc_DocIdUrl xmlns="2a6436df-3f7a-48ac-8ea6-44b411e24bbc">
-      <Url>https://educationgovuk.sharepoint.com/sites/efappp/_layouts/15/DocIdRedir.aspx?ID=FKMV6N5X2MYP-1953928680-73356</Url>
-      <Description>FKMV6N5X2MYP-1953928680-73356</Description>
-    </_dlc_DocIdUrl>
-    <_dlc_DocId xmlns="2a6436df-3f7a-48ac-8ea6-44b411e24bbc">FKMV6N5X2MYP-1953928680-73356</_dlc_DocId>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="ec07c698-60f5-424f-b9af-f4c59398b511" ContentTypeId="0x010100545E941595ED5448BA61900FDDAFF313" PreviousValue="false"/>
 </file>
 
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9C56A4F-6917-41AA-BBE5-DA7C75896563}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{035EEA42-582A-4724-B162-C22729062C2B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D00F0DC4-2D9F-43FC-8616-EC131ED26B7D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{334E8BC2-6B82-4EDA-BE50-EFE4767E8CD2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2a6436df-3f7a-48ac-8ea6-44b411e24bbc"/>
+    <ds:schemaRef ds:uri="8c566321-f672-4e06-a901-b5e72b4c4357"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2375,26 +2380,17 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{334E8BC2-6B82-4EDA-BE50-EFE4767E8CD2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D00F0DC4-2D9F-43FC-8616-EC131ED26B7D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="8c566321-f672-4e06-a901-b5e72b4c4357"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2a6436df-3f7a-48ac-8ea6-44b411e24bbc"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{035EEA42-582A-4724-B162-C22729062C2B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9C56A4F-6917-41AA-BBE5-DA7C75896563}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated metadata and technotes
</commit_message>
<xml_diff>
--- a/data/tech_guidance.xlsx
+++ b/data/tech_guidance.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\npaterson\repos\Scorecard dashboard\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/natalie_paterson_education_gov_uk/Documents/Documents/la-school-places-scorecards/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C5E800-B660-454D-8A31-A84BDC32C13B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3773382-40B4-404A-B639-A152162B8CE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9CCC1F63-2262-45DD-B4CA-7C937E5C8E7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9CCC1F63-2262-45DD-B4CA-7C937E5C8E7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Quantity" sheetId="2" r:id="rId1"/>
@@ -340,9 +340,6 @@
 &lt;br&gt;2. The data does not include free schools which opened before September 2022, as they will already be included in SCAP22 and are therefore existing places. It does not include free schools which are planned to open in the academic year 2024/25 and beyond. </t>
   </si>
   <si>
-    <t>The actual percentage increase between 2009/10 and 2023/24; the anticipated percentage increase in pupil numbers in primary or secondary state-funded mainstream provision between the 2009/10 and 2024/25 academic years.</t>
-  </si>
-  <si>
     <t>School census Jan 2023 data</t>
   </si>
   <si>
@@ -350,19 +347,10 @@
 </t>
   </si>
   <si>
-    <t>2. Pupil Numbers for the 2009/10 academic year taken from the pupil census in January 2023</t>
-  </si>
-  <si>
     <t>The one year ahead local authority forecast accuracy. It compares actual numbers on roll in 2022/23 with forecasts of pupil numbers for 2022/23 made one year previously (in SCAP 2022)</t>
   </si>
   <si>
     <t>The two year ahead forecast accuracy compares actual pupil numbers on roll with forecasts of pupil numbers for 2022/23 made two years previously (in SCAP 2021) by local authority).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Number of pupils in roll, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Number of pupils in roll, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. 							</t>
   </si>
   <si>
     <t>1. Forecasts, submitted by local authorities for SCAP22 , at planning area level and aggregated to local authority level. Forecasts include pupils expected to be educated in new schools (or expanded schools) funded through Housing Developer Contributions (HDC) and Housing Infrastructure Fund (HIF) agreements.
@@ -609,8 +597,20 @@
 </t>
   </si>
   <si>
-    <t>Growth in pupil numbers
-2009/10 to 2022/23; Anticipated growth in pupil numbers 2022/23 to 2024/25</t>
+    <t>2. Pupil Numbers for the 2022/23 academic year taken from the pupil census in January 2023</t>
+  </si>
+  <si>
+    <t>The actual percentage change in pupil numbers between 2009/10 and 2022/23; the anticipated percentage change in pupil numbers in primary or secondary state-funded mainstream provision between the 2022/23 and 2024/25 academic years.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Number of pupils in roll in January 2010, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Number of pupils in roll in January 2023, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. 							</t>
+  </si>
+  <si>
+    <t>Change in pupil numbers
+2009/10 to 2022/23; Anticipated change in pupil numbers 2022/23 to 2024/25</t>
   </si>
 </sst>
 </file>
@@ -1395,7 +1395,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1457,7 +1457,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>63</v>
@@ -1512,7 +1512,7 @@
       <c r="A8" s="8"/>
       <c r="B8" s="38"/>
       <c r="C8" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="19" t="s">
@@ -1553,7 +1553,7 @@
     </row>
     <row r="11" spans="1:5" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B11" s="21" t="s">
         <v>35</v>
@@ -1563,7 +1563,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1571,29 +1571,29 @@
         <v>90</v>
       </c>
       <c r="B12" s="35" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D12" s="25" t="s">
         <v>16</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="B13" s="31"/>
       <c r="C13" s="14" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="255.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1669,7 +1669,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>42</v>
@@ -1678,7 +1678,7 @@
         <v>44</v>
       </c>
       <c r="E2" s="40" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1695,7 +1695,7 @@
     <row r="4" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
       <c r="B4" s="42" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>40</v>
@@ -1704,7 +1704,7 @@
         <v>15</v>
       </c>
       <c r="E4" s="40" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1841,7 +1841,7 @@
     </row>
     <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>52</v>
@@ -1853,7 +1853,7 @@
         <v>17</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1960,13 +1960,13 @@
         <v>23</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D2" s="22" t="s">
         <v>25</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2021,15 +2021,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
@@ -2074,7 +2065,71 @@
 </p:properties>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="ec07c698-60f5-424f-b9af-f4c59398b511" ContentTypeId="0x010100545E941595ED5448BA61900FDDAFF313" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Official Document" ma:contentTypeID="0x010100545E941595ED5448BA61900FDDAFF31300C0D9F77D091A79449828113EF8250EF5" ma:contentTypeVersion="9" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="f90d64ba98617a6331a5780cc9b57993">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8c566321-f672-4e06-a901-b5e72b4c4357" xmlns:ns3="2a6436df-3f7a-48ac-8ea6-44b411e24bbc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a3658d73581f4a77afa8422430659c15" ns2:_="" ns3:_="">
     <xsd:import namespace="8c566321-f672-4e06-a901-b5e72b4c4357"/>
@@ -2280,62 +2335,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="ec07c698-60f5-424f-b9af-f4c59398b511" ContentTypeId="0x010100545E941595ED5448BA61900FDDAFF313" PreviousValue="false"/>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{334E8BC2-6B82-4EDA-BE50-EFE4767E8CD2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="2a6436df-3f7a-48ac-8ea6-44b411e24bbc"/>
+    <ds:schemaRef ds:uri="8c566321-f672-4e06-a901-b5e72b4c4357"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{035EEA42-582A-4724-B162-C22729062C2B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -2343,24 +2360,23 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{334E8BC2-6B82-4EDA-BE50-EFE4767E8CD2}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9C56A4F-6917-41AA-BBE5-DA7C75896563}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2a6436df-3f7a-48ac-8ea6-44b411e24bbc"/>
-    <ds:schemaRef ds:uri="8c566321-f672-4e06-a901-b5e72b4c4357"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D00F0DC4-2D9F-43FC-8616-EC131ED26B7D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0969FC7E-EEEC-4315-900C-25F913AD1B6E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2377,20 +2393,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D00F0DC4-2D9F-43FC-8616-EC131ED26B7D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9C56A4F-6917-41AA-BBE5-DA7C75896563}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated quantity chart label
</commit_message>
<xml_diff>
--- a/data/tech_guidance.xlsx
+++ b/data/tech_guidance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/natalie_paterson_education_gov_uk/Documents/Documents/la-school-places-scorecards/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{840724E6-C688-4ACB-8719-9DF4811675F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{840724E6-C688-4ACB-8719-9DF4811675F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7C520A3-221C-4E66-AB07-24336520C7C0}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9CCC1F63-2262-45DD-B4CA-7C937E5C8E7F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{9CCC1F63-2262-45DD-B4CA-7C937E5C8E7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Quantity" sheetId="2" r:id="rId1"/>
@@ -544,14 +544,6 @@
     </r>
   </si>
   <si>
-    <t>Total number of new places planned for delivery from 2022/23 to 2024/25;
-&lt;br&gt;This contains: 
-&lt;br&gt;1) local authority firm plans for new permanent additional places , new temporary bulge places and the removal of places,
-&lt;br&gt;2) capacity changes through the Condition Improvement Fund (CIF), School Rebuilding Programme (SRP), Selective Schools Expansion Fund (SSEF), and Voluntary Aided Schools Fund (VA)
-&lt;br&gt;3) places from free schools opened in September 2022 and planned to open in September 2023, and
-&lt;br&gt;4) reduction in places from free school and academy closures.</t>
-  </si>
-  <si>
     <t>5. Total number of planned places (sum of 1, 2, 3, 4 and 5 above)</t>
   </si>
   <si>
@@ -611,6 +603,14 @@
   </si>
   <si>
     <t>1. This relates to the difference between number of pupils on roll and capacity, in schools where the number on roll is lower than a school's reported capacity. &lt;br&gt;2. Calculated at school level and aggregated to local authority level.</t>
+  </si>
+  <si>
+    <t>Number of new places planned for delivery between May 2022 and September 2024;
+&lt;br&gt;This contains: 
+&lt;br&gt;1) local authority firm plans for new permanent additional places , new temporary bulge places and the removal of places,
+&lt;br&gt;2) capacity changes through the Condition Improvement Fund (CIF), School Rebuilding Programme (SRP), Selective Schools Expansion Fund (SSEF), and Voluntary Aided Schools Fund (VA)
+&lt;br&gt;3) places from free schools opened in September 2022 and planned to open in September 2023, and
+&lt;br&gt;4) reduction in places from free school and academy closures.</t>
   </si>
 </sst>
 </file>
@@ -1394,20 +1394,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8372DA64-5E2C-41C1-8CF4-85BC1C2AFF86}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="57.42578125" customWidth="1"/>
-    <col min="2" max="2" width="84.140625" customWidth="1"/>
-    <col min="3" max="3" width="54.140625" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" customWidth="1"/>
-    <col min="5" max="5" width="35.42578125" customWidth="1"/>
+    <col min="1" max="1" width="57.453125" customWidth="1"/>
+    <col min="2" max="2" width="84.1796875" customWidth="1"/>
+    <col min="3" max="3" width="54.1796875" customWidth="1"/>
+    <col min="4" max="4" width="28.81640625" customWidth="1"/>
+    <col min="5" max="5" width="35.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
         <v>14</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="8"/>
       <c r="B3" s="38"/>
       <c r="C3" s="6" t="s">
@@ -1452,12 +1452,12 @@
       </c>
       <c r="E3" s="38"/>
     </row>
-    <row r="4" spans="1:5" ht="300" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>62</v>
@@ -1469,7 +1469,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="8"/>
       <c r="B5" s="41"/>
       <c r="C5" s="6" t="s">
@@ -1482,7 +1482,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="285" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A6" s="8"/>
       <c r="B6" s="41"/>
       <c r="C6" s="6" t="s">
@@ -1495,7 +1495,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="8"/>
       <c r="B7" s="41"/>
       <c r="C7" s="6" t="s">
@@ -1508,18 +1508,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="240.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="218" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="8"/>
       <c r="B8" s="38"/>
       <c r="C8" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="19" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>60</v>
       </c>
@@ -1531,10 +1531,10 @@
         <v>59</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>66</v>
       </c>
@@ -1545,15 +1545,15 @@
         <v>5</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="409.6" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B11" s="21" t="s">
         <v>34</v>
@@ -1563,15 +1563,15 @@
         <v>1</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B12" s="35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>70</v>
@@ -1580,23 +1580,23 @@
         <v>16</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="8"/>
       <c r="B13" s="31"/>
       <c r="C13" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D13" s="25" t="s">
         <v>69</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="255.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="232.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="12"/>
       <c r="B14" s="36"/>
       <c r="C14" s="32" t="s">
@@ -1640,14 +1640,14 @@
       <selection activeCell="E2" sqref="E2:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="50.5703125" customWidth="1"/>
-    <col min="2" max="2" width="84.140625" customWidth="1"/>
-    <col min="3" max="3" width="54.140625" customWidth="1"/>
+    <col min="1" max="1" width="50.54296875" customWidth="1"/>
+    <col min="2" max="2" width="84.1796875" customWidth="1"/>
+    <col min="3" max="3" width="54.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>38</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="8"/>
       <c r="B3" s="38"/>
       <c r="C3" s="19" t="s">
@@ -1692,7 +1692,7 @@
       </c>
       <c r="E3" s="38"/>
     </row>
-    <row r="4" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="8"/>
       <c r="B4" s="42" t="s">
         <v>72</v>
@@ -1707,7 +1707,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="9"/>
       <c r="B5" s="43"/>
       <c r="C5" s="20" t="s">
@@ -1744,14 +1744,14 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="50.5703125" customWidth="1"/>
-    <col min="2" max="2" width="84.140625" customWidth="1"/>
-    <col min="3" max="3" width="54.140625" customWidth="1"/>
+    <col min="1" max="1" width="50.54296875" customWidth="1"/>
+    <col min="2" max="2" width="84.1796875" customWidth="1"/>
+    <col min="3" max="3" width="54.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A2" s="30" t="s">
         <v>45</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>48</v>
       </c>
@@ -1815,14 +1815,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="50.5703125" customWidth="1"/>
-    <col min="2" max="2" width="84.140625" customWidth="1"/>
-    <col min="3" max="3" width="54.140625" customWidth="1"/>
+    <col min="1" max="1" width="50.54296875" customWidth="1"/>
+    <col min="2" max="2" width="84.1796875" customWidth="1"/>
+    <col min="3" max="3" width="54.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1839,7 +1839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>75</v>
       </c>
@@ -1853,10 +1853,10 @@
         <v>17</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="11"/>
       <c r="B3" s="15"/>
       <c r="C3" s="6" t="s">
@@ -1867,7 +1867,7 @@
       </c>
       <c r="E3" s="15"/>
     </row>
-    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" s="11"/>
       <c r="B4" s="16" t="s">
         <v>55</v>
@@ -1882,7 +1882,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
         <v>19</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="409.6" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="12" t="s">
         <v>20</v>
       </c>
@@ -1928,14 +1928,14 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="50.5703125" customWidth="1"/>
-    <col min="2" max="2" width="84.140625" customWidth="1"/>
-    <col min="3" max="3" width="54.140625" customWidth="1"/>
+    <col min="1" max="1" width="50.54296875" customWidth="1"/>
+    <col min="2" max="2" width="84.1796875" customWidth="1"/>
+    <col min="3" max="3" width="54.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="12" t="s">
         <v>24</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>23</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D2" s="22" t="s">
         <v>25</v>
@@ -1969,48 +1969,48 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
       <c r="B3" s="27"/>
       <c r="C3" s="28"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B4" s="27"/>
       <c r="C4" s="29"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B5" s="27"/>
       <c r="C5" s="29"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" s="27"/>
       <c r="C6" s="29"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" s="27"/>
       <c r="C7" s="29"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B8" s="27"/>
       <c r="C8" s="29"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" s="27"/>
       <c r="C9" s="29"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B10" s="27"/>
       <c r="C10" s="29"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B11" s="27"/>
       <c r="C11" s="29"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B12" s="27"/>
       <c r="C12" s="29"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B13" s="27"/>
       <c r="C13" s="29"/>
     </row>
@@ -2021,6 +2021,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="ec07c698-60f5-424f-b9af-f4c59398b511" ContentTypeId="0x010100545E941595ED5448BA61900FDDAFF313" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -2070,12 +2075,61 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="ec07c698-60f5-424f-b9af-f4c59398b511" ContentTypeId="0x010100545E941595ED5448BA61900FDDAFF313" PreviousValue="false"/>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
+      <Value>5</Value>
+      <Value>25</Value>
+      <Value>1</Value>
+      <Value>4</Value>
+    </TaxCatchAll>
+    <p6919dbb65844893b164c5f63a6f0eeb xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">DfE</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">a484111e-5b24-4ad9-9778-c536c8c88985</TermId>
+        </TermInfo>
+      </Terms>
+    </p6919dbb65844893b164c5f63a6f0eeb>
+    <c02f73938b5741d4934b358b31a1b80f xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Official</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">0884c477-2e62-47ea-b19c-5af6e91124c5</TermId>
+        </TermInfo>
+      </Terms>
+    </c02f73938b5741d4934b358b31a1b80f>
+    <f6ec388a6d534bab86a259abd1bfa088 xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">DfE</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">cc08a6d4-dfde-4d0f-bd85-069ebcef80d5</TermId>
+        </TermInfo>
+      </Terms>
+    </f6ec388a6d534bab86a259abd1bfa088>
+    <i98b064926ea4fbe8f5b88c394ff652b xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </i98b064926ea4fbe8f5b88c394ff652b>
+    <_dlc_DocIdUrl xmlns="2a6436df-3f7a-48ac-8ea6-44b411e24bbc">
+      <Url>https://educationgovuk.sharepoint.com/sites/efappp/_layouts/15/DocIdRedir.aspx?ID=FKMV6N5X2MYP-1953928680-73356</Url>
+      <Description>FKMV6N5X2MYP-1953928680-73356</Description>
+    </_dlc_DocIdUrl>
+    <_dlc_DocId xmlns="2a6436df-3f7a-48ac-8ea6-44b411e24bbc">FKMV6N5X2MYP-1953928680-73356</_dlc_DocId>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Official Document" ma:contentTypeID="0x010100545E941595ED5448BA61900FDDAFF31300C0D9F77D091A79449828113EF8250EF5" ma:contentTypeVersion="9" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="f90d64ba98617a6331a5780cc9b57993">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8c566321-f672-4e06-a901-b5e72b4c4357" xmlns:ns3="2a6436df-3f7a-48ac-8ea6-44b411e24bbc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a3658d73581f4a77afa8422430659c15" ns2:_="" ns3:_="">
     <xsd:import namespace="8c566321-f672-4e06-a901-b5e72b4c4357"/>
@@ -2281,61 +2335,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
-      <Value>5</Value>
-      <Value>25</Value>
-      <Value>1</Value>
-      <Value>4</Value>
-    </TaxCatchAll>
-    <p6919dbb65844893b164c5f63a6f0eeb xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">DfE</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">a484111e-5b24-4ad9-9778-c536c8c88985</TermId>
-        </TermInfo>
-      </Terms>
-    </p6919dbb65844893b164c5f63a6f0eeb>
-    <c02f73938b5741d4934b358b31a1b80f xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Official</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">0884c477-2e62-47ea-b19c-5af6e91124c5</TermId>
-        </TermInfo>
-      </Terms>
-    </c02f73938b5741d4934b358b31a1b80f>
-    <f6ec388a6d534bab86a259abd1bfa088 xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">DfE</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">cc08a6d4-dfde-4d0f-bd85-069ebcef80d5</TermId>
-        </TermInfo>
-      </Terms>
-    </f6ec388a6d534bab86a259abd1bfa088>
-    <i98b064926ea4fbe8f5b88c394ff652b xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </i98b064926ea4fbe8f5b88c394ff652b>
-    <_dlc_DocIdUrl xmlns="2a6436df-3f7a-48ac-8ea6-44b411e24bbc">
-      <Url>https://educationgovuk.sharepoint.com/sites/efappp/_layouts/15/DocIdRedir.aspx?ID=FKMV6N5X2MYP-1953928680-73356</Url>
-      <Description>FKMV6N5X2MYP-1953928680-73356</Description>
-    </_dlc_DocIdUrl>
-    <_dlc_DocId xmlns="2a6436df-3f7a-48ac-8ea6-44b411e24bbc">FKMV6N5X2MYP-1953928680-73356</_dlc_DocId>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D00F0DC4-2D9F-43FC-8616-EC131ED26B7D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9C56A4F-6917-41AA-BBE5-DA7C75896563}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
@@ -2343,29 +2351,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D00F0DC4-2D9F-43FC-8616-EC131ED26B7D}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{035EEA42-582A-4724-B162-C22729062C2B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0969FC7E-EEEC-4315-900C-25F913AD1B6E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8c566321-f672-4e06-a901-b5e72b4c4357"/>
-    <ds:schemaRef ds:uri="2a6436df-3f7a-48ac-8ea6-44b411e24bbc"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2388,9 +2377,20 @@
 </file>
 
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{035EEA42-582A-4724-B162-C22729062C2B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0969FC7E-EEEC-4315-900C-25F913AD1B6E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8c566321-f672-4e06-a901-b5e72b4c4357"/>
+    <ds:schemaRef ds:uri="2a6436df-3f7a-48ac-8ea6-44b411e24bbc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated new places created label
</commit_message>
<xml_diff>
--- a/data/tech_guidance.xlsx
+++ b/data/tech_guidance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/natalie_paterson_education_gov_uk/Documents/Documents/la-school-places-scorecards/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{840724E6-C688-4ACB-8719-9DF4811675F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7C520A3-221C-4E66-AB07-24336520C7C0}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{840724E6-C688-4ACB-8719-9DF4811675F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56076225-DCC7-4DC4-9C71-D923D3F2E55C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{9CCC1F63-2262-45DD-B4CA-7C937E5C8E7F}"/>
   </bookViews>
@@ -182,9 +182,6 @@
 See Scorecard underlying data on explore education statistics</t>
   </si>
   <si>
-    <t>Total places created between 2009/10 and 2021/22</t>
-  </si>
-  <si>
     <t>2.Capacity at May 2022</t>
   </si>
   <si>
@@ -611,6 +608,9 @@
 &lt;br&gt;2) capacity changes through the Condition Improvement Fund (CIF), School Rebuilding Programme (SRP), Selective Schools Expansion Fund (SSEF), and Voluntary Aided Schools Fund (VA)
 &lt;br&gt;3) places from free schools opened in September 2022 and planned to open in September 2023, and
 &lt;br&gt;4) reduction in places from free school and academy closures.</t>
+  </si>
+  <si>
+    <t>Total places created between May 2010 and May 2022</t>
   </si>
 </sst>
 </file>
@@ -1394,8 +1394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8372DA64-5E2C-41C1-8CF4-85BC1C2AFF86}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1429,7 +1429,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>2</v>
@@ -1438,175 +1438,175 @@
         <v>3</v>
       </c>
       <c r="E2" s="39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="8"/>
       <c r="B3" s="38"/>
       <c r="C3" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E3" s="38"/>
     </row>
     <row r="4" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="40" t="s">
-        <v>90</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="E4" s="19" t="s">
         <v>62</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="8"/>
       <c r="B5" s="41"/>
       <c r="C5" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A6" s="8"/>
       <c r="B6" s="41"/>
       <c r="C6" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="8"/>
       <c r="B7" s="41"/>
       <c r="C7" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="218" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="8"/>
       <c r="B8" s="38"/>
       <c r="C8" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="32"/>
       <c r="D9" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C10" s="32" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="409.6" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="21"/>
       <c r="D11" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B12" s="35" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D12" s="25" t="s">
         <v>16</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="8"/>
       <c r="B13" s="31"/>
       <c r="C13" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="232.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="12"/>
       <c r="B14" s="36"/>
       <c r="C14" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="E14" s="30" t="s">
         <v>36</v>
-      </c>
-      <c r="E14" s="30" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1666,55 +1666,55 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E2" s="40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="8"/>
       <c r="B3" s="38"/>
       <c r="C3" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E3" s="38"/>
     </row>
     <row r="4" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="8"/>
       <c r="B4" s="42" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="24" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="9"/>
       <c r="B5" s="43"/>
       <c r="C5" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E5" s="43"/>
     </row>
@@ -1770,14 +1770,14 @@
     </row>
     <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A2" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="30" t="s">
         <v>45</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>46</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" s="30" t="s">
         <v>18</v>
@@ -1785,14 +1785,14 @@
     </row>
     <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="19" t="s">
         <v>48</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>49</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" s="19" t="s">
         <v>18</v>
@@ -1841,36 +1841,36 @@
     </row>
     <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="D2" s="25" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="11"/>
       <c r="B3" s="15"/>
       <c r="C3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="23" t="s">
         <v>53</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>54</v>
       </c>
       <c r="E3" s="15"/>
     </row>
     <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" s="11"/>
       <c r="B4" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>6</v>
@@ -1879,7 +1879,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
@@ -1887,7 +1887,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>8</v>
@@ -1960,13 +1960,13 @@
         <v>23</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D2" s="22" t="s">
         <v>25</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -2021,11 +2021,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="ec07c698-60f5-424f-b9af-f4c59398b511" ContentTypeId="0x010100545E941595ED5448BA61900FDDAFF313" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -2075,61 +2070,12 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="ec07c698-60f5-424f-b9af-f4c59398b511" ContentTypeId="0x010100545E941595ED5448BA61900FDDAFF313" PreviousValue="false"/>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
-      <Value>5</Value>
-      <Value>25</Value>
-      <Value>1</Value>
-      <Value>4</Value>
-    </TaxCatchAll>
-    <p6919dbb65844893b164c5f63a6f0eeb xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">DfE</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">a484111e-5b24-4ad9-9778-c536c8c88985</TermId>
-        </TermInfo>
-      </Terms>
-    </p6919dbb65844893b164c5f63a6f0eeb>
-    <c02f73938b5741d4934b358b31a1b80f xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Official</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">0884c477-2e62-47ea-b19c-5af6e91124c5</TermId>
-        </TermInfo>
-      </Terms>
-    </c02f73938b5741d4934b358b31a1b80f>
-    <f6ec388a6d534bab86a259abd1bfa088 xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">DfE</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">cc08a6d4-dfde-4d0f-bd85-069ebcef80d5</TermId>
-        </TermInfo>
-      </Terms>
-    </f6ec388a6d534bab86a259abd1bfa088>
-    <i98b064926ea4fbe8f5b88c394ff652b xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </i98b064926ea4fbe8f5b88c394ff652b>
-    <_dlc_DocIdUrl xmlns="2a6436df-3f7a-48ac-8ea6-44b411e24bbc">
-      <Url>https://educationgovuk.sharepoint.com/sites/efappp/_layouts/15/DocIdRedir.aspx?ID=FKMV6N5X2MYP-1953928680-73356</Url>
-      <Description>FKMV6N5X2MYP-1953928680-73356</Description>
-    </_dlc_DocIdUrl>
-    <_dlc_DocId xmlns="2a6436df-3f7a-48ac-8ea6-44b411e24bbc">FKMV6N5X2MYP-1953928680-73356</_dlc_DocId>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Official Document" ma:contentTypeID="0x010100545E941595ED5448BA61900FDDAFF31300C0D9F77D091A79449828113EF8250EF5" ma:contentTypeVersion="9" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="f90d64ba98617a6331a5780cc9b57993">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8c566321-f672-4e06-a901-b5e72b4c4357" xmlns:ns3="2a6436df-3f7a-48ac-8ea6-44b411e24bbc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a3658d73581f4a77afa8422430659c15" ns2:_="" ns3:_="">
     <xsd:import namespace="8c566321-f672-4e06-a901-b5e72b4c4357"/>
@@ -2335,7 +2281,69 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
+      <Value>5</Value>
+      <Value>25</Value>
+      <Value>1</Value>
+      <Value>4</Value>
+    </TaxCatchAll>
+    <p6919dbb65844893b164c5f63a6f0eeb xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">DfE</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">a484111e-5b24-4ad9-9778-c536c8c88985</TermId>
+        </TermInfo>
+      </Terms>
+    </p6919dbb65844893b164c5f63a6f0eeb>
+    <c02f73938b5741d4934b358b31a1b80f xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Official</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">0884c477-2e62-47ea-b19c-5af6e91124c5</TermId>
+        </TermInfo>
+      </Terms>
+    </c02f73938b5741d4934b358b31a1b80f>
+    <f6ec388a6d534bab86a259abd1bfa088 xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">DfE</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">cc08a6d4-dfde-4d0f-bd85-069ebcef80d5</TermId>
+        </TermInfo>
+      </Terms>
+    </f6ec388a6d534bab86a259abd1bfa088>
+    <i98b064926ea4fbe8f5b88c394ff652b xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </i98b064926ea4fbe8f5b88c394ff652b>
+    <_dlc_DocIdUrl xmlns="2a6436df-3f7a-48ac-8ea6-44b411e24bbc">
+      <Url>https://educationgovuk.sharepoint.com/sites/efappp/_layouts/15/DocIdRedir.aspx?ID=FKMV6N5X2MYP-1953928680-73356</Url>
+      <Description>FKMV6N5X2MYP-1953928680-73356</Description>
+    </_dlc_DocIdUrl>
+    <_dlc_DocId xmlns="2a6436df-3f7a-48ac-8ea6-44b411e24bbc">FKMV6N5X2MYP-1953928680-73356</_dlc_DocId>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9C56A4F-6917-41AA-BBE5-DA7C75896563}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D00F0DC4-2D9F-43FC-8616-EC131ED26B7D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
@@ -2343,18 +2351,21 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9C56A4F-6917-41AA-BBE5-DA7C75896563}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0969FC7E-EEEC-4315-900C-25F913AD1B6E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{035EEA42-582A-4724-B162-C22729062C2B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8c566321-f672-4e06-a901-b5e72b4c4357"/>
+    <ds:schemaRef ds:uri="2a6436df-3f7a-48ac-8ea6-44b411e24bbc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2377,20 +2388,9 @@
 </file>
 
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0969FC7E-EEEC-4315-900C-25F913AD1B6E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{035EEA42-582A-4724-B162-C22729062C2B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8c566321-f672-4e06-a901-b5e72b4c4357"/>
-    <ds:schemaRef ds:uri="2a6436df-3f7a-48ac-8ea6-44b411e24bbc"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated homepage and tech gudiance for cost
</commit_message>
<xml_diff>
--- a/data/tech_guidance.xlsx
+++ b/data/tech_guidance.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk.sharepoint.com/sites/efappp/WorkplaceDocuments/Data Team/Analysis/2023/Scorecard/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/simone_cardin-stewart_education_gov_uk/Documents/Documents/R/la-school-places-scorecards/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="250" documentId="8_{840724E6-C688-4ACB-8719-9DF4811675F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E823BB4-BCD7-46E9-A489-C683420B562D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D526DD1-D974-4CC6-AD68-810C619433ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="772" yWindow="862" windowWidth="14423" windowHeight="7208" xr2:uid="{9CCC1F63-2262-45DD-B4CA-7C937E5C8E7F}"/>
+    <workbookView xWindow="22450" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{9CCC1F63-2262-45DD-B4CA-7C937E5C8E7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Quantity" sheetId="2" r:id="rId1"/>
@@ -197,184 +197,7 @@
 </t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">1. The cost data used in the scorecard is the 2018 Capital Spend data as used in the 2018, 2019 and 2021 Scorecards. For the 2022 Scorecard, this data has been adjusted for inflation (rebased to 1st Quarter 2023 prices). National averages adjusted for 2023 regional location factors are shown. </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">You can use this data to establish developer contributions per school place, by adjusting for further inflation if needed </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(see examples below).
-&lt;br&gt;2. Projects which do not create additional mainstream places or where the project's additional place funding is zero are removed.
-&lt;br&gt;3. Projects were identified as primary  or secondary phase based on additional mainstream place year group breakdown. Where a project created places across both phases, it was assigned a phase corresponding to the phase of the school it affected (i.e. if its school was middle-deemed primary - the project was assigned to primary).
-&lt;br&gt;4. Average cost per place figures for all-through, middle-deemed primary and middle-deemed secondary schools have not been calculated separately due to low sample sizes for these project types. </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>To estimate average cost per place for middle-deemed primary schools, we recommend using primary average cost per place</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> as the middle school provides education equivalent to the education a primary school provides for all year groups. </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>To estimate average cost per place for middle-deemed secondary schools, we recommend using secondary average cost per place</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> for the same reason. </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>For new middle schools or whole school expansions for middle schools not ‘deemed’ primary or secondary, we recommend taking a mid-point of the primary and secondary costs if the project covers both primary- and secondary-equivalent year groups equally</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (e.g. 2 classes per Year 5 &amp; 6 and 2 classes per Year 7 &amp; 8). </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>If the project only covers certain year groups, we recommend using primary cost data if only primary-equivalent years groups are expanding</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (e.g. Years 5 &amp; 6) and </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>secondary data if only secondary-equivalent year groups are expanding</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (e.g. Years 7 &amp; 8).
-&lt;br&gt;5. The average cost does not include costs associated with land acquisition.
-&lt;br&gt;6. The average cost includes costs associated with maintenance and building condition or enhancement works.
-&lt;br&gt;7. The measure does not include places in special schools or units attached to mainstream schools, or new places which were funded through central programmes (including free schools). Where a project creates additional mainstream places and also creates SEN places or re-provides places, an adjustment has been applied to apportion out those costs. 
-&lt;br&gt;8. All costs have been normalised to a common UK average price level using regional location factors published by BCIS, March 2023, 1 is the base weight.
-&lt;br&gt;9. All costs have been adjusted for inflation using the latest BCIS All-In Tender Price of Index (TPI), published March 2023.  Costs have been rebased from the start of construction (or time of place provision if construction start date unavailable) to 1st Quarter (Jan – Mar) 2023 prices using this index (Q1 2023 index value = 379).
-10. </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>To adjust the national average to current or future prices, you need to uprate or downrate the prices in this scorecard relative to the change that has happened since Q1 2023</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.  If you have access to the BCIS indices via a subscription to BCIS Online (https://www.rics.org/uk/products/data-products/bcis-construction/bcis-online/) you can use the latest inflation index to re-base (weight to apply = latest index/379).  If not, you can apply a known change to the published cost (e.g. up or down x%).
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Example: New primary school in Outer London Q3 (Jul - Sep) 2023.  
-National average for primary new school place = £23,192. 
-Outer London location factor = 1.21 (taken from published BCIS regional location factors March 2023)
-Inflation weight = 383/379 = 1.01 ( taken from BCIS All-In TPI published March 2023). 
-Average primary New School place cost that applies to Outer London in Q3 2023 prices = £23,192 x 1.21 x 1.01 = £28,300 (rounded to nearest £100).  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-If you do not have access the BCIS index, but sources say TPI inflation is set to increase by 4% per annum, then approximate inflation weight = 6% (18 months’ worth of inflation) = 1.06.
-11. Some additional but limited benchmark information for similar capital programme schemes carried out by the DfE is available in the National School Delivery Cost Benchmarking study: https://ebdog.org.uk/wp-content/uploads/2019/06/F07125-National-School-Delivery-Cost-Benchmarking-Primary-Secondary-and--SEN-Schools-Final-June-2019-v6.7a.pdf.</t>
-    </r>
-  </si>
-  <si>
     <t>5. Total number of planned places (sum of 1, 2, 3, 4 and 5 above)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The national average has been adjusted to the relevant region for each local authority, using the Building Cost Information Service (BCIS) March 2023 published regional location factors. The England national average has been multiplied by the relevant regional location factor:  East Midlands: 1.03, East of England 0.99, Inner London: 1.29, North East: 0.91, North West: 1, Outer London: 1.21, South East: 1.13, South West: 1.01, West Midlands: 0.96, Yorkshire &amp; the Humber: 0.91. </t>
   </si>
   <si>
     <t xml:space="preserve">1. Number of pupils in roll in January 2010, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. </t>
@@ -676,6 +499,183 @@
     <t>1. Each school has been matched with the Ofsted judgement of 'Overall effectiveness: how good is the school." as at 31 August 2023 (published November 2023).
 &lt;br&gt;2. There are four Ofsted categories: 'Outstanding', 'Good', 'Requires improvement' and 'Inadequate'.
 &lt;br&gt;3. The calculation counts the number of existing and new places that have been created in schools of each category. &lt;br&gt;4. Note that many schools will have been inspected some time before August 2023, and some will have been inspected since this date. &lt;br&gt;5. There are school places with no rating, as the school has yet to be inspected so do not have an Ofsted judgement.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The national average has been adjusted to the relevant region for each local authority, using the Building Cost Information Service (BCIS) March 2024 published regional location factors. The England national average has been multiplied by the relevant regional location factor:  East Midlands: 1.03, East of England 0.99, Inner London: 1.29, North East: 0.91, North West: 1, Outer London: 1.21, South East: 1.13, South West: 1.01, West Midlands: 0.96, Yorkshire &amp; the Humber: 0.91. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. The cost data used in the scorecard is the 2018 Capital Spend data as used in the 2018, 2019 and 2021 Scorecards. For the 2023 Scorecard, this data has been adjusted for inflation (rebased to 1st Quarter 2024 prices). National averages adjusted for 2023 regional location factors are shown. </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">You can use this data to establish developer contributions per school place, by adjusting for further inflation if needed </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(see examples below).
+&lt;br&gt;2. Projects which do not create additional mainstream places or where the project's additional place funding is zero are removed.
+&lt;br&gt;3. Projects were identified as primary  or secondary phase based on additional mainstream place year group breakdown. Where a project created places across both phases, it was assigned a phase corresponding to the phase of the school it affected (i.e. if its school was middle-deemed primary - the project was assigned to primary).
+&lt;br&gt;4. Average cost per place figures for all-through, middle-deemed primary and middle-deemed secondary schools have not been calculated separately due to low sample sizes for these project types. </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>To estimate average cost per place for middle-deemed primary schools, we recommend using primary average cost per place</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> as the middle school provides education equivalent to the education a primary school provides for all year groups. </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>To estimate average cost per place for middle-deemed secondary schools, we recommend using secondary average cost per place</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for the same reason. </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>For new middle schools or whole school expansions for middle schools not ‘deemed’ primary or secondary, we recommend taking a mid-point of the primary and secondary costs if the project covers both primary- and secondary-equivalent year groups equally</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (e.g. 2 classes per Year 5 &amp; 6 and 2 classes per Year 7 &amp; 8). </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If the project only covers certain year groups, we recommend using primary cost data if only primary-equivalent years groups are expanding</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (e.g. Years 5 &amp; 6) and </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>secondary data if only secondary-equivalent year groups are expanding</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (e.g. Years 7 &amp; 8).
+&lt;br&gt;5. The average cost does not include costs associated with land acquisition.
+&lt;br&gt;6. The average cost includes costs associated with maintenance and building condition or enhancement works.
+&lt;br&gt;7. The measure does not include places in special schools or units attached to mainstream schools, or new places which were funded through central programmes (including free schools). Where a project creates additional mainstream places and also creates SEN places or re-provides places, an adjustment has been applied to apportion out those costs. 
+&lt;br&gt;8. All costs have been normalised to a common UK average price level using regional location factors published by BCIS, March 2024, 1 is the base weight.
+&lt;br&gt;9. All costs have been adjusted for inflation using the latest BCIS All-In Tender Price of Index (TPI), published March 2024.  Costs have been rebased from the start of construction (or time of place provision if construction start date unavailable) to 1st Quarter (Jan – Mar) 2024 prices using this index (Q1 2024 index value = 390).
+10. </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>To adjust the national average to current or future prices, you need to uprate or downrate the prices in this scorecard relative to the change that has happened since Q1 2024</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.  If you have access to the BCIS indices via a subscription to BCIS Online (https://www.rics.org/uk/products/data-products/bcis-construction/bcis-online/) you can use the latest inflation index to re-base (weight to apply = latest index/390).  If not, you can apply a known change to the published cost (e.g. up or down x%).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Example: New primary school in Outer London Q3 (Jul - Sep) 2024.  
+National average for primary new school place = £23,865. 
+Outer London location factor = 1.21 (taken from published BCIS regional location factors March 2023)
+Inflation weight = 394/390 = 1.01 ( taken from BCIS All-In TPI published March 2023). 
+Average primary New School place cost that applies to Outer London in Q3 2023 prices = £23,192 x 1.21 x 1.01 = £29,200 (rounded to nearest £100).  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+If you do not have access the BCIS index, but sources say TPI inflation is set to increase by 4% per annum, then approximate inflation weight = 6% (18 months’ worth of inflation) = 1.06.
+11. Some additional but limited benchmark information for similar capital programme schemes carried out by the DfE is available in the National School Delivery Cost Benchmarking study: https://documents.hants.gov.uk/property-services/NationalSchoolDeliveryBenchmarkingreport.pdf</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1196,6 +1196,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1497,8 +1501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8372DA64-5E2C-41C1-8CF4-85BC1C2AFF86}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B8"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1532,7 +1536,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>2</v>
@@ -1541,35 +1545,35 @@
         <v>3</v>
       </c>
       <c r="E2" s="48" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="87" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="8"/>
       <c r="B3" s="47"/>
       <c r="C3" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E3" s="47"/>
     </row>
     <row r="4" spans="1:5" ht="138" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="16" t="s">
+      <c r="E4" s="13" t="s">
         <v>41</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
@@ -1582,99 +1586,99 @@
         <v>4</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A6" s="8"/>
       <c r="B6" s="50"/>
       <c r="C6" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A7" s="8"/>
       <c r="B7" s="50"/>
       <c r="C7" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="85.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="8"/>
       <c r="B8" s="47"/>
       <c r="C8" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A9" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B9" s="36" t="s">
         <v>29</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="327.75" x14ac:dyDescent="0.45">
       <c r="A10" s="33" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C10" s="21" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="185.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>30</v>
@@ -1683,33 +1687,33 @@
         <v>16</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="57" x14ac:dyDescent="0.45">
       <c r="A13" s="8"/>
       <c r="B13" s="22"/>
       <c r="C13" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="21" t="s">
         <v>59</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="100.15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="9"/>
       <c r="B14" s="27"/>
       <c r="C14" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="31" t="s">
         <v>62</v>
-      </c>
-      <c r="D14" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14" s="31" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1766,55 +1770,55 @@
     </row>
     <row r="2" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="49" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="13" t="s">
+      <c r="D2" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="E2" s="49" t="s">
         <v>69</v>
-      </c>
-      <c r="E2" s="49" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="33"/>
       <c r="B3" s="52"/>
       <c r="C3" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="38" t="s">
         <v>68</v>
-      </c>
-      <c r="D3" s="38" t="s">
-        <v>70</v>
       </c>
       <c r="E3" s="52"/>
     </row>
     <row r="4" spans="1:5" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="33"/>
       <c r="B4" s="49" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D4" s="39" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="49" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="40"/>
       <c r="B5" s="51"/>
       <c r="C5" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E5" s="51"/>
     </row>
@@ -1880,14 +1884,14 @@
     </row>
     <row r="3" spans="1:5" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A3" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>17</v>
@@ -1934,38 +1938,38 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="384.75" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" ht="399" x14ac:dyDescent="0.45">
       <c r="A2" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>79</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>81</v>
       </c>
       <c r="D2" s="37" t="s">
         <v>28</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="42"/>
       <c r="B3" s="43"/>
       <c r="C3" s="13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D3" s="38" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E3" s="43"/>
     </row>
     <row r="4" spans="1:5" ht="128.25" x14ac:dyDescent="0.45">
       <c r="A4" s="42"/>
       <c r="B4" s="44" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>6</v>
@@ -1974,7 +1978,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="57" x14ac:dyDescent="0.45">
@@ -1982,7 +1986,7 @@
         <v>18</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>8</v>
@@ -1994,7 +1998,7 @@
     </row>
     <row r="6" spans="1:5" ht="114" x14ac:dyDescent="0.45">
       <c r="A6" s="28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B6" s="28" t="s">
         <v>19</v>
@@ -2007,88 +2011,88 @@
     </row>
     <row r="7" spans="1:5" ht="199.5" x14ac:dyDescent="0.45">
       <c r="A7" s="28" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B7" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>88</v>
-      </c>
       <c r="D7" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" s="30" t="s">
         <v>87</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="185.25" x14ac:dyDescent="0.45">
       <c r="A8" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>93</v>
-      </c>
       <c r="D8" s="29" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A9" s="28" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="29"/>
       <c r="E9" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A10" s="28" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="29"/>
       <c r="E10" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A11" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="28" t="s">
         <v>94</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>96</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A12" s="28" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -2107,8 +2111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB73E146-A141-4797-B302-F0B3455C0C2E}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="57.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2141,13 +2145,13 @@
         <v>21</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>33</v>
+        <v>106</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>23</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
@@ -2202,6 +2206,51 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
+      <Value>5</Value>
+      <Value>25</Value>
+      <Value>1</Value>
+      <Value>4</Value>
+    </TaxCatchAll>
+    <p6919dbb65844893b164c5f63a6f0eeb xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">DfE</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">a484111e-5b24-4ad9-9778-c536c8c88985</TermId>
+        </TermInfo>
+      </Terms>
+    </p6919dbb65844893b164c5f63a6f0eeb>
+    <c02f73938b5741d4934b358b31a1b80f xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Official</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">0884c477-2e62-47ea-b19c-5af6e91124c5</TermId>
+        </TermInfo>
+      </Terms>
+    </c02f73938b5741d4934b358b31a1b80f>
+    <f6ec388a6d534bab86a259abd1bfa088 xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">DfE</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">cc08a6d4-dfde-4d0f-bd85-069ebcef80d5</TermId>
+        </TermInfo>
+      </Terms>
+    </f6ec388a6d534bab86a259abd1bfa088>
+    <i98b064926ea4fbe8f5b88c394ff652b xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </i98b064926ea4fbe8f5b88c394ff652b>
+    <_dlc_DocIdUrl xmlns="2a6436df-3f7a-48ac-8ea6-44b411e24bbc">
+      <Url>https://educationgovuk.sharepoint.com/sites/efappp/_layouts/15/DocIdRedir.aspx?ID=FKMV6N5X2MYP-1953928680-76369</Url>
+      <Description>FKMV6N5X2MYP-1953928680-76369</Description>
+    </_dlc_DocIdUrl>
+    <_dlc_DocId xmlns="2a6436df-3f7a-48ac-8ea6-44b411e24bbc">FKMV6N5X2MYP-1953928680-76369</_dlc_DocId>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Official Document" ma:contentTypeID="0x010100545E941595ED5448BA61900FDDAFF31300C0D9F77D091A79449828113EF8250EF5" ma:contentTypeVersion="9" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="3acf8af8f3f036fb6d934619e757bc96">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8c566321-f672-4e06-a901-b5e72b4c4357" xmlns:ns3="2a6436df-3f7a-48ac-8ea6-44b411e24bbc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="926947be84ee9a0228ce6a037c6848ba" ns2:_="" ns3:_="">
     <xsd:import namespace="8c566321-f672-4e06-a901-b5e72b4c4357"/>
@@ -2407,58 +2456,9 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
-      <Value>5</Value>
-      <Value>25</Value>
-      <Value>1</Value>
-      <Value>4</Value>
-    </TaxCatchAll>
-    <p6919dbb65844893b164c5f63a6f0eeb xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">DfE</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">a484111e-5b24-4ad9-9778-c536c8c88985</TermId>
-        </TermInfo>
-      </Terms>
-    </p6919dbb65844893b164c5f63a6f0eeb>
-    <c02f73938b5741d4934b358b31a1b80f xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Official</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">0884c477-2e62-47ea-b19c-5af6e91124c5</TermId>
-        </TermInfo>
-      </Terms>
-    </c02f73938b5741d4934b358b31a1b80f>
-    <f6ec388a6d534bab86a259abd1bfa088 xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">DfE</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">cc08a6d4-dfde-4d0f-bd85-069ebcef80d5</TermId>
-        </TermInfo>
-      </Terms>
-    </f6ec388a6d534bab86a259abd1bfa088>
-    <i98b064926ea4fbe8f5b88c394ff652b xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </i98b064926ea4fbe8f5b88c394ff652b>
-    <_dlc_DocIdUrl xmlns="2a6436df-3f7a-48ac-8ea6-44b411e24bbc">
-      <Url>https://educationgovuk.sharepoint.com/sites/efappp/_layouts/15/DocIdRedir.aspx?ID=FKMV6N5X2MYP-1953928680-76369</Url>
-      <Description>FKMV6N5X2MYP-1953928680-76369</Description>
-    </_dlc_DocIdUrl>
-    <_dlc_DocId xmlns="2a6436df-3f7a-48ac-8ea6-44b411e24bbc">FKMV6N5X2MYP-1953928680-76369</_dlc_DocId>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="ec07c698-60f5-424f-b9af-f4c59398b511" ContentTypeId="0x010100545E941595ED5448BA61900FDDAFF313" PreviousValue="false"/>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2513,10 +2513,31 @@
 
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="ec07c698-60f5-424f-b9af-f4c59398b511" ContentTypeId="0x010100545E941595ED5448BA61900FDDAFF313" PreviousValue="false"/>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{334E8BC2-6B82-4EDA-BE50-EFE4767E8CD2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="8c566321-f672-4e06-a901-b5e72b4c4357"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2a6436df-3f7a-48ac-8ea6-44b411e24bbc"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1E94FF3-D2F7-4169-BE5C-5ED202BAA024}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2535,27 +2556,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{334E8BC2-6B82-4EDA-BE50-EFE4767E8CD2}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D00F0DC4-2D9F-43FC-8616-EC131ED26B7D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="8c566321-f672-4e06-a901-b5e72b4c4357"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2a6436df-3f7a-48ac-8ea6-44b411e24bbc"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{035EEA42-582A-4724-B162-C22729062C2B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2569,9 +2573,9 @@
 </file>
 
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D00F0DC4-2D9F-43FC-8616-EC131ED26B7D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{035EEA42-582A-4724-B162-C22729062C2B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updates for 2024 scorecard
</commit_message>
<xml_diff>
--- a/data/tech_guidance.xlsx
+++ b/data/tech_guidance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/simone_cardin-stewart_education_gov_uk/Documents/Documents/R/la-school-places-scorecards/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/robert_miller_education_gov_uk/Documents/Documents/R/la-school-places-scorecard-internal/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D526DD1-D974-4CC6-AD68-810C619433ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="8_{88D981E4-01D0-41D1-BFE9-9F41107BE635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{364AACDB-AEE9-4581-B73A-D53239F4F61E}"/>
   <bookViews>
-    <workbookView xWindow="22450" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{9CCC1F63-2262-45DD-B4CA-7C937E5C8E7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{9CCC1F63-2262-45DD-B4CA-7C937E5C8E7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Quantity" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="110">
   <si>
     <t>Notes</t>
   </si>
@@ -145,9 +145,6 @@
     <t>Places created since 2009/10</t>
   </si>
   <si>
-    <t>Local authority data provided through the School Capacity (SCAP) Collection 2021</t>
-  </si>
-  <si>
     <t>School census Jan 2010 data</t>
   </si>
   <si>
@@ -158,13 +155,6 @@
     <t>Percentage of new places created in good and outstanding schools</t>
   </si>
   <si>
-    <t>Ranks local authorities on their proportion of new school places which are in good and outstanding schools</t>
-  </si>
-  <si>
-    <t>1. Ranking of proportions of new places created in 'good' or 'outstanding' schools for each local authority, amongst all local authorities with new places. Local authorities with the same proportion are given an equal ranking. Ranking is only applied to local authorities where new places have been created.
-&lt;br&gt;2. The higher the rank the higher the proportion of new school places in good and outstanding schools compared to other local authorities. &lt;br&gt;3. Ranks can be tied and there will many local authorities with a rank of 1 due to 100% of new places in good and outstanding schools.</t>
-  </si>
-  <si>
     <t xml:space="preserve">The national average cost per place of permanent expansion, temporary expansion and new school projects in England. </t>
   </si>
   <si>
@@ -178,18 +168,6 @@
     <t>2. Capacity changes through the CIF, SRP, SSEF, VA.</t>
   </si>
   <si>
-    <t>School place offers by preference for September 2023 entry</t>
-  </si>
-  <si>
-    <t>The proportion of applicants who received an offer of a place in one of their top three preference schools for September 2023 on national offer day</t>
-  </si>
-  <si>
-    <t>Published School Applications and Offer data 2023/24 Academic Year</t>
-  </si>
-  <si>
-    <t>Local authority data, provided through School Capacity collection 2022</t>
-  </si>
-  <si>
     <t>Unfilled places as a percentage of total places</t>
   </si>
   <si>
@@ -197,152 +175,175 @@
 </t>
   </si>
   <si>
-    <t>5. Total number of planned places (sum of 1, 2, 3, 4 and 5 above)</t>
-  </si>
-  <si>
     <t xml:space="preserve">1. Number of pupils in roll in January 2010, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. </t>
   </si>
   <si>
     <t>1. This relates to the difference between number of pupils on roll and capacity, in schools where the number on roll is lower than a school's reported capacity. &lt;br&gt;2. Calculated at school level and aggregated to local authority level.</t>
   </si>
   <si>
-    <t>Total places created between May 2010 and May 2023</t>
-  </si>
-  <si>
-    <t>2.Capacity at May 2023</t>
-  </si>
-  <si>
-    <t>1. The number of places that have been created since May 2010 in each local authority is taken as the difference between capacity as reported by local authorities, via SCAP, at May 2010 and May 2023.
+    <t>School place offers by preference for September 2024 entry</t>
+  </si>
+  <si>
+    <t>The proportion of applicants who received an offer of a place in one of their top three preference schools for September 2024 on national offer day</t>
+  </si>
+  <si>
+    <t>Published School Applications and Offer data 2024/25 Academic Year</t>
+  </si>
+  <si>
+    <t>Local authority data, provided through School Capacity collection 2023</t>
+  </si>
+  <si>
+    <t>Performance tables</t>
+  </si>
+  <si>
+    <t>Key stage 2 progress measures</t>
+  </si>
+  <si>
+    <t>Key stage 4 progress 8 measure</t>
+  </si>
+  <si>
+    <t>1. Ranking of proportions of new places created in 'well above average' and 'above average' schools for each local authority, amongst all local authorities with new places. Local authorities with the same proportion are given an equal ranking. Ranking is only applied to local authorities where new places have been created.
+2. The higher the rank the higher the proportion of new school places in well above and above average schools compared to other local authorities.</t>
+  </si>
+  <si>
+    <t>1. Ranking of proportions of new places created in 'well above average' and 'above average' schools for each local authority, amongst all local authorities with new places. Local authorities with the same proportion are given an equal ranking. Ranking is only applied to local authorities where new places have been created. 
+2. The higher the rank the higher the proportion of new school places in well above and above average schools compared to other local authorities.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DfE internal model. Additional places needed are published in the school place planning published underlying data. </t>
+  </si>
+  <si>
+    <t>Percentage of  new school places in well above and above-average schools- key stage 2 measures</t>
+  </si>
+  <si>
+    <t>Percentage of  new school places in well above and above-average schools- key stage 4 progress 8 measure</t>
+  </si>
+  <si>
+    <t>Total places created between May 2010 and May 2024</t>
+  </si>
+  <si>
+    <t>2.Capacity at May 2024</t>
+  </si>
+  <si>
+    <t>Local authority data provided through School Capacity (SCAP) Survey 2024</t>
+  </si>
+  <si>
+    <t>1. The number of places that have been created since May 2010 in each local authority is taken as the difference between capacity as reported by local authorities, via SCAP, at May 2010 and May 2024.
 &lt;br&gt;2. The measure includes all primary and middle deemed primary school capacity in the primary phase, and all secondary, middle deemed secondary and all-through school capacity in the secondary phase.
-&lt;br&gt;3. The measure reports net increase in places only, if phase capacity in a local authority has reduced between May 2010 and May 2023, this is recorded as zero places created. Therefore the sum of the local authority-level figures will not equal the overall increase in places at national level.</t>
-  </si>
-  <si>
-    <t>Places planned to 2025/26</t>
-  </si>
-  <si>
-    <t>1. Local authority plans for places to be created or removed between May 2023 and before the start of the 2025/26 academic year.</t>
-  </si>
-  <si>
-    <t>Local authority data provided through the School Capacity (SCAP) Survey 2023.</t>
-  </si>
-  <si>
-    <t>Local authority data provided through School Capacity (SCAP) Survey 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Local authority data about new permanent additional places, new temporary bulge places (to accommodate large cohorts as they move through the school) and permanent places to remove  2023/24, 2024/25  and 2025/26 is aggregated to local authority level.
-&lt;br&gt;2. The data was provided by local authorities in May 2023, and only includes projects they were confident would proceed. Local authorities were asked to include the total places of any new provision, even if spaces would fill gradually. 
+&lt;br&gt;3. The measure reports net increase in places only, if phase capacity in a local authority has reduced between May 2010 and May 2024, this is recorded as zero places created. Therefore the sum of the local authority-level figures will not equal the overall increase in places at national level.</t>
+  </si>
+  <si>
+    <t>Number of new places planned for delivery between May 2024 and September 2026;
+&lt;br&gt;This contains: 
+&lt;br&gt;1) local authority firm plans for new permanent additional places , new temporary bulge places and the removal of places,
+&lt;br&gt;2) capacity changes through the Condition Improvement Fund (CIF), School Rebuilding Programme (SRP), Selective Schools Expansion Fund (SSEF), and Voluntary Aided Schools Fund (VA)
+&lt;br&gt;3) places from free schools opened in September 2024 and planned to open in September 2025
+&lt;br&gt;4) reduction in places from free school and academy closures.</t>
+  </si>
+  <si>
+    <t>1. Local authority plans for places to be created or removed between May 2024 and before the start of the 2026/27 academic year.</t>
+  </si>
+  <si>
+    <t>3. Places from free schools opened in September 2024 and due to be opened in September 2025.</t>
+  </si>
+  <si>
+    <t>4. Reduction in places from free school and academy closures between May 2024 and January 2025 or identified/confirmed to close before August 2025.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Local authority data about new permanent additional places, new temporary bulge places (to accommodate large cohorts as they move through the school) and permanent places to remove  2024/25, 2025/26  and 2026/27 is aggregated to local authority level.
+&lt;br&gt;2. The data was provided by local authorities in May 2024, and only includes projects they were confident would proceed. Local authorities were asked to include the total places of any new provision, even if spaces would fill gradually. 
 &lt;br&gt;3. Local authorities were asked not to include places created through free schools unless they were providing the funding for additional places themselves. </t>
   </si>
   <si>
-    <t xml:space="preserve">1. Changes to school capacity (both increases and decreases) as a consequence of works delivered through the CIF, SRP, SSEF, VA between 2023/24 and 2025/26 inclusive, aggregated to local authority level. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. The calculation mirrors the approach taken for basic need funding allocations published in March 2024. It includes mainstream primary and secondary free schools which opened in September 2023 and those with a high degree of certainty of opening in September 2024, and counts the total number of places which will be in use by September 2025.
-&lt;br&gt;2. The data does not include free schools which opened before September 2023, as they will already be included in SCAP23 and are therefore existing places. It does not include free schools which are planned to open in the academic year 2025/26 and beyond. </t>
-  </si>
-  <si>
-    <t>3. Places from free schools opened in September 2023 and due to be opened in September 2024.</t>
-  </si>
-  <si>
-    <t>4. Reduction in places from free school and academy closures between May 2023 and January 2024 or identified/confirmed to close before August 2024.</t>
-  </si>
-  <si>
-    <t>1. Where an academy or free school closed after 1 May 2023 its capacity, as reported in the School Capacity data, is now no longer available. Their capacity has therefore been removed from the planned delivery total.</t>
+    <t xml:space="preserve">1. Changes to school capacity (both increases and decreases) as a consequence of works delivered through the CIF, SRP, SSEF, VA between 2024/25 and 2026/27 inclusive, aggregated to local authority level. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. The calculation mirrors the approach taken for basic need funding allocations published in March 2025. It includes mainstream primary and secondary free schools which opened in September 2024 and those with a high degree of certainty of opening in September 2025, and counts the total number of places which will be in use by September 2026.
+&lt;br&gt;2. The data does not include free schools which opened before September 2024, as they will already be included in SCAP24 and are therefore existing places. It does not include free schools which are planned to open in the academic year 2026/27 and beyond. </t>
+  </si>
+  <si>
+    <t>1. Where an academy or free school closed after 1 May 2024 its capacity, as reported in the School Capacity data, is now no longer available. Their capacity has therefore been removed from the planned delivery total.</t>
   </si>
   <si>
     <t xml:space="preserve">1. This measure reports planned increases in capacity only. If there is a total net planned reduction in capacity (e.g. due to a free school closure), this is shown as zero places planned. Therefore the sum of local authority-level figures will not equal the national planned places figure.
-&lt;br&gt;2. Most local authorities will have further developed their plans since this data was reported in Summer 2023, and so although it allows for comparisons between local authorities, the figure is likely to be an understatement of the current position. </t>
-  </si>
-  <si>
-    <t>Unfilled places in 2022/23</t>
-  </si>
-  <si>
-    <t>Additional places needed in 2025/26; spare places in 2025/26</t>
-  </si>
-  <si>
-    <t>Estimated number of additional places needed to meet demand in 2025/26; estimated percentage of spare places in 2025/26.</t>
-  </si>
-  <si>
-    <t>1.This relates to the academic year 2025/26 and is the difference between local authority pupil forecasts and future capacity, taking account of planned future additions and places to remove.
-     places needed = forecast demand - (existing capacity + additional capacity - places to remove).  
-For further information on the methodology used, see the School Place Planning 2023: technical note found on the School Capacity 23 publication on Explore Education Statistics.
-&lt;br&gt;2. Where demand is greater than capacity a need for additional places results; where capacity is greater than demand spare places result. 
-&lt;br&gt;3. Local authority pupil forecasts for 2025/26 are collected through SCAP 2023&lt;br&gt;4. Additional capacity as at 2025/26 includes places that the local authority plans to add or remove between May 2023 and before the start of the 2025/26 academic year and places from programmes centrally funded by the department, as described above. 
-&lt;br&gt;5. The comparison of demand and capacity takes place for each national curriculum year group within each planning area to estimate places needed in each. The estimates in the scorecard do not allow for spare capacity in one year group or planning area to be off-set against need in another, or vice-versa. This avoids the risk of spare places in one or more planning areas masking areas of need for additional places in planning areas elsewhere in the local authority. For further information see the School Place Planning Tables 2023: technical note.
-&lt;br&gt;6. The estimated need for additional places and estimated spare places is calculated at planning area level and then aggregated to local authority level. It is common for a local authority to have both a need for additional places and spare places, reflecting pockets of localised need for places or pockets of localised spare places.
-&lt;br&gt;7. Estimates for need are rounded to the nearest 10.
-&lt;br&gt;8. Estimates for spare places are presented as a percentage of total future capacity.</t>
-  </si>
-  <si>
-    <t>Total basic need funding 2011 to 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total amount of basic need capital funding allocated to each local authority to support them to create new mainstream primary and secondary places from 2011 to 2025. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. This refers to the amount of basic need capital funding that the Department for Education (DfE) has allocated to each local authority to create new places from the 2011-12 financial year to the 2024-25 financial year. Basic Need funding for the 2024-25 financial year is intended to support the creation of mainstream places for pupils aged 5 to 16 for the 2025/26 academic year. &lt;br&gt;2. The figure includes formula-based funding allocations and funding provided through the Targeted Basic Need Programme. Basic Need formula-based funding allocations cover the whole period and are not ring-fenced (although they can only be used for capital purposes).  Targeted Basic Need funding was provided between 2013 and 2015 and had to be spent by agreed deadlines and on specific projects. Both types of allocations are published here. &lt;br&gt;3. The figure only includes funding allocated to local authorities and does not include centrally-funded capital programmes such as the free schools programme. &lt;br&gt;4. The England total will not match the sum of allocations for all local authorities in the scorecard because the England total includes allocations to predecessor local authorities.
+&lt;br&gt;2. Most local authorities will have further developed their plans since this data was reported in Summer 2024, and so although it allows for comparisons between local authorities, the figure is likely to be an understatement of the current position. </t>
+  </si>
+  <si>
+    <t>Places planned to 2026/27</t>
+  </si>
+  <si>
+    <t>Unfilled places in 2023/24</t>
+  </si>
+  <si>
+    <t>Additional places needed in 2026/27; spare places in 2026/27</t>
+  </si>
+  <si>
+    <t>Estimated number of additional places needed to meet demand in 2026/27; estimated percentage of spare places in 2026/27.</t>
+  </si>
+  <si>
+    <t>Total basic need funding 2011 to 2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total amount of basic need capital funding allocated to each local authority to support them to create new mainstream primary and secondary places from 2011 to 2026. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. This refers to the amount of basic need capital funding that the Department for Education (DfE) has allocated to each local authority to create new places from the 2011-12 financial year to the 2025-26 financial year. Basic Need funding for the 2025-26 financial year is intended to support the creation of mainstream places for pupils aged 5 to 16 for the 2026/27 academic year. &lt;br&gt;2. The figure includes formula-based funding allocations and funding provided through the Targeted Basic Need Programme. Basic Need formula-based funding allocations cover the whole period and are not ring-fenced (although they can only be used for capital purposes).  Targeted Basic Need funding was provided between 2013 and 2015 and had to be spent by agreed deadlines and on specific projects. Both types of allocations are published here. &lt;br&gt;3. The figure only includes funding allocated to local authorities and does not include centrally-funded capital programmes such as the free schools programme. &lt;br&gt;4. The England total will not match the sum of allocations for all local authorities in the scorecard because the England total includes allocations to predecessor local authorities.
 </t>
   </si>
   <si>
-    <t>The actual percentage change in pupil numbers between 2009/10 and 2023/24; the anticipated percentage change in pupil numbers in primary or secondary state-funded mainstream provision between the 2023/24 and 2025/26 academic years.</t>
-  </si>
-  <si>
     <t>Change in pupil numbers
-2009/10 to 2023/24; Anticipated change in pupil numbers 2023/24 to 2025/26</t>
-  </si>
-  <si>
-    <t>2. Pupil Numbers for the 2023/24 academic year taken from the pupil census in January 2024</t>
-  </si>
-  <si>
-    <t>School census Jan 2024 data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Number of pupils in roll in January 2024, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. 							</t>
-  </si>
-  <si>
-    <t>2. Forecast pupil numbers for the 2025/26 academic year</t>
-  </si>
-  <si>
-    <t>Local authority data provided through the  School Capacity (SCAP) Collection 2023</t>
-  </si>
-  <si>
-    <t>1. This is the local authority's forecast of pupil numbers for the academic year 2025/26 as provided in SCAP 2023.
+2009/10 to 2024/25; Anticipated change in pupil numbers 2024/25 to 2026/27</t>
+  </si>
+  <si>
+    <t>School census Jan 2025 data</t>
+  </si>
+  <si>
+    <t>Local authority data provided through the  School Capacity (SCAP) Collection 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Number of pupils in roll in January 2025, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. 							</t>
+  </si>
+  <si>
+    <t>1. This is the local authority's forecast of pupil numbers for the academic year 2026/27 as provided in SCAP 2024.
 2. These forecasts cover pupils that local authorities anticipate will attend primary schools (or primary provision in middle or all-through schools i.e. years R-6) and secondary schools (or secondary provision in middle or all-through schools i.e. years 7-11)
 3. These forecasts focus on local authorities expectations about new school places and do not include pupils who are expected to attend independent schools or special/non-mainstream provision.</t>
   </si>
   <si>
-    <t>Forecast accuracy of pupil projections for 2023/24</t>
-  </si>
-  <si>
-    <t>The one year ahead local authority forecast accuracy. It compares actual numbers on roll in 2023/24 with forecasts of pupil numbers for 2023/24 made one year previously (in SCAP 2023)</t>
-  </si>
-  <si>
-    <t>1. Forecasts of academic year 2023/24 pupil numbers made in 2022/23.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. Actual pupil numbers on roll in academic year 2023/24.
+    <t>Forecast accuracy of pupil projections for 2024/25</t>
+  </si>
+  <si>
+    <t>The one year ahead local authority forecast accuracy. It compares actual numbers on roll in 2024/25 with forecasts of pupil numbers for 2024/25 made one year previously (in SCAP 2024)</t>
+  </si>
+  <si>
+    <t>The three year ahead forecast accuracy compares actual pupil numbers on roll with forecasts of pupil numbers for 2024/25 made three years previously (in SCAP 2022) by local authority).</t>
+  </si>
+  <si>
+    <t>1. Forecasts of academic year 2024/25 pupil numbers made in 2023/24.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Actual pupil numbers on roll in academic year 2024/25.
 </t>
   </si>
   <si>
-    <t>Local authority data provided through the School Capacity (SCAP) Collection 2023</t>
-  </si>
-  <si>
-    <t>Pupils in school provided through the January 2024 School Census</t>
-  </si>
-  <si>
-    <t>1. Forecasts, submitted by local authorities for SCAP23 , at planning area level and aggregated to local authority level. Forecasts include pupils expected to be educated in new schools (or expanded schools) funded through Housing Developer Contributions (HDC) and Housing Infrastructure Fund (HIF) agreements.
-&lt;br&gt;2. Actual pupil numbers on roll for academic year 2023/24 are taken from the January school census and aggregated to local authority level. They include pupils in roll, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. &lt;br&gt;3. Forecast accuracy is calculated by  subtracting the years R-6 actual numbers from the years R-6 forecasts to give the absolute inaccuracy. Absolute inaccuracy is then divided by the R-6 actual number to give the relative percentage inaccuracy. The same is done for secondary using years 7-11. 
+    <t xml:space="preserve">1. Forecasts of academic year 2024/25 pupil numbers made in 2021/22.
+</t>
+  </si>
+  <si>
+    <t>2. Actual pupil numbers on roll in academic year 2024/25.</t>
+  </si>
+  <si>
+    <t>Local authority data provided through the School Capacity (SCAP) Collection 2024</t>
+  </si>
+  <si>
+    <t>Pupils in school provided through the January 2025 School Census</t>
+  </si>
+  <si>
+    <t>Local authority data provided through the School Capacity (SCAP) Collection 2022</t>
+  </si>
+  <si>
+    <t>1. Forecasts, submitted by local authorities for SCAP24 , at planning area level and aggregated to local authority level. Forecasts include pupils expected to be educated in new schools (or expanded schools) funded through Housing Developer Contributions (HDC) and Housing Infrastructure Fund (HIF) agreements.
+&lt;br&gt;2. Actual pupil numbers on roll for academic year 2024/25 are taken from the January school census and aggregated to local authority level. They include pupils in roll, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. &lt;br&gt;3. Forecast accuracy is calculated by  subtracting the years R-6 actual numbers from the years R-6 forecasts to give the absolute inaccuracy. Absolute inaccuracy is then divided by the R-6 actual number to give the relative percentage inaccuracy. The same is done for secondary using years 7-11. 
 &lt;br&gt;4.  Scorecard figures may differ to those published in SCAP due to the exclusion of years 12 to 14 in the pupil numbers and forecasts used in the scorecard.</t>
-  </si>
-  <si>
-    <t>The three year ahead forecast accuracy compares actual pupil numbers on roll with forecasts of pupil numbers for 2023/24 made two years previously (in SCAP 2021) by local authority).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Forecasts of academic year 2023/24 pupil numbers made in 2020/21.
-</t>
-  </si>
-  <si>
-    <t>2. Actual pupil numbers on roll in academic year 2023/24.</t>
   </si>
   <si>
     <r>
@@ -365,120 +366,60 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>as part of the SCAP 2021, at planning area level and aggregated to local authority level. Forecasts include pupils expected to be educated in new schools (or expanded schools) funded through HDC and HIF agreements.
-&lt;br&gt;2. Actual pupil numbers on roll for academic year 2023/24 are taken from the January school census and aggregated to local authority level. They include pupils in roll, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. 	&lt;br&gt;3. Forecast accuracy is calculated by subtracting the years R-6 actual numbers from the years R-6 forecasts to give the absolute inaccuracy. Absolute inaccuracy is then divided by the R-6 actual number to give the relative percentage inaccuracy. The same is done for secondary using years 7-11. 
+      <t>as part of the SCAP 2022, at planning area level and aggregated to local authority level. Forecasts include pupils expected to be educated in new schools (or expanded schools) funded through HDC and HIF agreements.
+&lt;br&gt;2. Actual pupil numbers on roll for academic year 2024/25 are taken from the January school census and aggregated to local authority level. They include pupils in roll, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. 	&lt;br&gt;3. Forecast accuracy is calculated by subtracting the years R-6 actual numbers from the years R-6 forecasts to give the absolute inaccuracy. Absolute inaccuracy is then divided by the R-6 actual number to give the relative percentage inaccuracy. The same is done for secondary using years 7-11. 
 &lt;br&gt;4.  Scorecard figures may differ to those published in SCAP due to the exclusion of years 12 to 14 in the pupil numbers and forecasts used in the scorecard.</t>
     </r>
   </si>
   <si>
-    <t>School place offers by preference for September 2024 entry</t>
-  </si>
-  <si>
-    <t>The proportion of applicants who received an offer of a place in one of their top three preference schools for September 2024 on national offer day</t>
-  </si>
-  <si>
-    <t>Published School Applications and Offer data 2024/25 Academic Year</t>
-  </si>
-  <si>
-    <t>Quality of new school places created between academic year 2021/22 and 2022/23, based on Ofsted rating</t>
-  </si>
-  <si>
-    <t>The number of new places created between academic year 2021/22 and academic year 2022/23</t>
-  </si>
-  <si>
-    <t>Capacity of each school in May 2022</t>
-  </si>
-  <si>
-    <t>1. The following school types, identified using Get Information About Schools, have been excluded:
-&lt;br&gt;- former independent schools which have not had an inspection since opening;
-&lt;br&gt;- sponsored academies which have not had an Ofsted inspection since opening as an academy.
-&lt;br&gt;- schools that have amalgamated and have not been inspected since amalgamation.
-&lt;br&gt;2.The capacity of schools present in May 2023 is compared with May 2022 capacity.
-&lt;br&gt;3. New places are identified as an increase in school capacity of 30 places or more between May 2022 and May 2023 at each school. For mergers and academy conversions where 2022 capacity is not available, the capacities of the ‘parent’ schools in 2022 have been used.
-&lt;br&gt;4. Schools where fewer than 30 places have been created between May 2022 and May 2023 have all of their capacity counted as existing places.
-&lt;br&gt;5. Existing places are the number of places present in May 2023 after subtracting the new places since May 2022 (if 30 or more) from the May 2022 capacity.
-&lt;br&gt;6. Primary places are based on primary capacity and secondary places are based on secondary capacity reported in May 2022 or 2023. 
-&lt;br&gt;7. New places in schools which had not had an Ofsted judgment or key stage 2 or 4 result by August 2023 have been excluded from the relevant version of the measure. These places are included in the figure beneath the chart.
-&lt;br&gt;8. Because any decreases in capacity are not factored, the number of places added for use in the quality measure may not be the same as the number of places added in the quantity measure.
-&lt;br&gt;9. From June 2019 the Ofsted grades of academy predecessor schools were factored into their data, even though it may have been some time since those schools converted and/or were inspected. 
-&lt;br&gt;10. The quality measures represent the window in time when places were added and this is not necessarily the same quality outcome as when the decision to add places was taken.</t>
-  </si>
-  <si>
-    <t>Capacity for each school in May 2023</t>
-  </si>
-  <si>
-    <t>Local authority data, provided through School Capacity collection 2023</t>
-  </si>
-  <si>
-    <t>Percentage of new places created in good and outstanding schools between academic year 2021/22 and academic year 2022/23.</t>
-  </si>
-  <si>
-    <t>Quality of new school places created between academic year 2021/22 and 2022/23, based on key stage 2 progress measures</t>
-  </si>
-  <si>
-    <t>Performance tables</t>
-  </si>
-  <si>
-    <t>Key stage 2 progress measures</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Each school has been matched with the key stage 2 progress measure for reading and maths, for academic year ending July 2023 (published December 2023).
-2. This measure judges schools’ performance as 'well above average', 'above average', 'average', 'below average' or 'well below average'.
-3. The calculation counts the number of new school places that have been created in schools of each category; and the number of existing school places in each category.
-4. Middle schools may not have a key stage 2 measure and if they do, due to the age range of pupils at middle schools, pupils will have only attended a middle school for a short time before they take their key stage 2 tests and will still have a number of years left at the school. This should be taken into account when comparing their results to schools which start educating their pupils from the beginning of key stage 1.  New schools may not have a key stage 2 measure until the first cohort of pupils reaches year 6.
-5. For further information on key stage 2 progress measures please use the following url: https://www.gov.uk/government/collections/school-performance-tables-about-the-data </t>
-  </si>
-  <si>
-    <t>The quality of school places created between academic year 2021/22 and academic year 2022/23, and the quality of existing school places. Based on key stage 2 progress measures</t>
-  </si>
-  <si>
-    <t>The quality of school places created between academic year 2021/22 and academic year 2022/23, and the quality of existing school places. Based on key stage 4 progress 8 measure</t>
-  </si>
-  <si>
-    <t>Quality of new school places created between academic year 2021/22 and 2022/23, based on key stage 4 progress 8 measure</t>
-  </si>
-  <si>
-    <t>Key stage 4 progress 8 measure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LA Rank- key stage 2 measures
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LA Rank- key stage 4 progress 8 measure
-</t>
-  </si>
-  <si>
-    <t>Ranks local authorities on their proportion of new school places of new school places created in well above- and above-average schools</t>
-  </si>
-  <si>
-    <t>1. Ranking of proportions of new places created in 'well above average' and 'above average' schools for each local authority, amongst all local authorities with new places. Local authorities with the same proportion are given an equal ranking. Ranking is only applied to local authorities where new places have been created.
-2. The higher the rank the higher the proportion of new school places in well above and above average schools compared to other local authorities.</t>
-  </si>
-  <si>
-    <t>Percentage of new places created in well above and above-average schools between academic year 2021/22 and academic year 2022/23.</t>
-  </si>
-  <si>
-    <t>1. Ranking of proportions of new places created in 'well above average' and 'above average' schools for each local authority, amongst all local authorities with new places. Local authorities with the same proportion are given an equal ranking. Ranking is only applied to local authorities where new places have been created. 
-2. The higher the rank the higher the proportion of new school places in well above and above average schools compared to other local authorities.</t>
-  </si>
-  <si>
-    <t>Number of new places planned for delivery between May 2023 and September 2025;
-&lt;br&gt;This contains: 
-&lt;br&gt;1) local authority firm plans for new permanent additional places , new temporary bulge places and the removal of places,
-&lt;br&gt;2) capacity changes through the Condition Improvement Fund (CIF), School Rebuilding Programme (SRP), Selective Schools Expansion Fund (SSEF), and Voluntary Aided Schools Fund (VA)
-&lt;br&gt;3) places from free schools opened in September 2023 and planned to open in September 2024
-&lt;br&gt;4) reduction in places from free school and academy closures.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DfE internal model. Additional places needed are published in the school place planning published underlying data. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">LA Rank- Ofsted
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Each school has been matched with the key stage 4 progress 8 measure across 8 key subjects, for academic year ending July 2023 (published February 2024).
+    <t>School place offers by preference for September 2025 entry</t>
+  </si>
+  <si>
+    <t>The proportion of applicants who received an offer of a place in one of their top three preference schools for September 2025 on national offer day</t>
+  </si>
+  <si>
+    <t>Published School Applications and Offer data 2025/26 Academic Year</t>
+  </si>
+  <si>
+    <t>Quality of new school places created between academic year 2022/23 and 2023/24, based on Ofsted rating</t>
+  </si>
+  <si>
+    <t>The number of new places created between academic year 2022/23 and academic year 2023/24</t>
+  </si>
+  <si>
+    <t>Capacity of each school in May 2023</t>
+  </si>
+  <si>
+    <t>Capacity for each school in May 2024</t>
+  </si>
+  <si>
+    <t>Local authority data, provided through School Capacity collection 2024</t>
+  </si>
+  <si>
+    <t>Quality of school places created between academic year 2022/23 and academic year 2023/24, based on Ofsted rating. The quality of existing school places (places in 2023/24 which were also present in 2022/23) is shown for context.</t>
+  </si>
+  <si>
+    <t>1. Each school has been matched with the Ofsted judgement of 'Overall effectiveness: how good is the school." as at 31 August 2024 (published November 2024).
+&lt;br&gt;2. There are four Ofsted categories: 'Outstanding', 'Good', 'Requires improvement' and 'Inadequate'.
+&lt;br&gt;3. The calculation counts the number of existing and new places that have been created in schools of each category. &lt;br&gt;4. Note that many schools will have been inspected some time before August 2024, and some will have been inspected since this date. &lt;br&gt;5. There are school places with no rating, as the school has yet to be inspected so do not have an Ofsted judgement.</t>
+  </si>
+  <si>
+    <t>Percentage of new places created in good and outstanding schools between academic year 2022/23 and academic year 2023/24.</t>
+  </si>
+  <si>
+    <t>The quality of school places created between academic year 2022/23 and academic year 2023/24, and the quality of existing school places. Based on key stage 2 progress measures</t>
+  </si>
+  <si>
+    <t>Quality of new school places created between academic year 2022/23 and 2023/24, based on key stage 2 progress measures</t>
+  </si>
+  <si>
+    <t>The quality of school places created between academic year 2022/23 and academic year 2023/24, and the quality of existing school places. Based on key stage 4 progress 8 measure</t>
+  </si>
+  <si>
+    <t>Quality of new school places created between academic year 2022/23 and 2023/24, based on key stage 4 progress 8 measure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Each school has been matched with the key stage 4 progress 8 measure across 8 key subjects, for academic year ending July 2024 (published February 2025).
 2. This measure judges schools’ performance as 'well above average', 'above average', 'average', 'below average' or 'well below average'.
 3. The calculation counts the number of new school places that have been created in schools of each category; and the number of existing school places in each category.
 4. Note that middle schools will not have a key stage 4 measure, and that new schools may not have a key stage 4 measure until the first cohort of pupils reaches year 11.
@@ -487,44 +428,90 @@
 </t>
   </si>
   <si>
-    <t>Percentage of  new school places in well above and above-average schools- key stage 2 measures</t>
-  </si>
-  <si>
-    <t>Percentage of  new school places in well above and above-average schools- key stage 4 progress 8 measure</t>
-  </si>
-  <si>
-    <t>Quality of school places created between academic year 2021/22 and academic year 2022/23, based on Ofsted rating. The quality of existing school places (places in 2022/23 which were also present in 2021/22) is shown for context.</t>
-  </si>
-  <si>
-    <t>1. Each school has been matched with the Ofsted judgement of 'Overall effectiveness: how good is the school." as at 31 August 2023 (published November 2023).
-&lt;br&gt;2. There are four Ofsted categories: 'Outstanding', 'Good', 'Requires improvement' and 'Inadequate'.
-&lt;br&gt;3. The calculation counts the number of existing and new places that have been created in schools of each category. &lt;br&gt;4. Note that many schools will have been inspected some time before August 2023, and some will have been inspected since this date. &lt;br&gt;5. There are school places with no rating, as the school has yet to be inspected so do not have an Ofsted judgement.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The national average has been adjusted to the relevant region for each local authority, using the Building Cost Information Service (BCIS) March 2024 published regional location factors. The England national average has been multiplied by the relevant regional location factor:  East Midlands: 1.03, East of England 0.99, Inner London: 1.29, North East: 0.91, North West: 1, Outer London: 1.21, South East: 1.13, South West: 1.01, West Midlands: 0.96, Yorkshire &amp; the Humber: 0.91. </t>
+    <t>Percentage of new places created in well above and above-average schools between academic year 2022/23 and academic year 2023/24.</t>
+  </si>
+  <si>
+    <t>Local authority data provided through the School Capacity (SCAP) Survey 2024.</t>
+  </si>
+  <si>
+    <t>The actual percentage change in pupil numbers between 2009/10, 2014/15 (for secondary), 2018/19 (for primary) and 2024/25; the anticipated percentage change in pupil numbers in primary or secondary state-funded mainstream provision between the 2024/25 and 2026/27 academic years.</t>
+  </si>
+  <si>
+    <t>School census Jan 2015 data</t>
+  </si>
+  <si>
+    <t>School census Jan 2019 data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Number of pupils in roll in January 2015, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Number of pupils in roll in January 2019, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. </t>
+  </si>
+  <si>
+    <t>5. Total number of planned places (sum of 1, 2, 3, and 4 above)</t>
+  </si>
+  <si>
+    <t>2. Pupil Numbers for the 2014/15 academic year taken from the pupil census in January 2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Pupil Numbers for the 2018/19 academic year taken from the pupil census in January 2019
+</t>
+  </si>
+  <si>
+    <t>4. Pupil Numbers for the 2024/25 academic year taken from the pupil census in January 2025</t>
+  </si>
+  <si>
+    <t>5. Forecast pupil numbers for the 2026/27 academic year</t>
+  </si>
+  <si>
+    <t>1.This relates to the academic year 2026/27 and is the difference between local authority pupil forecasts and future capacity, taking account of planned future additions and places to remove.
+     places needed = forecast demand - (existing capacity + additional capacity - places to remove).  
+For further information on the methodology used, see the School Place Planning 2024: technical note found on the School Capacity 24 publication on Explore Education Statistics.
+&lt;br&gt;2. Where demand is greater than capacity a need for additional places results; where capacity is greater than demand spare places result. 
+&lt;br&gt;3. Local authority pupil forecasts for 2026/27 are collected through SCAP 2024&lt;br&gt;4. Additional capacity as at 2026/27 includes places that the local authority plans to add or remove between May 2024 and before the start of the 2026/27 academic year and places from programmes centrally funded by the department, as described above. 
+&lt;br&gt;5. The comparison of demand and capacity takes place for each national curriculum year group within each planning area to estimate places needed in each. The estimates in the scorecard do not allow for spare capacity in one year group or planning area to be off-set against need in another, or vice-versa. This avoids the risk of spare places in one or more planning areas masking areas of need for additional places in planning areas elsewhere in the local authority. For further information see the School Place Planning Tables 2024: technical note.
+&lt;br&gt;6. The estimated need for additional places and estimated spare places is calculated at planning area level and then aggregated to local authority level. It is common for a local authority to have both a need for additional places and spare places, reflecting pockets of localised need for places or pockets of localised spare places.
+&lt;br&gt;7. Estimates for need are rounded to the nearest 10.
+&lt;br&gt;8. Estimates for spare places are presented as a percentage of total future capacity.</t>
+  </si>
+  <si>
+    <t>1. Number of new school places created
+2. Quality of new places created as judged by key stage 2 progress measures</t>
+  </si>
+  <si>
+    <t>1. Number of new school places created
+2. Quality of new places created as judged by key stage 4 progress 8 measure</t>
+  </si>
+  <si>
+    <t>1. The following school types, identified using Get Information About Schools, have been excluded:
+&lt;br&gt;- former independent schools which have not had an inspection since opening;
+&lt;br&gt;- sponsored academies which have not had an Ofsted inspection since opening as an academy.
+&lt;br&gt;- schools that have amalgamated and have not been inspected since amalgamation.
+&lt;br&gt;- schools which have split and have not been inspected since the split.
+&lt;br&gt;2.The capacity of schools present in May 2024 is compared with May 2023 capacity.
+&lt;br&gt;3. New places are identified as an increase in school capacity of 30 places or more between May 2023 and May 2024 at each school. For mergers and academy conversions where 2023 capacity is not available, the capacities of the ‘parent’ schools in 2023 have been used.
+&lt;br&gt;4. Schools where fewer than 30 places have been created between May 2023 and May 2024 have all of their capacity counted as existing places.
+&lt;br&gt;5. Existing places are the number of places present in May 2024 after subtracting the new places since May 2023 (if 30 or more) from the May 2023 capacity.
+&lt;br&gt;6. Primary places are based on primary capacity and secondary places are based on secondary capacity reported in May 2023 or 2024. 
+&lt;br&gt;7. New places in schools which had not had an Ofsted judgment or key stage 2 or 4 result by August 2024 have been excluded from the relevant version of the measure. These places are included in the figure beneath the chart.
+&lt;br&gt;8. Because any decreases in capacity are not factored, the number of places added for use in the quality measure may not be the same as the number of places added in the quantity measure.
+&lt;br&gt;9. From June 2019 the Ofsted grades of academy predecessor schools were factored into their data, even though it may have been some time since those schools converted and/or were inspected. 
+&lt;br&gt;10. The quality measures represent the window in time when places were added and this is not necessarily the same quality outcome as when the decision to add places was taken.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Each school has been matched with the key stage 2 progress measure for reading and maths, for academic year ending July 2023 (published December 2023). It was not be possible to calculate KS1-KS2 progress measures for the 2023/24 academic year, because there is no relevant KS1 data required to calculate KS1-KS2 progress measures for these cohorts, as primary tests and assessments were cancelled in academic years 2019/20 and 2020/21 due to COVID-19 disruption.
+2. This measure judges schools’ performance as 'well above average', 'above average', 'average', 'below average' or 'well below average'.
+3. The calculation counts the number of new school places that have been created in schools of each category; and the number of existing school places in each category.
+4. Middle schools may not have a key stage 2 measure and if they do, due to the age range of pupils at middle schools, pupils will have only attended a middle school for a short time before they take their key stage 2 tests and will still have a number of years left at the school. This should be taken into account when comparing their results to schools which start educating their pupils from the beginning of key stage 1.  New schools may not have a key stage 2 measure until the first cohort of pupils reaches year 6.
+5. For further information on key stage 2 progress measures please use the following url: https://www.gov.uk/government/collections/school-performance-tables-about-the-data </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The national average has been adjusted to the relevant region for each local authority, using the Building Cost Information Service (BCIS) March 2023 published regional location factors. The England national average has been multiplied by the relevant regional location factor:  East Midlands: 1.03, East of England 0.99, Inner London: 1.29, North East: 0.91, North West: 1, Outer London: 1.21, South East: 1.13, South West: 1.01, West Midlands: 0.96, Yorkshire &amp; the Humber: 0.91. </t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">1. The cost data used in the scorecard is the 2018 Capital Spend data as used in the 2018, 2019 and 2021 Scorecards. For the 2023 Scorecard, this data has been adjusted for inflation (rebased to 1st Quarter 2024 prices). National averages adjusted for 2023 regional location factors are shown. </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">You can use this data to establish developer contributions per school place, by adjusting for further inflation if needed </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(see examples below).
+      <t xml:space="preserve">1. The cost data used in the scorecard is the 2018 Capital Spend data as used in the 2018, 2019 and 2021 Scorecards. For the 2024 Scorecard, this data has been adjusted for inflation (rebased to 1st Quarter 2025 prices). National averages adjusted for 2024 regional location factors are shown. You can use this data to establish developer contributions per school place, by adjusting for further inflation if needed (see examples below).
 &lt;br&gt;2. Projects which do not create additional mainstream places or where the project's additional place funding is zero are removed.
 &lt;br&gt;3. Projects were identified as primary  or secondary phase based on additional mainstream place year group breakdown. Where a project created places across both phases, it was assigned a phase corresponding to the phase of the school it affected (i.e. if its school was middle-deemed primary - the project was assigned to primary).
 &lt;br&gt;4. Average cost per place figures for all-through, middle-deemed primary and middle-deemed secondary schools have not been calculated separately due to low sample sizes for these project types. </t>
@@ -625,9 +612,9 @@
       <t xml:space="preserve"> (e.g. Years 7 &amp; 8).
 &lt;br&gt;5. The average cost does not include costs associated with land acquisition.
 &lt;br&gt;6. The average cost includes costs associated with maintenance and building condition or enhancement works.
-&lt;br&gt;7. The measure does not include places in special schools or units attached to mainstream schools, or new places which were funded through central programmes (including free schools). Where a project creates additional mainstream places and also creates SEN places or re-provides places, an adjustment has been applied to apportion out those costs. 
-&lt;br&gt;8. All costs have been normalised to a common UK average price level using regional location factors published by BCIS, March 2024, 1 is the base weight.
-&lt;br&gt;9. All costs have been adjusted for inflation using the latest BCIS All-In Tender Price of Index (TPI), published March 2024.  Costs have been rebased from the start of construction (or time of place provision if construction start date unavailable) to 1st Quarter (Jan – Mar) 2024 prices using this index (Q1 2024 index value = 390).
+&lt;br&gt;7. The measure does not include places in special schools or units attached to mainstream schools, or new places which were funded through central programmes (including free schools). For projects within the 2018 Capital Spend dataset, a project which creates additional mainstream places and also creates SEN places or re-provides places, has been adjusted to apportion out those costs. For projects within the Capital Spend Survey, apportioning costs is not possible and therefore a project which creates additional mainstream places and also creates SEN places or re-provides places has been exlcuded.
+&lt;br&gt;8. All costs have been normalised to a common UK average price level using regional location factors published by BCIS, March 2023, 1 is the base weight.
+&lt;br&gt;9. All costs have been adjusted for inflation using the latest BCIS All-In Tender Price of Index (TPI), published March 2025.  Costs have been rebased from the start of construction (or time of place provision if construction start date unavailable) to 1st Quarter (Jan – Mar) 2025 prices using this index (Q1 2025 index value = 399).
 10. </t>
     </r>
     <r>
@@ -638,7 +625,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>To adjust the national average to current or future prices, you need to uprate or downrate the prices in this scorecard relative to the change that has happened since Q1 2024</t>
+      <t>To adjust the national average to current or future prices, you need to uprate or downrate the prices in this scorecard relative to the change that has happened since Q1 2025</t>
     </r>
     <r>
       <rPr>
@@ -647,7 +634,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">.  If you have access to the BCIS indices via a subscription to BCIS Online (https://www.rics.org/uk/products/data-products/bcis-construction/bcis-online/) you can use the latest inflation index to re-base (weight to apply = latest index/390).  If not, you can apply a known change to the published cost (e.g. up or down x%).
+      <t xml:space="preserve">.  If you have access to the BCIS indices via a subscription to BCIS Online (https://www.rics.org/uk/products/data-products/bcis-construction/bcis-online/) you can use the latest inflation index to re-base (weight to apply = latest index/399).  If not, you can apply a known change to the published cost (e.g. up or down x%).
 </t>
     </r>
     <r>
@@ -1024,7 +1011,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1048,9 +1035,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1087,92 +1071,101 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1196,10 +1189,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1499,22 +1488,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8372DA64-5E2C-41C1-8CF4-85BC1C2AFF86}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="C11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.73046875" customWidth="1"/>
-    <col min="2" max="2" width="29.59765625" customWidth="1"/>
-    <col min="3" max="3" width="54.265625" customWidth="1"/>
-    <col min="4" max="4" width="28.73046875" customWidth="1"/>
-    <col min="5" max="5" width="87.265625" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" customWidth="1"/>
+    <col min="3" max="3" width="54.28515625" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" customWidth="1"/>
+    <col min="5" max="5" width="87.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1531,12 +1520,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="87" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="46" t="s">
-        <v>34</v>
+      <c r="B2" s="42" t="s">
+        <v>38</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>2</v>
@@ -1544,183 +1533,211 @@
       <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="48" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="87" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E2" s="44" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
-      <c r="B3" s="47"/>
+      <c r="B3" s="43"/>
       <c r="C3" s="6" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="47"/>
-    </row>
-    <row r="4" spans="1:5" ht="138" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E3" s="43"/>
+    </row>
+    <row r="4" spans="1:5" ht="138" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="49" t="s">
-        <v>98</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+        <v>51</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
-      <c r="B5" s="50"/>
+      <c r="B5" s="46"/>
       <c r="C5" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="E5" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
-      <c r="B6" s="50"/>
-      <c r="C6" s="13" t="s">
+      <c r="B6" s="46"/>
+      <c r="C6" s="12" t="s">
         <v>44</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="E6" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="13" t="s">
+      <c r="B7" s="46"/>
+      <c r="C7" s="12" t="s">
         <v>45</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="85.9" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E7" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
-      <c r="B8" s="47"/>
-      <c r="C8" s="13" t="s">
-        <v>31</v>
+      <c r="B8" s="43"/>
+      <c r="C8" s="12" t="s">
+        <v>98</v>
       </c>
       <c r="D8" s="6"/>
-      <c r="E8" s="13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="E8" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="21"/>
+      <c r="D9" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="327.75" x14ac:dyDescent="0.45">
-      <c r="A10" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="21" t="s">
+      <c r="E9" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="375" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="185.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D10" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="14"/>
+        <v>55</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="13"/>
       <c r="D11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="57" x14ac:dyDescent="0.45">
-      <c r="A13" s="8"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="11" t="s">
+      <c r="E11" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="17" t="s">
+    </row>
+    <row r="12" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="B12" s="47" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="51"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="51"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="51"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D15" s="16" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="100.15" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="9"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="31" t="s">
+      <c r="E15" s="20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="52"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" s="31" t="s">
+      <c r="E16" s="27" t="s">
         <v>62</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="B4:B8"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="A12:A16"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <hyperlinks>
@@ -1728,13 +1745,15 @@
     <hyperlink ref="D10" r:id="rId2" display=" 2021/22 school place planning published underlying data. " xr:uid="{093B09C6-85AC-4B03-8BE4-078C82660B4C}"/>
     <hyperlink ref="D2" r:id="rId3" xr:uid="{8150C38D-D188-4C8E-86C3-B5575B8FFEE8}"/>
     <hyperlink ref="D11" r:id="rId4" xr:uid="{84C17436-4B87-48EB-BAE5-31DBACCBDB31}"/>
-    <hyperlink ref="D13" r:id="rId5" display="School census Jan 2023 data" xr:uid="{B4335ED1-45C2-43A8-BAE4-D6C4C7E179D0}"/>
+    <hyperlink ref="D15" r:id="rId5" display="School census Jan 2023 data" xr:uid="{B4335ED1-45C2-43A8-BAE4-D6C4C7E179D0}"/>
     <hyperlink ref="D12" r:id="rId6" xr:uid="{CCB6838D-DD36-44DD-BC08-5E652C942FA3}"/>
     <hyperlink ref="D9" r:id="rId7" display="Local authority data provided through School Capacity (SCAP) Survey 2021" xr:uid="{F7517439-C801-46CD-8DC3-B6DD58F4289A}"/>
-    <hyperlink ref="D14" r:id="rId8" display="Local authority data provided through the  School Capacity (SCAP) Collection 2022" xr:uid="{2257ADC3-56E0-46AA-984A-65A14B6B91D4}"/>
+    <hyperlink ref="D16" r:id="rId8" display="Local authority data provided through the  School Capacity (SCAP) Collection 2022" xr:uid="{2257ADC3-56E0-46AA-984A-65A14B6B91D4}"/>
+    <hyperlink ref="D13" r:id="rId9" xr:uid="{79AE5929-1652-4611-9E48-29269254E396}"/>
+    <hyperlink ref="D14" r:id="rId10" xr:uid="{4D3E4206-3C34-46F2-94BA-63E9C87A86E9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 
@@ -1742,85 +1761,85 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C67D23D-5B13-4F00-9F83-043839CEFFD1}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="55.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="55.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="55.3984375" style="35"/>
+    <col min="1" max="16384" width="55.42578125" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="28" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="33" t="s">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="45" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="300.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="29"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="54"/>
+    </row>
+    <row r="4" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="29"/>
+      <c r="B4" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="38" t="s">
-        <v>67</v>
-      </c>
-      <c r="E2" s="49" t="s">
+      <c r="C4" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="45" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="272.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="36"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="14" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="33"/>
-      <c r="B3" s="52"/>
-      <c r="C3" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" s="52"/>
-    </row>
-    <row r="4" spans="1:5" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="33"/>
-      <c r="B4" s="49" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="13" t="s">
+      <c r="D5" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="D4" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="49" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="40"/>
-      <c r="B5" s="51"/>
-      <c r="C5" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="D5" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5" s="51"/>
+      <c r="E5" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1831,7 +1850,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="Local authority data provided through the School Capacity (SCAP) Collection 2022" xr:uid="{D14A8E59-0240-4725-B7AC-4582058C6B59}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{586F3224-6D8F-4AF9-899D-550CFDC0058F}"/>
+    <hyperlink ref="D4" r:id="rId2" display="Local authority data provided through the School Capacity (SCAP) Collection 2021" xr:uid="{586F3224-6D8F-4AF9-899D-550CFDC0058F}"/>
     <hyperlink ref="D3" r:id="rId3" display="Pupils in school provided through the January 2023 School Census" xr:uid="{17405BAA-EC5B-41A8-9F2F-BBE920A0B9BB}"/>
     <hyperlink ref="D5" r:id="rId4" display="Pupils in school provided through the January 2023 School Census" xr:uid="{54B0E578-7E98-4CE5-8BEB-25623CA0296D}"/>
   </hyperlinks>
@@ -1844,13 +1863,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3163888B-9214-4218-82C5-5CD72F2D39D0}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="48.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="48.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1867,34 +1886,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A2" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="13" t="s">
+    <row r="2" spans="1:5" ht="197.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A3" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" s="13" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="E3" s="13" t="s">
-        <v>17</v>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1908,200 +1927,165 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{172A91E8-EE08-4774-802F-E9F4C78EAB63}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="B7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="37.265625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="37.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="37.265625" style="35"/>
-    <col min="5" max="5" width="77.265625" style="35" customWidth="1"/>
-    <col min="6" max="16384" width="37.265625" style="35"/>
+    <col min="1" max="4" width="37.28515625" style="31"/>
+    <col min="5" max="5" width="77.28515625" style="31" customWidth="1"/>
+    <col min="6" max="16384" width="37.28515625" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="28" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="399" x14ac:dyDescent="0.45">
-      <c r="A2" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="B2" s="12" t="s">
+    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="B2" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="12" t="s">
+      <c r="C2" s="10" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="42"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="13" t="s">
+      <c r="D2" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="38"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="43"/>
-    </row>
-    <row r="4" spans="1:5" ht="128.25" x14ac:dyDescent="0.45">
-      <c r="A4" s="42"/>
-      <c r="B4" s="44" t="s">
+      <c r="E3" s="39"/>
+    </row>
+    <row r="4" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="A4" s="38"/>
+      <c r="B4" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="315" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="240" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="38" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="13" t="s">
+      <c r="D8" s="25"/>
+      <c r="E8" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="57" x14ac:dyDescent="0.45">
-      <c r="A5" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="114" x14ac:dyDescent="0.45">
-      <c r="A6" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="B6" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="199.5" x14ac:dyDescent="0.45">
-      <c r="A7" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="185.25" x14ac:dyDescent="0.45">
-      <c r="A8" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A9" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="13" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A10" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="13" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A11" s="28" t="s">
-        <v>92</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A12" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="B12" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13" t="s">
-        <v>95</v>
+      <c r="D9" s="25"/>
+      <c r="E9" s="12" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{6EE32724-1837-46BD-9FD6-A4EEFD1E0A4A}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{F8935CE3-E46D-430A-A5BC-BAB4A254BDA2}"/>
+    <hyperlink ref="D2" r:id="rId1" display="Local authority data, provided through School Capacity collection 2022" xr:uid="{6EE32724-1837-46BD-9FD6-A4EEFD1E0A4A}"/>
+    <hyperlink ref="D3" r:id="rId2" display="Local authority data, provided through School Capacity collection 2023" xr:uid="{F8935CE3-E46D-430A-A5BC-BAB4A254BDA2}"/>
     <hyperlink ref="D4" r:id="rId3" xr:uid="{2FB89BF4-390E-4CD5-92FB-FD0FF31F028D}"/>
-    <hyperlink ref="D7" r:id="rId4" xr:uid="{4534F643-19C4-4655-8095-8044AC4B7902}"/>
-    <hyperlink ref="D8" r:id="rId5" xr:uid="{4889CA3C-1157-412C-ACB1-EE5DA00A90DF}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{4534F643-19C4-4655-8095-8044AC4B7902}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{4889CA3C-1157-412C-ACB1-EE5DA00A90DF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2115,89 +2099,89 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="57.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="57.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="57.59765625" style="35"/>
+    <col min="1" max="16384" width="57.5703125" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="28" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="409.6" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="45"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="19"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B4" s="18"/>
-      <c r="C4" s="20"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B5" s="18"/>
-      <c r="C5" s="20"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B6" s="18"/>
-      <c r="C6" s="20"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B7" s="18"/>
-      <c r="C7" s="20"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B8" s="18"/>
-      <c r="C8" s="20"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B9" s="18"/>
-      <c r="C9" s="20"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B10" s="18"/>
-      <c r="C10" s="20"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B11" s="18"/>
-      <c r="C11" s="20"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B12" s="18"/>
-      <c r="C12" s="20"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B13" s="18"/>
-      <c r="C13" s="20"/>
+    <row r="2" spans="1:5" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="41"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="17"/>
+      <c r="C4" s="19"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="17"/>
+      <c r="C5" s="19"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="17"/>
+      <c r="C6" s="19"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="17"/>
+      <c r="C7" s="19"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="17"/>
+      <c r="C8" s="19"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="17"/>
+      <c r="C9" s="19"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="17"/>
+      <c r="C10" s="19"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="17"/>
+      <c r="C11" s="19"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="17"/>
+      <c r="C12" s="19"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="17"/>
+      <c r="C13" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2206,51 +2190,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
-      <Value>5</Value>
-      <Value>25</Value>
-      <Value>1</Value>
-      <Value>4</Value>
-    </TaxCatchAll>
-    <p6919dbb65844893b164c5f63a6f0eeb xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">DfE</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">a484111e-5b24-4ad9-9778-c536c8c88985</TermId>
-        </TermInfo>
-      </Terms>
-    </p6919dbb65844893b164c5f63a6f0eeb>
-    <c02f73938b5741d4934b358b31a1b80f xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Official</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">0884c477-2e62-47ea-b19c-5af6e91124c5</TermId>
-        </TermInfo>
-      </Terms>
-    </c02f73938b5741d4934b358b31a1b80f>
-    <f6ec388a6d534bab86a259abd1bfa088 xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">DfE</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">cc08a6d4-dfde-4d0f-bd85-069ebcef80d5</TermId>
-        </TermInfo>
-      </Terms>
-    </f6ec388a6d534bab86a259abd1bfa088>
-    <i98b064926ea4fbe8f5b88c394ff652b xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </i98b064926ea4fbe8f5b88c394ff652b>
-    <_dlc_DocIdUrl xmlns="2a6436df-3f7a-48ac-8ea6-44b411e24bbc">
-      <Url>https://educationgovuk.sharepoint.com/sites/efappp/_layouts/15/DocIdRedir.aspx?ID=FKMV6N5X2MYP-1953928680-76369</Url>
-      <Description>FKMV6N5X2MYP-1953928680-76369</Description>
-    </_dlc_DocIdUrl>
-    <_dlc_DocId xmlns="2a6436df-3f7a-48ac-8ea6-44b411e24bbc">FKMV6N5X2MYP-1953928680-76369</_dlc_DocId>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Official Document" ma:contentTypeID="0x010100545E941595ED5448BA61900FDDAFF31300C0D9F77D091A79449828113EF8250EF5" ma:contentTypeVersion="9" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="3acf8af8f3f036fb6d934619e757bc96">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8c566321-f672-4e06-a901-b5e72b4c4357" xmlns:ns3="2a6436df-3f7a-48ac-8ea6-44b411e24bbc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="926947be84ee9a0228ce6a037c6848ba" ns2:_="" ns3:_="">
     <xsd:import namespace="8c566321-f672-4e06-a901-b5e72b4c4357"/>
@@ -2456,9 +2395,58 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
+      <Value>5</Value>
+      <Value>25</Value>
+      <Value>1</Value>
+      <Value>4</Value>
+    </TaxCatchAll>
+    <p6919dbb65844893b164c5f63a6f0eeb xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">DfE</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">a484111e-5b24-4ad9-9778-c536c8c88985</TermId>
+        </TermInfo>
+      </Terms>
+    </p6919dbb65844893b164c5f63a6f0eeb>
+    <c02f73938b5741d4934b358b31a1b80f xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Official</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">0884c477-2e62-47ea-b19c-5af6e91124c5</TermId>
+        </TermInfo>
+      </Terms>
+    </c02f73938b5741d4934b358b31a1b80f>
+    <f6ec388a6d534bab86a259abd1bfa088 xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">DfE</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">cc08a6d4-dfde-4d0f-bd85-069ebcef80d5</TermId>
+        </TermInfo>
+      </Terms>
+    </f6ec388a6d534bab86a259abd1bfa088>
+    <i98b064926ea4fbe8f5b88c394ff652b xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </i98b064926ea4fbe8f5b88c394ff652b>
+    <_dlc_DocIdUrl xmlns="2a6436df-3f7a-48ac-8ea6-44b411e24bbc">
+      <Url>https://educationgovuk.sharepoint.com/sites/efappp/_layouts/15/DocIdRedir.aspx?ID=FKMV6N5X2MYP-1953928680-76369</Url>
+      <Description>FKMV6N5X2MYP-1953928680-76369</Description>
+    </_dlc_DocIdUrl>
+    <_dlc_DocId xmlns="2a6436df-3f7a-48ac-8ea6-44b411e24bbc">FKMV6N5X2MYP-1953928680-76369</_dlc_DocId>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="ec07c698-60f5-424f-b9af-f4c59398b511" ContentTypeId="0x010100545E941595ED5448BA61900FDDAFF313" PreviousValue="false"/>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2513,31 +2501,10 @@
 
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="ec07c698-60f5-424f-b9af-f4c59398b511" ContentTypeId="0x010100545E941595ED5448BA61900FDDAFF313" PreviousValue="false"/>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{334E8BC2-6B82-4EDA-BE50-EFE4767E8CD2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="8c566321-f672-4e06-a901-b5e72b4c4357"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2a6436df-3f7a-48ac-8ea6-44b411e24bbc"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1E94FF3-D2F7-4169-BE5C-5ED202BAA024}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2556,10 +2523,27 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{334E8BC2-6B82-4EDA-BE50-EFE4767E8CD2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8c566321-f672-4e06-a901-b5e72b4c4357"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2a6436df-3f7a-48ac-8ea6-44b411e24bbc"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D00F0DC4-2D9F-43FC-8616-EC131ED26B7D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{035EEA42-582A-4724-B162-C22729062C2B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2573,9 +2557,9 @@
 </file>
 
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{035EEA42-582A-4724-B162-C22729062C2B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D00F0DC4-2D9F-43FC-8616-EC131ED26B7D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adding 2023 data to 2024 scorecard
</commit_message>
<xml_diff>
--- a/data/tech_guidance.xlsx
+++ b/data/tech_guidance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/robert_miller_education_gov_uk/Documents/Documents/R/la-school-places-scorecard-internal/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\shenetapp01\Pupil Place Planning\Scorecards\Scorecards 2024\Combined years\technical guidance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="8_{88D981E4-01D0-41D1-BFE9-9F41107BE635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{364AACDB-AEE9-4581-B73A-D53239F4F61E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E79E806B-0C3D-4EA2-98AE-858B85EF11E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{9CCC1F63-2262-45DD-B4CA-7C937E5C8E7F}"/>
+    <workbookView xWindow="-38520" yWindow="-5355" windowWidth="38640" windowHeight="21120" xr2:uid="{9CCC1F63-2262-45DD-B4CA-7C937E5C8E7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Quantity" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="183">
   <si>
     <t>Notes</t>
   </si>
@@ -145,6 +145,9 @@
     <t>Places created since 2009/10</t>
   </si>
   <si>
+    <t>Local authority data provided through the School Capacity (SCAP) Collection 2021</t>
+  </si>
+  <si>
     <t>School census Jan 2010 data</t>
   </si>
   <si>
@@ -155,6 +158,13 @@
     <t>Percentage of new places created in good and outstanding schools</t>
   </si>
   <si>
+    <t>Ranks local authorities on their proportion of new school places which are in good and outstanding schools</t>
+  </si>
+  <si>
+    <t>1. Ranking of proportions of new places created in 'good' or 'outstanding' schools for each local authority, amongst all local authorities with new places. Local authorities with the same proportion are given an equal ranking. Ranking is only applied to local authorities where new places have been created.
+&lt;br&gt;2. The higher the rank the higher the proportion of new school places in good and outstanding schools compared to other local authorities. &lt;br&gt;3. Ranks can be tied and there will many local authorities with a rank of 1 due to 100% of new places in good and outstanding schools.</t>
+  </si>
+  <si>
     <t xml:space="preserve">The national average cost per place of permanent expansion, temporary expansion and new school projects in England. </t>
   </si>
   <si>
@@ -168,6 +178,18 @@
     <t>2. Capacity changes through the CIF, SRP, SSEF, VA.</t>
   </si>
   <si>
+    <t>School place offers by preference for September 2023 entry</t>
+  </si>
+  <si>
+    <t>The proportion of applicants who received an offer of a place in one of their top three preference schools for September 2023 on national offer day</t>
+  </si>
+  <si>
+    <t>Published School Applications and Offer data 2023/24 Academic Year</t>
+  </si>
+  <si>
+    <t>Local authority data, provided through School Capacity collection 2022</t>
+  </si>
+  <si>
     <t>Unfilled places as a percentage of total places</t>
   </si>
   <si>
@@ -175,12 +197,180 @@
 </t>
   </si>
   <si>
+    <t>5. Total number of planned places (sum of 1, 2, 3, 4 and 5 above)</t>
+  </si>
+  <si>
     <t xml:space="preserve">1. Number of pupils in roll in January 2010, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. </t>
   </si>
   <si>
     <t>1. This relates to the difference between number of pupils on roll and capacity, in schools where the number on roll is lower than a school's reported capacity. &lt;br&gt;2. Calculated at school level and aggregated to local authority level.</t>
   </si>
   <si>
+    <t>Total places created between May 2010 and May 2023</t>
+  </si>
+  <si>
+    <t>2.Capacity at May 2023</t>
+  </si>
+  <si>
+    <t>1. The number of places that have been created since May 2010 in each local authority is taken as the difference between capacity as reported by local authorities, via SCAP, at May 2010 and May 2023.
+&lt;br&gt;2. The measure includes all primary and middle deemed primary school capacity in the primary phase, and all secondary, middle deemed secondary and all-through school capacity in the secondary phase.
+&lt;br&gt;3. The measure reports net increase in places only, if phase capacity in a local authority has reduced between May 2010 and May 2023, this is recorded as zero places created. Therefore the sum of the local authority-level figures will not equal the overall increase in places at national level.</t>
+  </si>
+  <si>
+    <t>Places planned to 2025/26</t>
+  </si>
+  <si>
+    <t>1. Local authority plans for places to be created or removed between May 2023 and before the start of the 2025/26 academic year.</t>
+  </si>
+  <si>
+    <t>Local authority data provided through the School Capacity (SCAP) Survey 2023.</t>
+  </si>
+  <si>
+    <t>Local authority data provided through School Capacity (SCAP) Survey 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Local authority data about new permanent additional places, new temporary bulge places (to accommodate large cohorts as they move through the school) and permanent places to remove  2023/24, 2024/25  and 2025/26 is aggregated to local authority level.
+&lt;br&gt;2. The data was provided by local authorities in May 2023, and only includes projects they were confident would proceed. Local authorities were asked to include the total places of any new provision, even if spaces would fill gradually. 
+&lt;br&gt;3. Local authorities were asked not to include places created through free schools unless they were providing the funding for additional places themselves. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Changes to school capacity (both increases and decreases) as a consequence of works delivered through the CIF, SRP, SSEF, VA between 2023/24 and 2025/26 inclusive, aggregated to local authority level. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. The calculation mirrors the approach taken for basic need funding allocations published in March 2024. It includes mainstream primary and secondary free schools which opened in September 2023 and those with a high degree of certainty of opening in September 2024, and counts the total number of places which will be in use by September 2025.
+&lt;br&gt;2. The data does not include free schools which opened before September 2023, as they will already be included in SCAP23 and are therefore existing places. It does not include free schools which are planned to open in the academic year 2025/26 and beyond. </t>
+  </si>
+  <si>
+    <t>3. Places from free schools opened in September 2023 and due to be opened in September 2024.</t>
+  </si>
+  <si>
+    <t>4. Reduction in places from free school and academy closures between May 2023 and January 2024 or identified/confirmed to close before August 2024.</t>
+  </si>
+  <si>
+    <t>1. Where an academy or free school closed after 1 May 2023 its capacity, as reported in the School Capacity data, is now no longer available. Their capacity has therefore been removed from the planned delivery total.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. This measure reports planned increases in capacity only. If there is a total net planned reduction in capacity (e.g. due to a free school closure), this is shown as zero places planned. Therefore the sum of local authority-level figures will not equal the national planned places figure.
+&lt;br&gt;2. Most local authorities will have further developed their plans since this data was reported in Summer 2023, and so although it allows for comparisons between local authorities, the figure is likely to be an understatement of the current position. </t>
+  </si>
+  <si>
+    <t>Unfilled places in 2022/23</t>
+  </si>
+  <si>
+    <t>Additional places needed in 2025/26; spare places in 2025/26</t>
+  </si>
+  <si>
+    <t>Estimated number of additional places needed to meet demand in 2025/26; estimated percentage of spare places in 2025/26.</t>
+  </si>
+  <si>
+    <t>1.This relates to the academic year 2025/26 and is the difference between local authority pupil forecasts and future capacity, taking account of planned future additions and places to remove.
+     places needed = forecast demand - (existing capacity + additional capacity - places to remove).  
+For further information on the methodology used, see the School Place Planning 2023: technical note found on the School Capacity 23 publication on Explore Education Statistics.
+&lt;br&gt;2. Where demand is greater than capacity a need for additional places results; where capacity is greater than demand spare places result. 
+&lt;br&gt;3. Local authority pupil forecasts for 2025/26 are collected through SCAP 2023&lt;br&gt;4. Additional capacity as at 2025/26 includes places that the local authority plans to add or remove between May 2023 and before the start of the 2025/26 academic year and places from programmes centrally funded by the department, as described above. 
+&lt;br&gt;5. The comparison of demand and capacity takes place for each national curriculum year group within each planning area to estimate places needed in each. The estimates in the scorecard do not allow for spare capacity in one year group or planning area to be off-set against need in another, or vice-versa. This avoids the risk of spare places in one or more planning areas masking areas of need for additional places in planning areas elsewhere in the local authority. For further information see the School Place Planning Tables 2023: technical note.
+&lt;br&gt;6. The estimated need for additional places and estimated spare places is calculated at planning area level and then aggregated to local authority level. It is common for a local authority to have both a need for additional places and spare places, reflecting pockets of localised need for places or pockets of localised spare places.
+&lt;br&gt;7. Estimates for need are rounded to the nearest 10.
+&lt;br&gt;8. Estimates for spare places are presented as a percentage of total future capacity.</t>
+  </si>
+  <si>
+    <t>Total basic need funding 2011 to 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total amount of basic need capital funding allocated to each local authority to support them to create new mainstream primary and secondary places from 2011 to 2025. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. This refers to the amount of basic need capital funding that the Department for Education (DfE) has allocated to each local authority to create new places from the 2011-12 financial year to the 2024-25 financial year. Basic Need funding for the 2024-25 financial year is intended to support the creation of mainstream places for pupils aged 5 to 16 for the 2025/26 academic year. &lt;br&gt;2. The figure includes formula-based funding allocations and funding provided through the Targeted Basic Need Programme. Basic Need formula-based funding allocations cover the whole period and are not ring-fenced (although they can only be used for capital purposes).  Targeted Basic Need funding was provided between 2013 and 2015 and had to be spent by agreed deadlines and on specific projects. Both types of allocations are published here. &lt;br&gt;3. The figure only includes funding allocated to local authorities and does not include centrally-funded capital programmes such as the free schools programme. &lt;br&gt;4. The England total will not match the sum of allocations for all local authorities in the scorecard because the England total includes allocations to predecessor local authorities.
+</t>
+  </si>
+  <si>
+    <t>The actual percentage change in pupil numbers between 2009/10 and 2023/24; the anticipated percentage change in pupil numbers in primary or secondary state-funded mainstream provision between the 2023/24 and 2025/26 academic years.</t>
+  </si>
+  <si>
+    <t>Change in pupil numbers
+2009/10 to 2023/24; Anticipated change in pupil numbers 2023/24 to 2025/26</t>
+  </si>
+  <si>
+    <t>2. Pupil Numbers for the 2023/24 academic year taken from the pupil census in January 2024</t>
+  </si>
+  <si>
+    <t>School census Jan 2024 data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Number of pupils in roll in January 2024, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. 							</t>
+  </si>
+  <si>
+    <t>2. Forecast pupil numbers for the 2025/26 academic year</t>
+  </si>
+  <si>
+    <t>Local authority data provided through the  School Capacity (SCAP) Collection 2023</t>
+  </si>
+  <si>
+    <t>1. This is the local authority's forecast of pupil numbers for the academic year 2025/26 as provided in SCAP 2023.
+2. These forecasts cover pupils that local authorities anticipate will attend primary schools (or primary provision in middle or all-through schools i.e. years R-6) and secondary schools (or secondary provision in middle or all-through schools i.e. years 7-11)
+3. These forecasts focus on local authorities expectations about new school places and do not include pupils who are expected to attend independent schools or special/non-mainstream provision.</t>
+  </si>
+  <si>
+    <t>Forecast accuracy of pupil projections for 2023/24</t>
+  </si>
+  <si>
+    <t>The one year ahead local authority forecast accuracy. It compares actual numbers on roll in 2023/24 with forecasts of pupil numbers for 2023/24 made one year previously (in SCAP 2023)</t>
+  </si>
+  <si>
+    <t>1. Forecasts of academic year 2023/24 pupil numbers made in 2022/23.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Actual pupil numbers on roll in academic year 2023/24.
+</t>
+  </si>
+  <si>
+    <t>Local authority data provided through the School Capacity (SCAP) Collection 2023</t>
+  </si>
+  <si>
+    <t>Pupils in school provided through the January 2024 School Census</t>
+  </si>
+  <si>
+    <t>1. Forecasts, submitted by local authorities for SCAP23 , at planning area level and aggregated to local authority level. Forecasts include pupils expected to be educated in new schools (or expanded schools) funded through Housing Developer Contributions (HDC) and Housing Infrastructure Fund (HIF) agreements.
+&lt;br&gt;2. Actual pupil numbers on roll for academic year 2023/24 are taken from the January school census and aggregated to local authority level. They include pupils in roll, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. &lt;br&gt;3. Forecast accuracy is calculated by  subtracting the years R-6 actual numbers from the years R-6 forecasts to give the absolute inaccuracy. Absolute inaccuracy is then divided by the R-6 actual number to give the relative percentage inaccuracy. The same is done for secondary using years 7-11. 
+&lt;br&gt;4.  Scorecard figures may differ to those published in SCAP due to the exclusion of years 12 to 14 in the pupil numbers and forecasts used in the scorecard.</t>
+  </si>
+  <si>
+    <t>The three year ahead forecast accuracy compares actual pupil numbers on roll with forecasts of pupil numbers for 2023/24 made two years previously (in SCAP 2021) by local authority).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Forecasts of academic year 2023/24 pupil numbers made in 2020/21.
+</t>
+  </si>
+  <si>
+    <t>2. Actual pupil numbers on roll in academic year 2023/24.</t>
+  </si>
+  <si>
+    <r>
+      <t>1. Forecasts, submitted by local authorities</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>as part of the SCAP 2021, at planning area level and aggregated to local authority level. Forecasts include pupils expected to be educated in new schools (or expanded schools) funded through HDC and HIF agreements.
+&lt;br&gt;2. Actual pupil numbers on roll for academic year 2023/24 are taken from the January school census and aggregated to local authority level. They include pupils in roll, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. 	&lt;br&gt;3. Forecast accuracy is calculated by subtracting the years R-6 actual numbers from the years R-6 forecasts to give the absolute inaccuracy. Absolute inaccuracy is then divided by the R-6 actual number to give the relative percentage inaccuracy. The same is done for secondary using years 7-11. 
+&lt;br&gt;4.  Scorecard figures may differ to those published in SCAP due to the exclusion of years 12 to 14 in the pupil numbers and forecasts used in the scorecard.</t>
+    </r>
+  </si>
+  <si>
     <t>School place offers by preference for September 2024 entry</t>
   </si>
   <si>
@@ -190,236 +380,105 @@
     <t>Published School Applications and Offer data 2024/25 Academic Year</t>
   </si>
   <si>
+    <t>Quality of new school places created between academic year 2021/22 and 2022/23, based on Ofsted rating</t>
+  </si>
+  <si>
+    <t>The number of new places created between academic year 2021/22 and academic year 2022/23</t>
+  </si>
+  <si>
+    <t>Capacity of each school in May 2022</t>
+  </si>
+  <si>
+    <t>1. The following school types, identified using Get Information About Schools, have been excluded:
+&lt;br&gt;- former independent schools which have not had an inspection since opening;
+&lt;br&gt;- sponsored academies which have not had an Ofsted inspection since opening as an academy.
+&lt;br&gt;- schools that have amalgamated and have not been inspected since amalgamation.
+&lt;br&gt;2.The capacity of schools present in May 2023 is compared with May 2022 capacity.
+&lt;br&gt;3. New places are identified as an increase in school capacity of 30 places or more between May 2022 and May 2023 at each school. For mergers and academy conversions where 2022 capacity is not available, the capacities of the ‘parent’ schools in 2022 have been used.
+&lt;br&gt;4. Schools where fewer than 30 places have been created between May 2022 and May 2023 have all of their capacity counted as existing places.
+&lt;br&gt;5. Existing places are the number of places present in May 2023 after subtracting the new places since May 2022 (if 30 or more) from the May 2022 capacity.
+&lt;br&gt;6. Primary places are based on primary capacity and secondary places are based on secondary capacity reported in May 2022 or 2023. 
+&lt;br&gt;7. New places in schools which had not had an Ofsted judgment or key stage 2 or 4 result by August 2023 have been excluded from the relevant version of the measure. These places are included in the figure beneath the chart.
+&lt;br&gt;8. Because any decreases in capacity are not factored, the number of places added for use in the quality measure may not be the same as the number of places added in the quantity measure.
+&lt;br&gt;9. From June 2019 the Ofsted grades of academy predecessor schools were factored into their data, even though it may have been some time since those schools converted and/or were inspected. 
+&lt;br&gt;10. The quality measures represent the window in time when places were added and this is not necessarily the same quality outcome as when the decision to add places was taken.</t>
+  </si>
+  <si>
+    <t>Capacity for each school in May 2023</t>
+  </si>
+  <si>
     <t>Local authority data, provided through School Capacity collection 2023</t>
   </si>
   <si>
+    <t>Percentage of new places created in good and outstanding schools between academic year 2021/22 and academic year 2022/23.</t>
+  </si>
+  <si>
+    <t>Quality of new school places created between academic year 2021/22 and 2022/23, based on key stage 2 progress measures</t>
+  </si>
+  <si>
     <t>Performance tables</t>
   </si>
   <si>
     <t>Key stage 2 progress measures</t>
   </si>
   <si>
+    <t xml:space="preserve">1. Each school has been matched with the key stage 2 progress measure for reading and maths, for academic year ending July 2023 (published December 2023).
+2. This measure judges schools’ performance as 'well above average', 'above average', 'average', 'below average' or 'well below average'.
+3. The calculation counts the number of new school places that have been created in schools of each category; and the number of existing school places in each category.
+4. Middle schools may not have a key stage 2 measure and if they do, due to the age range of pupils at middle schools, pupils will have only attended a middle school for a short time before they take their key stage 2 tests and will still have a number of years left at the school. This should be taken into account when comparing their results to schools which start educating their pupils from the beginning of key stage 1.  New schools may not have a key stage 2 measure until the first cohort of pupils reaches year 6.
+5. For further information on key stage 2 progress measures please use the following url: https://www.gov.uk/government/collections/school-performance-tables-about-the-data </t>
+  </si>
+  <si>
+    <t>The quality of school places created between academic year 2021/22 and academic year 2022/23, and the quality of existing school places. Based on key stage 2 progress measures</t>
+  </si>
+  <si>
+    <t>The quality of school places created between academic year 2021/22 and academic year 2022/23, and the quality of existing school places. Based on key stage 4 progress 8 measure</t>
+  </si>
+  <si>
+    <t>Quality of new school places created between academic year 2021/22 and 2022/23, based on key stage 4 progress 8 measure</t>
+  </si>
+  <si>
     <t>Key stage 4 progress 8 measure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LA Rank- key stage 2 measures
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LA Rank- key stage 4 progress 8 measure
+</t>
+  </si>
+  <si>
+    <t>Ranks local authorities on their proportion of new school places of new school places created in well above- and above-average schools</t>
   </si>
   <si>
     <t>1. Ranking of proportions of new places created in 'well above average' and 'above average' schools for each local authority, amongst all local authorities with new places. Local authorities with the same proportion are given an equal ranking. Ranking is only applied to local authorities where new places have been created.
 2. The higher the rank the higher the proportion of new school places in well above and above average schools compared to other local authorities.</t>
   </si>
   <si>
+    <t>Percentage of new places created in well above and above-average schools between academic year 2021/22 and academic year 2022/23.</t>
+  </si>
+  <si>
     <t>1. Ranking of proportions of new places created in 'well above average' and 'above average' schools for each local authority, amongst all local authorities with new places. Local authorities with the same proportion are given an equal ranking. Ranking is only applied to local authorities where new places have been created. 
 2. The higher the rank the higher the proportion of new school places in well above and above average schools compared to other local authorities.</t>
   </si>
   <si>
-    <t xml:space="preserve">DfE internal model. Additional places needed are published in the school place planning published underlying data. </t>
-  </si>
-  <si>
-    <t>Percentage of  new school places in well above and above-average schools- key stage 2 measures</t>
-  </si>
-  <si>
-    <t>Percentage of  new school places in well above and above-average schools- key stage 4 progress 8 measure</t>
-  </si>
-  <si>
-    <t>Total places created between May 2010 and May 2024</t>
-  </si>
-  <si>
-    <t>2.Capacity at May 2024</t>
-  </si>
-  <si>
-    <t>Local authority data provided through School Capacity (SCAP) Survey 2024</t>
-  </si>
-  <si>
-    <t>1. The number of places that have been created since May 2010 in each local authority is taken as the difference between capacity as reported by local authorities, via SCAP, at May 2010 and May 2024.
-&lt;br&gt;2. The measure includes all primary and middle deemed primary school capacity in the primary phase, and all secondary, middle deemed secondary and all-through school capacity in the secondary phase.
-&lt;br&gt;3. The measure reports net increase in places only, if phase capacity in a local authority has reduced between May 2010 and May 2024, this is recorded as zero places created. Therefore the sum of the local authority-level figures will not equal the overall increase in places at national level.</t>
-  </si>
-  <si>
-    <t>Number of new places planned for delivery between May 2024 and September 2026;
+    <t>Number of new places planned for delivery between May 2023 and September 2025;
 &lt;br&gt;This contains: 
 &lt;br&gt;1) local authority firm plans for new permanent additional places , new temporary bulge places and the removal of places,
 &lt;br&gt;2) capacity changes through the Condition Improvement Fund (CIF), School Rebuilding Programme (SRP), Selective Schools Expansion Fund (SSEF), and Voluntary Aided Schools Fund (VA)
-&lt;br&gt;3) places from free schools opened in September 2024 and planned to open in September 2025
+&lt;br&gt;3) places from free schools opened in September 2023 and planned to open in September 2024
 &lt;br&gt;4) reduction in places from free school and academy closures.</t>
   </si>
   <si>
-    <t>1. Local authority plans for places to be created or removed between May 2024 and before the start of the 2026/27 academic year.</t>
-  </si>
-  <si>
-    <t>3. Places from free schools opened in September 2024 and due to be opened in September 2025.</t>
-  </si>
-  <si>
-    <t>4. Reduction in places from free school and academy closures between May 2024 and January 2025 or identified/confirmed to close before August 2025.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Local authority data about new permanent additional places, new temporary bulge places (to accommodate large cohorts as they move through the school) and permanent places to remove  2024/25, 2025/26  and 2026/27 is aggregated to local authority level.
-&lt;br&gt;2. The data was provided by local authorities in May 2024, and only includes projects they were confident would proceed. Local authorities were asked to include the total places of any new provision, even if spaces would fill gradually. 
-&lt;br&gt;3. Local authorities were asked not to include places created through free schools unless they were providing the funding for additional places themselves. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Changes to school capacity (both increases and decreases) as a consequence of works delivered through the CIF, SRP, SSEF, VA between 2024/25 and 2026/27 inclusive, aggregated to local authority level. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. The calculation mirrors the approach taken for basic need funding allocations published in March 2025. It includes mainstream primary and secondary free schools which opened in September 2024 and those with a high degree of certainty of opening in September 2025, and counts the total number of places which will be in use by September 2026.
-&lt;br&gt;2. The data does not include free schools which opened before September 2024, as they will already be included in SCAP24 and are therefore existing places. It does not include free schools which are planned to open in the academic year 2026/27 and beyond. </t>
-  </si>
-  <si>
-    <t>1. Where an academy or free school closed after 1 May 2024 its capacity, as reported in the School Capacity data, is now no longer available. Their capacity has therefore been removed from the planned delivery total.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. This measure reports planned increases in capacity only. If there is a total net planned reduction in capacity (e.g. due to a free school closure), this is shown as zero places planned. Therefore the sum of local authority-level figures will not equal the national planned places figure.
-&lt;br&gt;2. Most local authorities will have further developed their plans since this data was reported in Summer 2024, and so although it allows for comparisons between local authorities, the figure is likely to be an understatement of the current position. </t>
-  </si>
-  <si>
-    <t>Places planned to 2026/27</t>
-  </si>
-  <si>
-    <t>Unfilled places in 2023/24</t>
-  </si>
-  <si>
-    <t>Additional places needed in 2026/27; spare places in 2026/27</t>
-  </si>
-  <si>
-    <t>Estimated number of additional places needed to meet demand in 2026/27; estimated percentage of spare places in 2026/27.</t>
-  </si>
-  <si>
-    <t>Total basic need funding 2011 to 2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total amount of basic need capital funding allocated to each local authority to support them to create new mainstream primary and secondary places from 2011 to 2026. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. This refers to the amount of basic need capital funding that the Department for Education (DfE) has allocated to each local authority to create new places from the 2011-12 financial year to the 2025-26 financial year. Basic Need funding for the 2025-26 financial year is intended to support the creation of mainstream places for pupils aged 5 to 16 for the 2026/27 academic year. &lt;br&gt;2. The figure includes formula-based funding allocations and funding provided through the Targeted Basic Need Programme. Basic Need formula-based funding allocations cover the whole period and are not ring-fenced (although they can only be used for capital purposes).  Targeted Basic Need funding was provided between 2013 and 2015 and had to be spent by agreed deadlines and on specific projects. Both types of allocations are published here. &lt;br&gt;3. The figure only includes funding allocated to local authorities and does not include centrally-funded capital programmes such as the free schools programme. &lt;br&gt;4. The England total will not match the sum of allocations for all local authorities in the scorecard because the England total includes allocations to predecessor local authorities.
+    <t xml:space="preserve">DfE internal model. Additional places needed are published in the school place planning published underlying data. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LA Rank- Ofsted
 </t>
   </si>
   <si>
-    <t>Change in pupil numbers
-2009/10 to 2024/25; Anticipated change in pupil numbers 2024/25 to 2026/27</t>
-  </si>
-  <si>
-    <t>School census Jan 2025 data</t>
-  </si>
-  <si>
-    <t>Local authority data provided through the  School Capacity (SCAP) Collection 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Number of pupils in roll in January 2025, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. 							</t>
-  </si>
-  <si>
-    <t>1. This is the local authority's forecast of pupil numbers for the academic year 2026/27 as provided in SCAP 2024.
-2. These forecasts cover pupils that local authorities anticipate will attend primary schools (or primary provision in middle or all-through schools i.e. years R-6) and secondary schools (or secondary provision in middle or all-through schools i.e. years 7-11)
-3. These forecasts focus on local authorities expectations about new school places and do not include pupils who are expected to attend independent schools or special/non-mainstream provision.</t>
-  </si>
-  <si>
-    <t>Forecast accuracy of pupil projections for 2024/25</t>
-  </si>
-  <si>
-    <t>The one year ahead local authority forecast accuracy. It compares actual numbers on roll in 2024/25 with forecasts of pupil numbers for 2024/25 made one year previously (in SCAP 2024)</t>
-  </si>
-  <si>
-    <t>The three year ahead forecast accuracy compares actual pupil numbers on roll with forecasts of pupil numbers for 2024/25 made three years previously (in SCAP 2022) by local authority).</t>
-  </si>
-  <si>
-    <t>1. Forecasts of academic year 2024/25 pupil numbers made in 2023/24.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. Actual pupil numbers on roll in academic year 2024/25.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Forecasts of academic year 2024/25 pupil numbers made in 2021/22.
-</t>
-  </si>
-  <si>
-    <t>2. Actual pupil numbers on roll in academic year 2024/25.</t>
-  </si>
-  <si>
-    <t>Local authority data provided through the School Capacity (SCAP) Collection 2024</t>
-  </si>
-  <si>
-    <t>Pupils in school provided through the January 2025 School Census</t>
-  </si>
-  <si>
-    <t>Local authority data provided through the School Capacity (SCAP) Collection 2022</t>
-  </si>
-  <si>
-    <t>1. Forecasts, submitted by local authorities for SCAP24 , at planning area level and aggregated to local authority level. Forecasts include pupils expected to be educated in new schools (or expanded schools) funded through Housing Developer Contributions (HDC) and Housing Infrastructure Fund (HIF) agreements.
-&lt;br&gt;2. Actual pupil numbers on roll for academic year 2024/25 are taken from the January school census and aggregated to local authority level. They include pupils in roll, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. &lt;br&gt;3. Forecast accuracy is calculated by  subtracting the years R-6 actual numbers from the years R-6 forecasts to give the absolute inaccuracy. Absolute inaccuracy is then divided by the R-6 actual number to give the relative percentage inaccuracy. The same is done for secondary using years 7-11. 
-&lt;br&gt;4.  Scorecard figures may differ to those published in SCAP due to the exclusion of years 12 to 14 in the pupil numbers and forecasts used in the scorecard.</t>
-  </si>
-  <si>
-    <r>
-      <t>1. Forecasts, submitted by local authorities</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>as part of the SCAP 2022, at planning area level and aggregated to local authority level. Forecasts include pupils expected to be educated in new schools (or expanded schools) funded through HDC and HIF agreements.
-&lt;br&gt;2. Actual pupil numbers on roll for academic year 2024/25 are taken from the January school census and aggregated to local authority level. They include pupils in roll, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. 	&lt;br&gt;3. Forecast accuracy is calculated by subtracting the years R-6 actual numbers from the years R-6 forecasts to give the absolute inaccuracy. Absolute inaccuracy is then divided by the R-6 actual number to give the relative percentage inaccuracy. The same is done for secondary using years 7-11. 
-&lt;br&gt;4.  Scorecard figures may differ to those published in SCAP due to the exclusion of years 12 to 14 in the pupil numbers and forecasts used in the scorecard.</t>
-    </r>
-  </si>
-  <si>
-    <t>School place offers by preference for September 2025 entry</t>
-  </si>
-  <si>
-    <t>The proportion of applicants who received an offer of a place in one of their top three preference schools for September 2025 on national offer day</t>
-  </si>
-  <si>
-    <t>Published School Applications and Offer data 2025/26 Academic Year</t>
-  </si>
-  <si>
-    <t>Quality of new school places created between academic year 2022/23 and 2023/24, based on Ofsted rating</t>
-  </si>
-  <si>
-    <t>The number of new places created between academic year 2022/23 and academic year 2023/24</t>
-  </si>
-  <si>
-    <t>Capacity of each school in May 2023</t>
-  </si>
-  <si>
-    <t>Capacity for each school in May 2024</t>
-  </si>
-  <si>
-    <t>Local authority data, provided through School Capacity collection 2024</t>
-  </si>
-  <si>
-    <t>Quality of school places created between academic year 2022/23 and academic year 2023/24, based on Ofsted rating. The quality of existing school places (places in 2023/24 which were also present in 2022/23) is shown for context.</t>
-  </si>
-  <si>
-    <t>1. Each school has been matched with the Ofsted judgement of 'Overall effectiveness: how good is the school." as at 31 August 2024 (published November 2024).
-&lt;br&gt;2. There are four Ofsted categories: 'Outstanding', 'Good', 'Requires improvement' and 'Inadequate'.
-&lt;br&gt;3. The calculation counts the number of existing and new places that have been created in schools of each category. &lt;br&gt;4. Note that many schools will have been inspected some time before August 2024, and some will have been inspected since this date. &lt;br&gt;5. There are school places with no rating, as the school has yet to be inspected so do not have an Ofsted judgement.</t>
-  </si>
-  <si>
-    <t>Percentage of new places created in good and outstanding schools between academic year 2022/23 and academic year 2023/24.</t>
-  </si>
-  <si>
-    <t>The quality of school places created between academic year 2022/23 and academic year 2023/24, and the quality of existing school places. Based on key stage 2 progress measures</t>
-  </si>
-  <si>
-    <t>Quality of new school places created between academic year 2022/23 and 2023/24, based on key stage 2 progress measures</t>
-  </si>
-  <si>
-    <t>The quality of school places created between academic year 2022/23 and academic year 2023/24, and the quality of existing school places. Based on key stage 4 progress 8 measure</t>
-  </si>
-  <si>
-    <t>Quality of new school places created between academic year 2022/23 and 2023/24, based on key stage 4 progress 8 measure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Each school has been matched with the key stage 4 progress 8 measure across 8 key subjects, for academic year ending July 2024 (published February 2025).
+    <t xml:space="preserve">1. Each school has been matched with the key stage 4 progress 8 measure across 8 key subjects, for academic year ending July 2023 (published February 2024).
 2. This measure judges schools’ performance as 'well above average', 'above average', 'average', 'below average' or 'well below average'.
 3. The calculation counts the number of new school places that have been created in schools of each category; and the number of existing school places in each category.
 4. Note that middle schools will not have a key stage 4 measure, and that new schools may not have a key stage 4 measure until the first cohort of pupils reaches year 11.
@@ -428,41 +487,246 @@
 </t>
   </si>
   <si>
-    <t>Percentage of new places created in well above and above-average schools between academic year 2022/23 and academic year 2023/24.</t>
+    <t>Percentage of  new school places in well above and above-average schools- key stage 2 measures</t>
+  </si>
+  <si>
+    <t>Percentage of  new school places in well above and above-average schools- key stage 4 progress 8 measure</t>
+  </si>
+  <si>
+    <t>Quality of school places created between academic year 2021/22 and academic year 2022/23, based on Ofsted rating. The quality of existing school places (places in 2022/23 which were also present in 2021/22) is shown for context.</t>
+  </si>
+  <si>
+    <t>1. Each school has been matched with the Ofsted judgement of 'Overall effectiveness: how good is the school." as at 31 August 2023 (published November 2023).
+&lt;br&gt;2. There are four Ofsted categories: 'Outstanding', 'Good', 'Requires improvement' and 'Inadequate'.
+&lt;br&gt;3. The calculation counts the number of existing and new places that have been created in schools of each category. &lt;br&gt;4. Note that many schools will have been inspected some time before August 2023, and some will have been inspected since this date. &lt;br&gt;5. There are school places with no rating, as the school has yet to be inspected so do not have an Ofsted judgement.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The national average has been adjusted to the relevant region for each local authority, using the Building Cost Information Service (BCIS) March 2024 published regional location factors. The England national average has been multiplied by the relevant regional location factor:  East Midlands: 1.03, East of England 0.99, Inner London: 1.29, North East: 0.91, North West: 1, Outer London: 1.21, South East: 1.13, South West: 1.01, West Midlands: 0.96, Yorkshire &amp; the Humber: 0.91. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. The cost data used in the scorecard is the 2018 Capital Spend data as used in the 2018, 2019 and 2021 Scorecards. For the 2023 Scorecard, this data has been adjusted for inflation (rebased to 1st Quarter 2024 prices). National averages adjusted for 2023 regional location factors are shown. </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">You can use this data to establish developer contributions per school place, by adjusting for further inflation if needed </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(see examples below).
+&lt;br&gt;2. Projects which do not create additional mainstream places or where the project's additional place funding is zero are removed.
+&lt;br&gt;3. Projects were identified as primary  or secondary phase based on additional mainstream place year group breakdown. Where a project created places across both phases, it was assigned a phase corresponding to the phase of the school it affected (i.e. if its school was middle-deemed primary - the project was assigned to primary).
+&lt;br&gt;4. Average cost per place figures for all-through, middle-deemed primary and middle-deemed secondary schools have not been calculated separately due to low sample sizes for these project types. </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>To estimate average cost per place for middle-deemed primary schools, we recommend using primary average cost per place</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> as the middle school provides education equivalent to the education a primary school provides for all year groups. </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>To estimate average cost per place for middle-deemed secondary schools, we recommend using secondary average cost per place</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for the same reason. </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>For new middle schools or whole school expansions for middle schools not ‘deemed’ primary or secondary, we recommend taking a mid-point of the primary and secondary costs if the project covers both primary- and secondary-equivalent year groups equally</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (e.g. 2 classes per Year 5 &amp; 6 and 2 classes per Year 7 &amp; 8). </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If the project only covers certain year groups, we recommend using primary cost data if only primary-equivalent years groups are expanding</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (e.g. Years 5 &amp; 6) and </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>secondary data if only secondary-equivalent year groups are expanding</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (e.g. Years 7 &amp; 8).
+&lt;br&gt;5. The average cost does not include costs associated with land acquisition.
+&lt;br&gt;6. The average cost includes costs associated with maintenance and building condition or enhancement works.
+&lt;br&gt;7. The measure does not include places in special schools or units attached to mainstream schools, or new places which were funded through central programmes (including free schools). Where a project creates additional mainstream places and also creates SEN places or re-provides places, an adjustment has been applied to apportion out those costs. 
+&lt;br&gt;8. All costs have been normalised to a common UK average price level using regional location factors published by BCIS, March 2024, 1 is the base weight.
+&lt;br&gt;9. All costs have been adjusted for inflation using the latest BCIS All-In Tender Price of Index (TPI), published March 2024.  Costs have been rebased from the start of construction (or time of place provision if construction start date unavailable) to 1st Quarter (Jan – Mar) 2024 prices using this index (Q1 2024 index value = 390).
+10. </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>To adjust the national average to current or future prices, you need to uprate or downrate the prices in this scorecard relative to the change that has happened since Q1 2024</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.  If you have access to the BCIS indices via a subscription to BCIS Online (https://www.rics.org/uk/products/data-products/bcis-construction/bcis-online/) you can use the latest inflation index to re-base (weight to apply = latest index/390).  If not, you can apply a known change to the published cost (e.g. up or down x%).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Example: New primary school in Outer London Q3 (Jul - Sep) 2024.  
+National average for primary new school place = £23,865. 
+Outer London location factor = 1.21 (taken from published BCIS regional location factors March 2023)
+Inflation weight = 394/390 = 1.01 ( taken from BCIS All-In TPI published March 2023). 
+Average primary New School place cost that applies to Outer London in Q3 2023 prices = £23,192 x 1.21 x 1.01 = £29,200 (rounded to nearest £100).  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+If you do not have access the BCIS index, but sources say TPI inflation is set to increase by 4% per annum, then approximate inflation weight = 6% (18 months’ worth of inflation) = 1.06.
+11. Some additional but limited benchmark information for similar capital programme schemes carried out by the DfE is available in the National School Delivery Cost Benchmarking study: https://documents.hants.gov.uk/property-services/NationalSchoolDeliveryBenchmarkingreport.pdf</t>
+    </r>
+  </si>
+  <si>
+    <t>Publication</t>
+  </si>
+  <si>
+    <t>2022/23</t>
+  </si>
+  <si>
+    <t>1. The number of places that have been created since May 2010 in each local authority is taken as the difference between capacity as reported by local authorities, via SCAP, at May 2010 and May 2024.
+&lt;br&gt;2. The measure includes all primary and middle deemed primary school capacity in the primary phase, and all secondary, middle deemed secondary and all-through school capacity in the secondary phase.
+&lt;br&gt;3. The measure reports net increase in places only, if phase capacity in a local authority has reduced between May 2010 and May 2024, this is recorded as zero places created. Therefore the sum of the local authority-level figures will not equal the overall increase in places at national level.</t>
+  </si>
+  <si>
+    <t>2.Capacity at May 2024</t>
+  </si>
+  <si>
+    <t>Local authority data provided through School Capacity (SCAP) Survey 2024</t>
+  </si>
+  <si>
+    <t>1. Local authority plans for places to be created or removed between May 2024 and before the start of the 2026/27 academic year.</t>
   </si>
   <si>
     <t>Local authority data provided through the School Capacity (SCAP) Survey 2024.</t>
   </si>
   <si>
-    <t>The actual percentage change in pupil numbers between 2009/10, 2014/15 (for secondary), 2018/19 (for primary) and 2024/25; the anticipated percentage change in pupil numbers in primary or secondary state-funded mainstream provision between the 2024/25 and 2026/27 academic years.</t>
-  </si>
-  <si>
-    <t>School census Jan 2015 data</t>
-  </si>
-  <si>
-    <t>School census Jan 2019 data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Number of pupils in roll in January 2015, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Number of pupils in roll in January 2019, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. </t>
+    <t xml:space="preserve">1. Local authority data about new permanent additional places, new temporary bulge places (to accommodate large cohorts as they move through the school) and permanent places to remove  2024/25, 2025/26  and 2026/27 is aggregated to local authority level.
+&lt;br&gt;2. The data was provided by local authorities in May 2024, and only includes projects they were confident would proceed. Local authorities were asked to include the total places of any new provision, even if spaces would fill gradually. 
+&lt;br&gt;3. Local authorities were asked not to include places created through free schools unless they were providing the funding for additional places themselves. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Changes to school capacity (both increases and decreases) as a consequence of works delivered through the CIF, SRP, SSEF, VA between 2024/25 and 2026/27 inclusive, aggregated to local authority level. </t>
+  </si>
+  <si>
+    <t>3. Places from free schools opened in September 2024 and due to be opened in September 2025.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. The calculation mirrors the approach taken for basic need funding allocations published in March 2025. It includes mainstream primary and secondary free schools which opened in September 2024 and those with a high degree of certainty of opening in September 2025, and counts the total number of places which will be in use by September 2026.
+&lt;br&gt;2. The data does not include free schools which opened before September 2024, as they will already be included in SCAP24 and are therefore existing places. It does not include free schools which are planned to open in the academic year 2026/27 and beyond. </t>
+  </si>
+  <si>
+    <t>4. Reduction in places from free school and academy closures between May 2024 and January 2025 or identified/confirmed to close before August 2025.</t>
+  </si>
+  <si>
+    <t>1. Where an academy or free school closed after 1 May 2024 its capacity, as reported in the School Capacity data, is now no longer available. Their capacity has therefore been removed from the planned delivery total.</t>
   </si>
   <si>
     <t>5. Total number of planned places (sum of 1, 2, 3, and 4 above)</t>
   </si>
   <si>
-    <t>2. Pupil Numbers for the 2014/15 academic year taken from the pupil census in January 2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3. Pupil Numbers for the 2018/19 academic year taken from the pupil census in January 2019
-</t>
-  </si>
-  <si>
-    <t>4. Pupil Numbers for the 2024/25 academic year taken from the pupil census in January 2025</t>
-  </si>
-  <si>
-    <t>5. Forecast pupil numbers for the 2026/27 academic year</t>
+    <t xml:space="preserve">1. This measure reports planned increases in capacity only. If there is a total net planned reduction in capacity (e.g. due to a free school closure), this is shown as zero places planned. Therefore the sum of local authority-level figures will not equal the national planned places figure.
+&lt;br&gt;2. Most local authorities will have further developed their plans since this data was reported in Summer 2024, and so although it allows for comparisons between local authorities, the figure is likely to be an understatement of the current position. </t>
   </si>
   <si>
     <t>1.This relates to the academic year 2026/27 and is the difference between local authority pupil forecasts and future capacity, taking account of planned future additions and places to remove.
@@ -476,12 +740,167 @@
 &lt;br&gt;8. Estimates for spare places are presented as a percentage of total future capacity.</t>
   </si>
   <si>
-    <t>1. Number of new school places created
-2. Quality of new places created as judged by key stage 2 progress measures</t>
-  </si>
-  <si>
-    <t>1. Number of new school places created
-2. Quality of new places created as judged by key stage 4 progress 8 measure</t>
+    <t xml:space="preserve">1. This refers to the amount of basic need capital funding that the Department for Education (DfE) has allocated to each local authority to create new places from the 2011-12 financial year to the 2025-26 financial year. Basic Need funding for the 2025-26 financial year is intended to support the creation of mainstream places for pupils aged 5 to 16 for the 2026/27 academic year. &lt;br&gt;2. The figure includes formula-based funding allocations and funding provided through the Targeted Basic Need Programme. Basic Need formula-based funding allocations cover the whole period and are not ring-fenced (although they can only be used for capital purposes).  Targeted Basic Need funding was provided between 2013 and 2015 and had to be spent by agreed deadlines and on specific projects. Both types of allocations are published here. &lt;br&gt;3. The figure only includes funding allocated to local authorities and does not include centrally-funded capital programmes such as the free schools programme. &lt;br&gt;4. The England total will not match the sum of allocations for all local authorities in the scorecard because the England total includes allocations to predecessor local authorities.
+</t>
+  </si>
+  <si>
+    <t>2. Pupil Numbers for the 2014/15 academic year taken from the pupil census in January 2015</t>
+  </si>
+  <si>
+    <t>School census Jan 2015 data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Number of pupils in roll in January 2015, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Pupil Numbers for the 2018/19 academic year taken from the pupil census in January 2019
+</t>
+  </si>
+  <si>
+    <t>School census Jan 2019 data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Number of pupils in roll in January 2019, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. </t>
+  </si>
+  <si>
+    <t>4. Pupil Numbers for the 2024/25 academic year taken from the pupil census in January 2025</t>
+  </si>
+  <si>
+    <t>School census Jan 2025 data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Number of pupils in roll in January 2025, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. 							</t>
+  </si>
+  <si>
+    <t>5. Forecast pupil numbers for the 2026/27 academic year</t>
+  </si>
+  <si>
+    <t>Local authority data provided through the  School Capacity (SCAP) Collection 2024</t>
+  </si>
+  <si>
+    <t>1. This is the local authority's forecast of pupil numbers for the academic year 2026/27 as provided in SCAP 2024.
+2. These forecasts cover pupils that local authorities anticipate will attend primary schools (or primary provision in middle or all-through schools i.e. years R-6) and secondary schools (or secondary provision in middle or all-through schools i.e. years 7-11)
+3. These forecasts focus on local authorities expectations about new school places and do not include pupils who are expected to attend independent schools or special/non-mainstream provision.</t>
+  </si>
+  <si>
+    <t>Total places created between May 2010 and May 2024</t>
+  </si>
+  <si>
+    <t>Places planned to 2026/27</t>
+  </si>
+  <si>
+    <t>Number of new places planned for delivery between May 2024 and September 2026;
+&lt;br&gt;This contains: 
+&lt;br&gt;1) local authority firm plans for new permanent additional places , new temporary bulge places and the removal of places,
+&lt;br&gt;2) capacity changes through the Condition Improvement Fund (CIF), School Rebuilding Programme (SRP), Selective Schools Expansion Fund (SSEF), and Voluntary Aided Schools Fund (VA)
+&lt;br&gt;3) places from free schools opened in September 2024 and planned to open in September 2025
+&lt;br&gt;4) reduction in places from free school and academy closures.</t>
+  </si>
+  <si>
+    <t>Unfilled places in 2023/24</t>
+  </si>
+  <si>
+    <t>Additional places needed in 2026/27; spare places in 2026/27</t>
+  </si>
+  <si>
+    <t>Estimated number of additional places needed to meet demand in 2026/27; estimated percentage of spare places in 2026/27.</t>
+  </si>
+  <si>
+    <t>Total basic need funding 2011 to 2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total amount of basic need capital funding allocated to each local authority to support them to create new mainstream primary and secondary places from 2011 to 2026. </t>
+  </si>
+  <si>
+    <t>Change in pupil numbers
+2009/10 to 2024/25; Anticipated change in pupil numbers 2024/25 to 2026/27</t>
+  </si>
+  <si>
+    <t>The actual percentage change in pupil numbers between 2009/10, 2014/15 (for secondary), 2018/19 (for primary) and 2024/25; the anticipated percentage change in pupil numbers in primary or secondary state-funded mainstream provision between the 2024/25 and 2026/27 academic years.</t>
+  </si>
+  <si>
+    <t>2023/24</t>
+  </si>
+  <si>
+    <t>Forecast accuracy of pupil projections for 2024/25</t>
+  </si>
+  <si>
+    <t>The one year ahead local authority forecast accuracy. It compares actual numbers on roll in 2024/25 with forecasts of pupil numbers for 2024/25 made one year previously (in SCAP 2024)</t>
+  </si>
+  <si>
+    <t>1. Forecasts of academic year 2024/25 pupil numbers made in 2023/24.</t>
+  </si>
+  <si>
+    <t>Local authority data provided through the School Capacity (SCAP) Collection 2024</t>
+  </si>
+  <si>
+    <t>1. Forecasts, submitted by local authorities for SCAP24 , at planning area level and aggregated to local authority level. Forecasts include pupils expected to be educated in new schools (or expanded schools) funded through Housing Developer Contributions (HDC) and Housing Infrastructure Fund (HIF) agreements.
+&lt;br&gt;2. Actual pupil numbers on roll for academic year 2024/25 are taken from the January school census and aggregated to local authority level. They include pupils in roll, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. &lt;br&gt;3. Forecast accuracy is calculated by  subtracting the years R-6 actual numbers from the years R-6 forecasts to give the absolute inaccuracy. Absolute inaccuracy is then divided by the R-6 actual number to give the relative percentage inaccuracy. The same is done for secondary using years 7-11. 
+&lt;br&gt;4.  Scorecard figures may differ to those published in SCAP due to the exclusion of years 12 to 14 in the pupil numbers and forecasts used in the scorecard.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Actual pupil numbers on roll in academic year 2024/25.
+</t>
+  </si>
+  <si>
+    <t>Pupils in school provided through the January 2025 School Census</t>
+  </si>
+  <si>
+    <t>The three year ahead forecast accuracy compares actual pupil numbers on roll with forecasts of pupil numbers for 2024/25 made three years previously (in SCAP 2022) by local authority).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Forecasts of academic year 2024/25 pupil numbers made in 2021/22.
+</t>
+  </si>
+  <si>
+    <t>Local authority data provided through the School Capacity (SCAP) Collection 2022</t>
+  </si>
+  <si>
+    <r>
+      <t>1. Forecasts, submitted by local authorities</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>as part of the SCAP 2022, at planning area level and aggregated to local authority level. Forecasts include pupils expected to be educated in new schools (or expanded schools) funded through HDC and HIF agreements.
+&lt;br&gt;2. Actual pupil numbers on roll for academic year 2024/25 are taken from the January school census and aggregated to local authority level. They include pupils in roll, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. 	&lt;br&gt;3. Forecast accuracy is calculated by subtracting the years R-6 actual numbers from the years R-6 forecasts to give the absolute inaccuracy. Absolute inaccuracy is then divided by the R-6 actual number to give the relative percentage inaccuracy. The same is done for secondary using years 7-11. 
+&lt;br&gt;4.  Scorecard figures may differ to those published in SCAP due to the exclusion of years 12 to 14 in the pupil numbers and forecasts used in the scorecard.</t>
+    </r>
+  </si>
+  <si>
+    <t>2. Actual pupil numbers on roll in academic year 2024/25.</t>
+  </si>
+  <si>
+    <t>School place offers by preference for September 2025 entry</t>
+  </si>
+  <si>
+    <t>The proportion of applicants who received an offer of a place in one of their top three preference schools for September 2025 on national offer day</t>
+  </si>
+  <si>
+    <t>Published School Applications and Offer data 2025/26 Academic Year</t>
+  </si>
+  <si>
+    <t>Quality of new school places created between academic year 2022/23 and 2023/24, based on Ofsted rating</t>
+  </si>
+  <si>
+    <t>The number of new places created between academic year 2022/23 and academic year 2023/24</t>
+  </si>
+  <si>
+    <t>Capacity of each school in May 2023</t>
   </si>
   <si>
     <t>1. The following school types, identified using Get Information About Schools, have been excluded:
@@ -500,11 +919,60 @@
 &lt;br&gt;10. The quality measures represent the window in time when places were added and this is not necessarily the same quality outcome as when the decision to add places was taken.</t>
   </si>
   <si>
+    <t>Capacity for each school in May 2024</t>
+  </si>
+  <si>
+    <t>Local authority data, provided through School Capacity collection 2024</t>
+  </si>
+  <si>
+    <t>Quality of school places created between academic year 2022/23 and academic year 2023/24, based on Ofsted rating. The quality of existing school places (places in 2023/24 which were also present in 2022/23) is shown for context.</t>
+  </si>
+  <si>
+    <t>1. Each school has been matched with the Ofsted judgement of 'Overall effectiveness: how good is the school." as at 31 August 2024 (published November 2024).
+&lt;br&gt;2. There are four Ofsted categories: 'Outstanding', 'Good', 'Requires improvement' and 'Inadequate'.
+&lt;br&gt;3. The calculation counts the number of existing and new places that have been created in schools of each category. &lt;br&gt;4. Note that many schools will have been inspected some time before August 2024, and some will have been inspected since this date. &lt;br&gt;5. There are school places with no rating, as the school has yet to be inspected so do not have an Ofsted judgement.</t>
+  </si>
+  <si>
+    <t>Percentage of new places created in good and outstanding schools between academic year 2022/23 and academic year 2023/24.</t>
+  </si>
+  <si>
+    <t>The quality of school places created between academic year 2022/23 and academic year 2023/24, and the quality of existing school places. Based on key stage 2 progress measures</t>
+  </si>
+  <si>
+    <t>Quality of new school places created between academic year 2022/23 and 2023/24, based on key stage 2 progress measures</t>
+  </si>
+  <si>
     <t xml:space="preserve">1. Each school has been matched with the key stage 2 progress measure for reading and maths, for academic year ending July 2023 (published December 2023). It was not be possible to calculate KS1-KS2 progress measures for the 2023/24 academic year, because there is no relevant KS1 data required to calculate KS1-KS2 progress measures for these cohorts, as primary tests and assessments were cancelled in academic years 2019/20 and 2020/21 due to COVID-19 disruption.
 2. This measure judges schools’ performance as 'well above average', 'above average', 'average', 'below average' or 'well below average'.
 3. The calculation counts the number of new school places that have been created in schools of each category; and the number of existing school places in each category.
 4. Middle schools may not have a key stage 2 measure and if they do, due to the age range of pupils at middle schools, pupils will have only attended a middle school for a short time before they take their key stage 2 tests and will still have a number of years left at the school. This should be taken into account when comparing their results to schools which start educating their pupils from the beginning of key stage 1.  New schools may not have a key stage 2 measure until the first cohort of pupils reaches year 6.
 5. For further information on key stage 2 progress measures please use the following url: https://www.gov.uk/government/collections/school-performance-tables-about-the-data </t>
+  </si>
+  <si>
+    <t>The quality of school places created between academic year 2022/23 and academic year 2023/24, and the quality of existing school places. Based on key stage 4 progress 8 measure</t>
+  </si>
+  <si>
+    <t>Quality of new school places created between academic year 2022/23 and 2023/24, based on key stage 4 progress 8 measure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Each school has been matched with the key stage 4 progress 8 measure across 8 key subjects, for academic year ending July 2024 (published February 2025).
+2. This measure judges schools’ performance as 'well above average', 'above average', 'average', 'below average' or 'well below average'.
+3. The calculation counts the number of new school places that have been created in schools of each category; and the number of existing school places in each category.
+4. Note that middle schools will not have a key stage 4 measure, and that new schools may not have a key stage 4 measure until the first cohort of pupils reaches year 11.
+5. Note that this progress 8 measure is not a strict measure of the effectiveness of the entire school as a school may add value before pupils take the key stage tests. 
+6. For further information on progress 8 measure please use the following url: https://www.gov.uk/government/collections/school-performance-tables-about-the-data 
+</t>
+  </si>
+  <si>
+    <t>Percentage of new places created in well above and above-average schools between academic year 2022/23 and academic year 2023/24.</t>
+  </si>
+  <si>
+    <t>1. Number of new school places created
+2. Quality of new places created as judged by key stage 2 progress measures</t>
+  </si>
+  <si>
+    <t>1. Number of new school places created
+2. Quality of new places created as judged by key stage 4 progress 8 measure</t>
   </si>
   <si>
     <t xml:space="preserve">The national average has been adjusted to the relevant region for each local authority, using the Building Cost Information Service (BCIS) March 2023 published regional location factors. The England national average has been multiplied by the relevant regional location factor:  East Midlands: 1.03, East of England 0.99, Inner London: 1.29, North East: 0.91, North West: 1, Outer London: 1.21, South East: 1.13, South West: 1.01, West Midlands: 0.96, Yorkshire &amp; the Humber: 0.91. </t>
@@ -983,9 +1451,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF104F75"/>
-      </left>
+      <left/>
       <right style="dotted">
         <color auto="1"/>
       </right>
@@ -996,13 +1462,13 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="dotted">
-        <color auto="1"/>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
       </right>
-      <top style="dotted">
-        <color auto="1"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -1011,7 +1477,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1035,6 +1501,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1062,15 +1531,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1080,7 +1549,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
@@ -1131,9 +1606,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1149,28 +1621,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1488,10 +1964,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8372DA64-5E2C-41C1-8CF4-85BC1C2AFF86}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView topLeftCell="C11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1503,7 +1979,7 @@
     <col min="5" max="5" width="87.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1519,13 +1995,16 @@
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F1" s="51" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="42" t="s">
-        <v>38</v>
+      <c r="B2" s="44" t="s">
+        <v>34</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>2</v>
@@ -1533,211 +2012,483 @@
       <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="44" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
-      <c r="B3" s="43"/>
+      <c r="B3" s="45"/>
       <c r="C3" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="43"/>
-    </row>
-    <row r="4" spans="1:5" ht="138" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="45"/>
+      <c r="F3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="138" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
-      <c r="B5" s="46"/>
+      <c r="B5" s="48"/>
       <c r="C5" s="6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="E5" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="12" t="s">
+      <c r="B6" s="48"/>
+      <c r="C6" s="13" t="s">
         <v>44</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="E6" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="12" t="s">
+      <c r="B7" s="48"/>
+      <c r="C7" s="13" t="s">
         <v>45</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="22"/>
+      <c r="D9" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="375" x14ac:dyDescent="0.25">
+      <c r="A10" s="32" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="12" t="s">
+      <c r="B10" s="13" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="375" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>54</v>
       </c>
       <c r="C10" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="22" t="s">
-        <v>35</v>
+      <c r="D10" s="23" t="s">
+        <v>99</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="F10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" s="13"/>
+        <v>52</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="14"/>
       <c r="D11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="11" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="50" t="s">
+      <c r="D13" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="47" t="s">
-        <v>93</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="10" t="s">
+      <c r="E13" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="46" t="s">
+        <v>110</v>
+      </c>
+      <c r="F15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E16" s="45"/>
+      <c r="F16" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B17" s="47" t="s">
+        <v>139</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="F17" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="51"/>
-      <c r="B13" s="48"/>
-      <c r="C13" s="10" t="s">
+      <c r="D18" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="F18" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="F19" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="F20" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="8"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="F21" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B22" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="22"/>
+      <c r="D22" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="375" x14ac:dyDescent="0.25">
+      <c r="A23" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="D13" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="51"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="51"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="52"/>
-      <c r="B16" s="49"/>
-      <c r="C16" s="27" t="s">
-        <v>102</v>
-      </c>
-      <c r="D16" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" s="27" t="s">
-        <v>62</v>
+      <c r="E23" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="F23" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="C24" s="14"/>
+      <c r="D24" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="F24" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="52" t="s">
+        <v>145</v>
+      </c>
+      <c r="B25" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="54"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="F26" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="54"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="F27" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="54"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="F28" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="56"/>
+      <c r="B29" s="57"/>
+      <c r="C29" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="E29" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="F29" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="B25:B29"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="B4:B8"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="E15:E16"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <hyperlinks>
@@ -1745,131 +2496,229 @@
     <hyperlink ref="D10" r:id="rId2" display=" 2021/22 school place planning published underlying data. " xr:uid="{093B09C6-85AC-4B03-8BE4-078C82660B4C}"/>
     <hyperlink ref="D2" r:id="rId3" xr:uid="{8150C38D-D188-4C8E-86C3-B5575B8FFEE8}"/>
     <hyperlink ref="D11" r:id="rId4" xr:uid="{84C17436-4B87-48EB-BAE5-31DBACCBDB31}"/>
-    <hyperlink ref="D15" r:id="rId5" display="School census Jan 2023 data" xr:uid="{B4335ED1-45C2-43A8-BAE4-D6C4C7E179D0}"/>
+    <hyperlink ref="D13" r:id="rId5" display="School census Jan 2023 data" xr:uid="{B4335ED1-45C2-43A8-BAE4-D6C4C7E179D0}"/>
     <hyperlink ref="D12" r:id="rId6" xr:uid="{CCB6838D-DD36-44DD-BC08-5E652C942FA3}"/>
     <hyperlink ref="D9" r:id="rId7" display="Local authority data provided through School Capacity (SCAP) Survey 2021" xr:uid="{F7517439-C801-46CD-8DC3-B6DD58F4289A}"/>
-    <hyperlink ref="D16" r:id="rId8" display="Local authority data provided through the  School Capacity (SCAP) Collection 2022" xr:uid="{2257ADC3-56E0-46AA-984A-65A14B6B91D4}"/>
-    <hyperlink ref="D13" r:id="rId9" xr:uid="{79AE5929-1652-4611-9E48-29269254E396}"/>
-    <hyperlink ref="D14" r:id="rId10" xr:uid="{4D3E4206-3C34-46F2-94BA-63E9C87A86E9}"/>
+    <hyperlink ref="D14" r:id="rId8" display="Local authority data provided through the  School Capacity (SCAP) Collection 2022" xr:uid="{2257ADC3-56E0-46AA-984A-65A14B6B91D4}"/>
+    <hyperlink ref="D17" r:id="rId9" display="Local authority data provided through the School Capacity (SCAP) Survey 2022." xr:uid="{D140B5FC-6CE2-48F1-BF21-C9EC2586782D}"/>
+    <hyperlink ref="D23" r:id="rId10" display=" 2021/22 school place planning published underlying data. " xr:uid="{168FA84B-11B4-4C80-A7A5-597B690A65BF}"/>
+    <hyperlink ref="D15" r:id="rId11" xr:uid="{D7EB4574-CB25-42A9-B4C2-3913F62B5513}"/>
+    <hyperlink ref="D24" r:id="rId12" xr:uid="{3D41CC56-05BA-471B-ABB1-3CB74AC2778A}"/>
+    <hyperlink ref="D28" r:id="rId13" display="School census Jan 2023 data" xr:uid="{F0889FF8-A60B-411C-A004-D5DA89758A71}"/>
+    <hyperlink ref="D25" r:id="rId14" xr:uid="{57A1343E-B39E-429E-94B0-FD3C6471C21E}"/>
+    <hyperlink ref="D22" r:id="rId15" display="Local authority data provided through School Capacity (SCAP) Survey 2021" xr:uid="{4E4AE6EF-3D53-4105-97A1-065AADC66650}"/>
+    <hyperlink ref="D29" r:id="rId16" display="Local authority data provided through the  School Capacity (SCAP) Collection 2022" xr:uid="{712DF8AA-676E-41AB-BBBE-2AB832B676D0}"/>
+    <hyperlink ref="D26" r:id="rId17" xr:uid="{506A2691-ED47-412F-A8C0-7648AE09BFD7}"/>
+    <hyperlink ref="D27" r:id="rId18" xr:uid="{CC0BA90D-BAE6-4C2F-9262-0D1CAD7283ED}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C67D23D-5B13-4F00-9F83-043839CEFFD1}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="55.42578125" style="31"/>
+    <col min="1" max="16384" width="55.42578125" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="31" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="F1" s="31" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="32"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D3" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="50"/>
+      <c r="F3" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="32"/>
+      <c r="B4" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="45" t="s">
+      <c r="C4" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="47" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="300.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="54"/>
-      <c r="C3" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="E3" s="54"/>
-    </row>
-    <row r="4" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="29"/>
-      <c r="B4" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="12" t="s">
+      <c r="F4" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="39"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="E4" s="45" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="272.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="36"/>
-      <c r="B5" s="53"/>
-      <c r="C5" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="D5" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="E5" s="53"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="E6" s="47" t="s">
+        <v>152</v>
+      </c>
+      <c r="F6" s="34" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="32"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="D7" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="E7" s="50"/>
+      <c r="F7" s="34" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="32"/>
+      <c r="B8" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" s="38" t="s">
+        <v>157</v>
+      </c>
+      <c r="E8" s="47" t="s">
+        <v>158</v>
+      </c>
+      <c r="F8" s="34" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="39"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="D9" s="40" t="s">
+        <v>154</v>
+      </c>
+      <c r="E9" s="49"/>
+      <c r="F9" s="34" t="s">
+        <v>147</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="E8:E9"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="E2:E3"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="E6:E7"/>
   </mergeCells>
+  <phoneticPr fontId="9" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="Local authority data provided through the School Capacity (SCAP) Collection 2022" xr:uid="{D14A8E59-0240-4725-B7AC-4582058C6B59}"/>
-    <hyperlink ref="D4" r:id="rId2" display="Local authority data provided through the School Capacity (SCAP) Collection 2021" xr:uid="{586F3224-6D8F-4AF9-899D-550CFDC0058F}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{586F3224-6D8F-4AF9-899D-550CFDC0058F}"/>
     <hyperlink ref="D3" r:id="rId3" display="Pupils in school provided through the January 2023 School Census" xr:uid="{17405BAA-EC5B-41A8-9F2F-BBE920A0B9BB}"/>
     <hyperlink ref="D5" r:id="rId4" display="Pupils in school provided through the January 2023 School Census" xr:uid="{54B0E578-7E98-4CE5-8BEB-25623CA0296D}"/>
+    <hyperlink ref="D6" r:id="rId5" display="Local authority data provided through the School Capacity (SCAP) Collection 2022" xr:uid="{F94E27B9-93F2-492F-B022-03D1BF2ED50B}"/>
+    <hyperlink ref="D8" r:id="rId6" display="Local authority data provided through the School Capacity (SCAP) Collection 2021" xr:uid="{DB6C9518-4974-4D88-A3FD-A0D73E1156DA}"/>
+    <hyperlink ref="D7" r:id="rId7" display="Pupils in school provided through the January 2023 School Census" xr:uid="{D4EB79EF-B53B-4F30-A202-85F4FBDCA5DB}"/>
+    <hyperlink ref="D9" r:id="rId8" display="Pupils in school provided through the January 2023 School Census" xr:uid="{A8F94BE9-CA43-4F91-A3C7-D2BD25322736}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3163888B-9214-4218-82C5-5CD72F2D39D0}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="48.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1885,41 +2734,88 @@
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="197.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="F1" s="31" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="E2" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="C3" s="13"/>
+      <c r="D3" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>16</v>
+      <c r="E3" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="58" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="58" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="Published School Applications and Offer data 2022/23 Academic Year" xr:uid="{65C563AA-E96A-4DA3-9BD3-0A919A6BB712}"/>
     <hyperlink ref="D3" r:id="rId2" display="Published School Applications and Offer data 2022/23 Academic Year" xr:uid="{73E1A89E-78ED-4859-B41E-1AE6B97802E3}"/>
+    <hyperlink ref="D4" r:id="rId3" display="Published School Applications and Offer data 2022/23 Academic Year" xr:uid="{DEAC6B57-4AAA-46A4-8F99-7C21A4EAB388}"/>
+    <hyperlink ref="D5" r:id="rId4" display="Published School Applications and Offer data 2022/23 Academic Year" xr:uid="{1A8CD594-5A7A-4EBE-87C4-EDF4055AC3CF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1927,165 +2823,388 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{172A91E8-EE08-4774-802F-E9F4C78EAB63}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="37.28515625" style="31"/>
-    <col min="5" max="5" width="77.28515625" style="31" customWidth="1"/>
-    <col min="6" max="16384" width="37.28515625" style="31"/>
+    <col min="1" max="4" width="37.28515625" style="34"/>
+    <col min="5" max="5" width="77.28515625" style="34" customWidth="1"/>
+    <col min="6" max="16384" width="37.28515625" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="31" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="F1" s="31" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="C2" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="12" t="s">
+      <c r="F2" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="41"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="39"/>
-    </row>
-    <row r="4" spans="1:5" ht="150" x14ac:dyDescent="0.25">
-      <c r="A4" s="38"/>
-      <c r="B4" s="40" t="s">
+      <c r="E3" s="42"/>
+      <c r="F3" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A4" s="41"/>
+      <c r="B4" s="43" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="F4" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="255" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="240" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="F8" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="F10" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="D13" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="F13" s="34" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="41"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="D14" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="E14" s="42"/>
+      <c r="F14" s="34" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A15" s="41"/>
+      <c r="B15" s="43" t="s">
+        <v>169</v>
+      </c>
+      <c r="C15" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D15" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="12" t="s">
+      <c r="E15" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="F15" s="34" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="34" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="315" x14ac:dyDescent="0.25">
+      <c r="A17" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="315" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="240" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="12" t="s">
+      <c r="E17" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="F17" s="34" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="240" x14ac:dyDescent="0.25">
+      <c r="A18" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="C18" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="12" t="s">
-        <v>34</v>
+      <c r="D18" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="F18" s="34" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="D19" s="28"/>
+      <c r="E19" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F19" s="34" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="D20" s="28"/>
+      <c r="E20" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="F20" s="34" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="Local authority data, provided through School Capacity collection 2022" xr:uid="{6EE32724-1837-46BD-9FD6-A4EEFD1E0A4A}"/>
-    <hyperlink ref="D3" r:id="rId2" display="Local authority data, provided through School Capacity collection 2023" xr:uid="{F8935CE3-E46D-430A-A5BC-BAB4A254BDA2}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{6EE32724-1837-46BD-9FD6-A4EEFD1E0A4A}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{F8935CE3-E46D-430A-A5BC-BAB4A254BDA2}"/>
     <hyperlink ref="D4" r:id="rId3" xr:uid="{2FB89BF4-390E-4CD5-92FB-FD0FF31F028D}"/>
-    <hyperlink ref="D6" r:id="rId4" xr:uid="{4534F643-19C4-4655-8095-8044AC4B7902}"/>
-    <hyperlink ref="D7" r:id="rId5" xr:uid="{4889CA3C-1157-412C-ACB1-EE5DA00A90DF}"/>
+    <hyperlink ref="D7" r:id="rId4" xr:uid="{4534F643-19C4-4655-8095-8044AC4B7902}"/>
+    <hyperlink ref="D8" r:id="rId5" xr:uid="{4889CA3C-1157-412C-ACB1-EE5DA00A90DF}"/>
+    <hyperlink ref="D13" r:id="rId6" display="Local authority data, provided through School Capacity collection 2022" xr:uid="{73725C21-EC8E-495A-8521-6604BDCA9BF5}"/>
+    <hyperlink ref="D14" r:id="rId7" display="Local authority data, provided through School Capacity collection 2023" xr:uid="{3107590D-6B8F-4322-8365-F40271488FAC}"/>
+    <hyperlink ref="D15" r:id="rId8" xr:uid="{169006D7-2497-4BE8-90DB-4A1783604C5F}"/>
+    <hyperlink ref="D17" r:id="rId9" xr:uid="{6D9BDEC1-A85B-4BAE-B25C-DC97AE840965}"/>
+    <hyperlink ref="D18" r:id="rId10" xr:uid="{D90B4F41-BA2F-44BC-AA85-E0C3BEF1F585}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2093,94 +3212,115 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB73E146-A141-4797-B302-F0B3455C0C2E}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="57.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="57.5703125" style="31"/>
+    <col min="1" max="16384" width="57.5703125" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="31" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="14" t="s">
+      <c r="F1" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="14" t="s">
+    </row>
+    <row r="2" spans="1:6" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="34" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="41"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="18"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="17"/>
+    <row r="3" spans="1:6" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="18"/>
       <c r="C4" s="19"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="17"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="18"/>
       <c r="C5" s="19"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="17"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="18"/>
       <c r="C6" s="19"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="17"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="18"/>
       <c r="C7" s="19"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="17"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="18"/>
       <c r="C8" s="19"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="17"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="18"/>
       <c r="C9" s="19"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="17"/>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="18"/>
       <c r="C10" s="19"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="17"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="18"/>
       <c r="C11" s="19"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="17"/>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="18"/>
       <c r="C12" s="19"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="17"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="18"/>
       <c r="C13" s="19"/>
     </row>
   </sheetData>
@@ -2190,6 +3330,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="ec07c698-60f5-424f-b9af-f4c59398b511" ContentTypeId="0x010100545E941595ED5448BA61900FDDAFF313" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Official Document" ma:contentTypeID="0x010100545E941595ED5448BA61900FDDAFF31300C0D9F77D091A79449828113EF8250EF5" ma:contentTypeVersion="9" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="3acf8af8f3f036fb6d934619e757bc96">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8c566321-f672-4e06-a901-b5e72b4c4357" xmlns:ns3="2a6436df-3f7a-48ac-8ea6-44b411e24bbc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="926947be84ee9a0228ce6a037c6848ba" ns2:_="" ns3:_="">
     <xsd:import namespace="8c566321-f672-4e06-a901-b5e72b4c4357"/>
@@ -2395,7 +3540,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
@@ -2440,7 +3585,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2449,7 +3594,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -2499,12 +3644,15 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="ec07c698-60f5-424f-b9af-f4c59398b511" ContentTypeId="0x010100545E941595ED5448BA61900FDDAFF313" PreviousValue="false"/>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D00F0DC4-2D9F-43FC-8616-EC131ED26B7D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1E94FF3-D2F7-4169-BE5C-5ED202BAA024}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2523,24 +3671,24 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{334E8BC2-6B82-4EDA-BE50-EFE4767E8CD2}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="8c566321-f672-4e06-a901-b5e72b4c4357"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8c566321-f672-4e06-a901-b5e72b4c4357"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="2a6436df-3f7a-48ac-8ea6-44b411e24bbc"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{035EEA42-582A-4724-B162-C22729062C2B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -2548,18 +3696,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9C56A4F-6917-41AA-BBE5-DA7C75896563}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D00F0DC4-2D9F-43FC-8616-EC131ED26B7D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adding 2023 data to 2024 scorecard (#127)
* Adding 2023 data to 2024 scorecard

* install data.table
</commit_message>
<xml_diff>
--- a/data/tech_guidance.xlsx
+++ b/data/tech_guidance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/robert_miller_education_gov_uk/Documents/Documents/R/la-school-places-scorecard-internal/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\shenetapp01\Pupil Place Planning\Scorecards\Scorecards 2024\Combined years\technical guidance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="8_{88D981E4-01D0-41D1-BFE9-9F41107BE635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{364AACDB-AEE9-4581-B73A-D53239F4F61E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E79E806B-0C3D-4EA2-98AE-858B85EF11E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{9CCC1F63-2262-45DD-B4CA-7C937E5C8E7F}"/>
+    <workbookView xWindow="-38520" yWindow="-5355" windowWidth="38640" windowHeight="21120" xr2:uid="{9CCC1F63-2262-45DD-B4CA-7C937E5C8E7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Quantity" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="183">
   <si>
     <t>Notes</t>
   </si>
@@ -145,6 +145,9 @@
     <t>Places created since 2009/10</t>
   </si>
   <si>
+    <t>Local authority data provided through the School Capacity (SCAP) Collection 2021</t>
+  </si>
+  <si>
     <t>School census Jan 2010 data</t>
   </si>
   <si>
@@ -155,6 +158,13 @@
     <t>Percentage of new places created in good and outstanding schools</t>
   </si>
   <si>
+    <t>Ranks local authorities on their proportion of new school places which are in good and outstanding schools</t>
+  </si>
+  <si>
+    <t>1. Ranking of proportions of new places created in 'good' or 'outstanding' schools for each local authority, amongst all local authorities with new places. Local authorities with the same proportion are given an equal ranking. Ranking is only applied to local authorities where new places have been created.
+&lt;br&gt;2. The higher the rank the higher the proportion of new school places in good and outstanding schools compared to other local authorities. &lt;br&gt;3. Ranks can be tied and there will many local authorities with a rank of 1 due to 100% of new places in good and outstanding schools.</t>
+  </si>
+  <si>
     <t xml:space="preserve">The national average cost per place of permanent expansion, temporary expansion and new school projects in England. </t>
   </si>
   <si>
@@ -168,6 +178,18 @@
     <t>2. Capacity changes through the CIF, SRP, SSEF, VA.</t>
   </si>
   <si>
+    <t>School place offers by preference for September 2023 entry</t>
+  </si>
+  <si>
+    <t>The proportion of applicants who received an offer of a place in one of their top three preference schools for September 2023 on national offer day</t>
+  </si>
+  <si>
+    <t>Published School Applications and Offer data 2023/24 Academic Year</t>
+  </si>
+  <si>
+    <t>Local authority data, provided through School Capacity collection 2022</t>
+  </si>
+  <si>
     <t>Unfilled places as a percentage of total places</t>
   </si>
   <si>
@@ -175,12 +197,180 @@
 </t>
   </si>
   <si>
+    <t>5. Total number of planned places (sum of 1, 2, 3, 4 and 5 above)</t>
+  </si>
+  <si>
     <t xml:space="preserve">1. Number of pupils in roll in January 2010, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. </t>
   </si>
   <si>
     <t>1. This relates to the difference between number of pupils on roll and capacity, in schools where the number on roll is lower than a school's reported capacity. &lt;br&gt;2. Calculated at school level and aggregated to local authority level.</t>
   </si>
   <si>
+    <t>Total places created between May 2010 and May 2023</t>
+  </si>
+  <si>
+    <t>2.Capacity at May 2023</t>
+  </si>
+  <si>
+    <t>1. The number of places that have been created since May 2010 in each local authority is taken as the difference between capacity as reported by local authorities, via SCAP, at May 2010 and May 2023.
+&lt;br&gt;2. The measure includes all primary and middle deemed primary school capacity in the primary phase, and all secondary, middle deemed secondary and all-through school capacity in the secondary phase.
+&lt;br&gt;3. The measure reports net increase in places only, if phase capacity in a local authority has reduced between May 2010 and May 2023, this is recorded as zero places created. Therefore the sum of the local authority-level figures will not equal the overall increase in places at national level.</t>
+  </si>
+  <si>
+    <t>Places planned to 2025/26</t>
+  </si>
+  <si>
+    <t>1. Local authority plans for places to be created or removed between May 2023 and before the start of the 2025/26 academic year.</t>
+  </si>
+  <si>
+    <t>Local authority data provided through the School Capacity (SCAP) Survey 2023.</t>
+  </si>
+  <si>
+    <t>Local authority data provided through School Capacity (SCAP) Survey 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Local authority data about new permanent additional places, new temporary bulge places (to accommodate large cohorts as they move through the school) and permanent places to remove  2023/24, 2024/25  and 2025/26 is aggregated to local authority level.
+&lt;br&gt;2. The data was provided by local authorities in May 2023, and only includes projects they were confident would proceed. Local authorities were asked to include the total places of any new provision, even if spaces would fill gradually. 
+&lt;br&gt;3. Local authorities were asked not to include places created through free schools unless they were providing the funding for additional places themselves. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Changes to school capacity (both increases and decreases) as a consequence of works delivered through the CIF, SRP, SSEF, VA between 2023/24 and 2025/26 inclusive, aggregated to local authority level. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. The calculation mirrors the approach taken for basic need funding allocations published in March 2024. It includes mainstream primary and secondary free schools which opened in September 2023 and those with a high degree of certainty of opening in September 2024, and counts the total number of places which will be in use by September 2025.
+&lt;br&gt;2. The data does not include free schools which opened before September 2023, as they will already be included in SCAP23 and are therefore existing places. It does not include free schools which are planned to open in the academic year 2025/26 and beyond. </t>
+  </si>
+  <si>
+    <t>3. Places from free schools opened in September 2023 and due to be opened in September 2024.</t>
+  </si>
+  <si>
+    <t>4. Reduction in places from free school and academy closures between May 2023 and January 2024 or identified/confirmed to close before August 2024.</t>
+  </si>
+  <si>
+    <t>1. Where an academy or free school closed after 1 May 2023 its capacity, as reported in the School Capacity data, is now no longer available. Their capacity has therefore been removed from the planned delivery total.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. This measure reports planned increases in capacity only. If there is a total net planned reduction in capacity (e.g. due to a free school closure), this is shown as zero places planned. Therefore the sum of local authority-level figures will not equal the national planned places figure.
+&lt;br&gt;2. Most local authorities will have further developed their plans since this data was reported in Summer 2023, and so although it allows for comparisons between local authorities, the figure is likely to be an understatement of the current position. </t>
+  </si>
+  <si>
+    <t>Unfilled places in 2022/23</t>
+  </si>
+  <si>
+    <t>Additional places needed in 2025/26; spare places in 2025/26</t>
+  </si>
+  <si>
+    <t>Estimated number of additional places needed to meet demand in 2025/26; estimated percentage of spare places in 2025/26.</t>
+  </si>
+  <si>
+    <t>1.This relates to the academic year 2025/26 and is the difference between local authority pupil forecasts and future capacity, taking account of planned future additions and places to remove.
+     places needed = forecast demand - (existing capacity + additional capacity - places to remove).  
+For further information on the methodology used, see the School Place Planning 2023: technical note found on the School Capacity 23 publication on Explore Education Statistics.
+&lt;br&gt;2. Where demand is greater than capacity a need for additional places results; where capacity is greater than demand spare places result. 
+&lt;br&gt;3. Local authority pupil forecasts for 2025/26 are collected through SCAP 2023&lt;br&gt;4. Additional capacity as at 2025/26 includes places that the local authority plans to add or remove between May 2023 and before the start of the 2025/26 academic year and places from programmes centrally funded by the department, as described above. 
+&lt;br&gt;5. The comparison of demand and capacity takes place for each national curriculum year group within each planning area to estimate places needed in each. The estimates in the scorecard do not allow for spare capacity in one year group or planning area to be off-set against need in another, or vice-versa. This avoids the risk of spare places in one or more planning areas masking areas of need for additional places in planning areas elsewhere in the local authority. For further information see the School Place Planning Tables 2023: technical note.
+&lt;br&gt;6. The estimated need for additional places and estimated spare places is calculated at planning area level and then aggregated to local authority level. It is common for a local authority to have both a need for additional places and spare places, reflecting pockets of localised need for places or pockets of localised spare places.
+&lt;br&gt;7. Estimates for need are rounded to the nearest 10.
+&lt;br&gt;8. Estimates for spare places are presented as a percentage of total future capacity.</t>
+  </si>
+  <si>
+    <t>Total basic need funding 2011 to 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total amount of basic need capital funding allocated to each local authority to support them to create new mainstream primary and secondary places from 2011 to 2025. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. This refers to the amount of basic need capital funding that the Department for Education (DfE) has allocated to each local authority to create new places from the 2011-12 financial year to the 2024-25 financial year. Basic Need funding for the 2024-25 financial year is intended to support the creation of mainstream places for pupils aged 5 to 16 for the 2025/26 academic year. &lt;br&gt;2. The figure includes formula-based funding allocations and funding provided through the Targeted Basic Need Programme. Basic Need formula-based funding allocations cover the whole period and are not ring-fenced (although they can only be used for capital purposes).  Targeted Basic Need funding was provided between 2013 and 2015 and had to be spent by agreed deadlines and on specific projects. Both types of allocations are published here. &lt;br&gt;3. The figure only includes funding allocated to local authorities and does not include centrally-funded capital programmes such as the free schools programme. &lt;br&gt;4. The England total will not match the sum of allocations for all local authorities in the scorecard because the England total includes allocations to predecessor local authorities.
+</t>
+  </si>
+  <si>
+    <t>The actual percentage change in pupil numbers between 2009/10 and 2023/24; the anticipated percentage change in pupil numbers in primary or secondary state-funded mainstream provision between the 2023/24 and 2025/26 academic years.</t>
+  </si>
+  <si>
+    <t>Change in pupil numbers
+2009/10 to 2023/24; Anticipated change in pupil numbers 2023/24 to 2025/26</t>
+  </si>
+  <si>
+    <t>2. Pupil Numbers for the 2023/24 academic year taken from the pupil census in January 2024</t>
+  </si>
+  <si>
+    <t>School census Jan 2024 data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Number of pupils in roll in January 2024, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. 							</t>
+  </si>
+  <si>
+    <t>2. Forecast pupil numbers for the 2025/26 academic year</t>
+  </si>
+  <si>
+    <t>Local authority data provided through the  School Capacity (SCAP) Collection 2023</t>
+  </si>
+  <si>
+    <t>1. This is the local authority's forecast of pupil numbers for the academic year 2025/26 as provided in SCAP 2023.
+2. These forecasts cover pupils that local authorities anticipate will attend primary schools (or primary provision in middle or all-through schools i.e. years R-6) and secondary schools (or secondary provision in middle or all-through schools i.e. years 7-11)
+3. These forecasts focus on local authorities expectations about new school places and do not include pupils who are expected to attend independent schools or special/non-mainstream provision.</t>
+  </si>
+  <si>
+    <t>Forecast accuracy of pupil projections for 2023/24</t>
+  </si>
+  <si>
+    <t>The one year ahead local authority forecast accuracy. It compares actual numbers on roll in 2023/24 with forecasts of pupil numbers for 2023/24 made one year previously (in SCAP 2023)</t>
+  </si>
+  <si>
+    <t>1. Forecasts of academic year 2023/24 pupil numbers made in 2022/23.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Actual pupil numbers on roll in academic year 2023/24.
+</t>
+  </si>
+  <si>
+    <t>Local authority data provided through the School Capacity (SCAP) Collection 2023</t>
+  </si>
+  <si>
+    <t>Pupils in school provided through the January 2024 School Census</t>
+  </si>
+  <si>
+    <t>1. Forecasts, submitted by local authorities for SCAP23 , at planning area level and aggregated to local authority level. Forecasts include pupils expected to be educated in new schools (or expanded schools) funded through Housing Developer Contributions (HDC) and Housing Infrastructure Fund (HIF) agreements.
+&lt;br&gt;2. Actual pupil numbers on roll for academic year 2023/24 are taken from the January school census and aggregated to local authority level. They include pupils in roll, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. &lt;br&gt;3. Forecast accuracy is calculated by  subtracting the years R-6 actual numbers from the years R-6 forecasts to give the absolute inaccuracy. Absolute inaccuracy is then divided by the R-6 actual number to give the relative percentage inaccuracy. The same is done for secondary using years 7-11. 
+&lt;br&gt;4.  Scorecard figures may differ to those published in SCAP due to the exclusion of years 12 to 14 in the pupil numbers and forecasts used in the scorecard.</t>
+  </si>
+  <si>
+    <t>The three year ahead forecast accuracy compares actual pupil numbers on roll with forecasts of pupil numbers for 2023/24 made two years previously (in SCAP 2021) by local authority).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Forecasts of academic year 2023/24 pupil numbers made in 2020/21.
+</t>
+  </si>
+  <si>
+    <t>2. Actual pupil numbers on roll in academic year 2023/24.</t>
+  </si>
+  <si>
+    <r>
+      <t>1. Forecasts, submitted by local authorities</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>as part of the SCAP 2021, at planning area level and aggregated to local authority level. Forecasts include pupils expected to be educated in new schools (or expanded schools) funded through HDC and HIF agreements.
+&lt;br&gt;2. Actual pupil numbers on roll for academic year 2023/24 are taken from the January school census and aggregated to local authority level. They include pupils in roll, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. 	&lt;br&gt;3. Forecast accuracy is calculated by subtracting the years R-6 actual numbers from the years R-6 forecasts to give the absolute inaccuracy. Absolute inaccuracy is then divided by the R-6 actual number to give the relative percentage inaccuracy. The same is done for secondary using years 7-11. 
+&lt;br&gt;4.  Scorecard figures may differ to those published in SCAP due to the exclusion of years 12 to 14 in the pupil numbers and forecasts used in the scorecard.</t>
+    </r>
+  </si>
+  <si>
     <t>School place offers by preference for September 2024 entry</t>
   </si>
   <si>
@@ -190,236 +380,105 @@
     <t>Published School Applications and Offer data 2024/25 Academic Year</t>
   </si>
   <si>
+    <t>Quality of new school places created between academic year 2021/22 and 2022/23, based on Ofsted rating</t>
+  </si>
+  <si>
+    <t>The number of new places created between academic year 2021/22 and academic year 2022/23</t>
+  </si>
+  <si>
+    <t>Capacity of each school in May 2022</t>
+  </si>
+  <si>
+    <t>1. The following school types, identified using Get Information About Schools, have been excluded:
+&lt;br&gt;- former independent schools which have not had an inspection since opening;
+&lt;br&gt;- sponsored academies which have not had an Ofsted inspection since opening as an academy.
+&lt;br&gt;- schools that have amalgamated and have not been inspected since amalgamation.
+&lt;br&gt;2.The capacity of schools present in May 2023 is compared with May 2022 capacity.
+&lt;br&gt;3. New places are identified as an increase in school capacity of 30 places or more between May 2022 and May 2023 at each school. For mergers and academy conversions where 2022 capacity is not available, the capacities of the ‘parent’ schools in 2022 have been used.
+&lt;br&gt;4. Schools where fewer than 30 places have been created between May 2022 and May 2023 have all of their capacity counted as existing places.
+&lt;br&gt;5. Existing places are the number of places present in May 2023 after subtracting the new places since May 2022 (if 30 or more) from the May 2022 capacity.
+&lt;br&gt;6. Primary places are based on primary capacity and secondary places are based on secondary capacity reported in May 2022 or 2023. 
+&lt;br&gt;7. New places in schools which had not had an Ofsted judgment or key stage 2 or 4 result by August 2023 have been excluded from the relevant version of the measure. These places are included in the figure beneath the chart.
+&lt;br&gt;8. Because any decreases in capacity are not factored, the number of places added for use in the quality measure may not be the same as the number of places added in the quantity measure.
+&lt;br&gt;9. From June 2019 the Ofsted grades of academy predecessor schools were factored into their data, even though it may have been some time since those schools converted and/or were inspected. 
+&lt;br&gt;10. The quality measures represent the window in time when places were added and this is not necessarily the same quality outcome as when the decision to add places was taken.</t>
+  </si>
+  <si>
+    <t>Capacity for each school in May 2023</t>
+  </si>
+  <si>
     <t>Local authority data, provided through School Capacity collection 2023</t>
   </si>
   <si>
+    <t>Percentage of new places created in good and outstanding schools between academic year 2021/22 and academic year 2022/23.</t>
+  </si>
+  <si>
+    <t>Quality of new school places created between academic year 2021/22 and 2022/23, based on key stage 2 progress measures</t>
+  </si>
+  <si>
     <t>Performance tables</t>
   </si>
   <si>
     <t>Key stage 2 progress measures</t>
   </si>
   <si>
+    <t xml:space="preserve">1. Each school has been matched with the key stage 2 progress measure for reading and maths, for academic year ending July 2023 (published December 2023).
+2. This measure judges schools’ performance as 'well above average', 'above average', 'average', 'below average' or 'well below average'.
+3. The calculation counts the number of new school places that have been created in schools of each category; and the number of existing school places in each category.
+4. Middle schools may not have a key stage 2 measure and if they do, due to the age range of pupils at middle schools, pupils will have only attended a middle school for a short time before they take their key stage 2 tests and will still have a number of years left at the school. This should be taken into account when comparing their results to schools which start educating their pupils from the beginning of key stage 1.  New schools may not have a key stage 2 measure until the first cohort of pupils reaches year 6.
+5. For further information on key stage 2 progress measures please use the following url: https://www.gov.uk/government/collections/school-performance-tables-about-the-data </t>
+  </si>
+  <si>
+    <t>The quality of school places created between academic year 2021/22 and academic year 2022/23, and the quality of existing school places. Based on key stage 2 progress measures</t>
+  </si>
+  <si>
+    <t>The quality of school places created between academic year 2021/22 and academic year 2022/23, and the quality of existing school places. Based on key stage 4 progress 8 measure</t>
+  </si>
+  <si>
+    <t>Quality of new school places created between academic year 2021/22 and 2022/23, based on key stage 4 progress 8 measure</t>
+  </si>
+  <si>
     <t>Key stage 4 progress 8 measure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LA Rank- key stage 2 measures
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LA Rank- key stage 4 progress 8 measure
+</t>
+  </si>
+  <si>
+    <t>Ranks local authorities on their proportion of new school places of new school places created in well above- and above-average schools</t>
   </si>
   <si>
     <t>1. Ranking of proportions of new places created in 'well above average' and 'above average' schools for each local authority, amongst all local authorities with new places. Local authorities with the same proportion are given an equal ranking. Ranking is only applied to local authorities where new places have been created.
 2. The higher the rank the higher the proportion of new school places in well above and above average schools compared to other local authorities.</t>
   </si>
   <si>
+    <t>Percentage of new places created in well above and above-average schools between academic year 2021/22 and academic year 2022/23.</t>
+  </si>
+  <si>
     <t>1. Ranking of proportions of new places created in 'well above average' and 'above average' schools for each local authority, amongst all local authorities with new places. Local authorities with the same proportion are given an equal ranking. Ranking is only applied to local authorities where new places have been created. 
 2. The higher the rank the higher the proportion of new school places in well above and above average schools compared to other local authorities.</t>
   </si>
   <si>
-    <t xml:space="preserve">DfE internal model. Additional places needed are published in the school place planning published underlying data. </t>
-  </si>
-  <si>
-    <t>Percentage of  new school places in well above and above-average schools- key stage 2 measures</t>
-  </si>
-  <si>
-    <t>Percentage of  new school places in well above and above-average schools- key stage 4 progress 8 measure</t>
-  </si>
-  <si>
-    <t>Total places created between May 2010 and May 2024</t>
-  </si>
-  <si>
-    <t>2.Capacity at May 2024</t>
-  </si>
-  <si>
-    <t>Local authority data provided through School Capacity (SCAP) Survey 2024</t>
-  </si>
-  <si>
-    <t>1. The number of places that have been created since May 2010 in each local authority is taken as the difference between capacity as reported by local authorities, via SCAP, at May 2010 and May 2024.
-&lt;br&gt;2. The measure includes all primary and middle deemed primary school capacity in the primary phase, and all secondary, middle deemed secondary and all-through school capacity in the secondary phase.
-&lt;br&gt;3. The measure reports net increase in places only, if phase capacity in a local authority has reduced between May 2010 and May 2024, this is recorded as zero places created. Therefore the sum of the local authority-level figures will not equal the overall increase in places at national level.</t>
-  </si>
-  <si>
-    <t>Number of new places planned for delivery between May 2024 and September 2026;
+    <t>Number of new places planned for delivery between May 2023 and September 2025;
 &lt;br&gt;This contains: 
 &lt;br&gt;1) local authority firm plans for new permanent additional places , new temporary bulge places and the removal of places,
 &lt;br&gt;2) capacity changes through the Condition Improvement Fund (CIF), School Rebuilding Programme (SRP), Selective Schools Expansion Fund (SSEF), and Voluntary Aided Schools Fund (VA)
-&lt;br&gt;3) places from free schools opened in September 2024 and planned to open in September 2025
+&lt;br&gt;3) places from free schools opened in September 2023 and planned to open in September 2024
 &lt;br&gt;4) reduction in places from free school and academy closures.</t>
   </si>
   <si>
-    <t>1. Local authority plans for places to be created or removed between May 2024 and before the start of the 2026/27 academic year.</t>
-  </si>
-  <si>
-    <t>3. Places from free schools opened in September 2024 and due to be opened in September 2025.</t>
-  </si>
-  <si>
-    <t>4. Reduction in places from free school and academy closures between May 2024 and January 2025 or identified/confirmed to close before August 2025.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Local authority data about new permanent additional places, new temporary bulge places (to accommodate large cohorts as they move through the school) and permanent places to remove  2024/25, 2025/26  and 2026/27 is aggregated to local authority level.
-&lt;br&gt;2. The data was provided by local authorities in May 2024, and only includes projects they were confident would proceed. Local authorities were asked to include the total places of any new provision, even if spaces would fill gradually. 
-&lt;br&gt;3. Local authorities were asked not to include places created through free schools unless they were providing the funding for additional places themselves. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Changes to school capacity (both increases and decreases) as a consequence of works delivered through the CIF, SRP, SSEF, VA between 2024/25 and 2026/27 inclusive, aggregated to local authority level. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. The calculation mirrors the approach taken for basic need funding allocations published in March 2025. It includes mainstream primary and secondary free schools which opened in September 2024 and those with a high degree of certainty of opening in September 2025, and counts the total number of places which will be in use by September 2026.
-&lt;br&gt;2. The data does not include free schools which opened before September 2024, as they will already be included in SCAP24 and are therefore existing places. It does not include free schools which are planned to open in the academic year 2026/27 and beyond. </t>
-  </si>
-  <si>
-    <t>1. Where an academy or free school closed after 1 May 2024 its capacity, as reported in the School Capacity data, is now no longer available. Their capacity has therefore been removed from the planned delivery total.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. This measure reports planned increases in capacity only. If there is a total net planned reduction in capacity (e.g. due to a free school closure), this is shown as zero places planned. Therefore the sum of local authority-level figures will not equal the national planned places figure.
-&lt;br&gt;2. Most local authorities will have further developed their plans since this data was reported in Summer 2024, and so although it allows for comparisons between local authorities, the figure is likely to be an understatement of the current position. </t>
-  </si>
-  <si>
-    <t>Places planned to 2026/27</t>
-  </si>
-  <si>
-    <t>Unfilled places in 2023/24</t>
-  </si>
-  <si>
-    <t>Additional places needed in 2026/27; spare places in 2026/27</t>
-  </si>
-  <si>
-    <t>Estimated number of additional places needed to meet demand in 2026/27; estimated percentage of spare places in 2026/27.</t>
-  </si>
-  <si>
-    <t>Total basic need funding 2011 to 2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total amount of basic need capital funding allocated to each local authority to support them to create new mainstream primary and secondary places from 2011 to 2026. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. This refers to the amount of basic need capital funding that the Department for Education (DfE) has allocated to each local authority to create new places from the 2011-12 financial year to the 2025-26 financial year. Basic Need funding for the 2025-26 financial year is intended to support the creation of mainstream places for pupils aged 5 to 16 for the 2026/27 academic year. &lt;br&gt;2. The figure includes formula-based funding allocations and funding provided through the Targeted Basic Need Programme. Basic Need formula-based funding allocations cover the whole period and are not ring-fenced (although they can only be used for capital purposes).  Targeted Basic Need funding was provided between 2013 and 2015 and had to be spent by agreed deadlines and on specific projects. Both types of allocations are published here. &lt;br&gt;3. The figure only includes funding allocated to local authorities and does not include centrally-funded capital programmes such as the free schools programme. &lt;br&gt;4. The England total will not match the sum of allocations for all local authorities in the scorecard because the England total includes allocations to predecessor local authorities.
+    <t xml:space="preserve">DfE internal model. Additional places needed are published in the school place planning published underlying data. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LA Rank- Ofsted
 </t>
   </si>
   <si>
-    <t>Change in pupil numbers
-2009/10 to 2024/25; Anticipated change in pupil numbers 2024/25 to 2026/27</t>
-  </si>
-  <si>
-    <t>School census Jan 2025 data</t>
-  </si>
-  <si>
-    <t>Local authority data provided through the  School Capacity (SCAP) Collection 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Number of pupils in roll in January 2025, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. 							</t>
-  </si>
-  <si>
-    <t>1. This is the local authority's forecast of pupil numbers for the academic year 2026/27 as provided in SCAP 2024.
-2. These forecasts cover pupils that local authorities anticipate will attend primary schools (or primary provision in middle or all-through schools i.e. years R-6) and secondary schools (or secondary provision in middle or all-through schools i.e. years 7-11)
-3. These forecasts focus on local authorities expectations about new school places and do not include pupils who are expected to attend independent schools or special/non-mainstream provision.</t>
-  </si>
-  <si>
-    <t>Forecast accuracy of pupil projections for 2024/25</t>
-  </si>
-  <si>
-    <t>The one year ahead local authority forecast accuracy. It compares actual numbers on roll in 2024/25 with forecasts of pupil numbers for 2024/25 made one year previously (in SCAP 2024)</t>
-  </si>
-  <si>
-    <t>The three year ahead forecast accuracy compares actual pupil numbers on roll with forecasts of pupil numbers for 2024/25 made three years previously (in SCAP 2022) by local authority).</t>
-  </si>
-  <si>
-    <t>1. Forecasts of academic year 2024/25 pupil numbers made in 2023/24.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. Actual pupil numbers on roll in academic year 2024/25.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Forecasts of academic year 2024/25 pupil numbers made in 2021/22.
-</t>
-  </si>
-  <si>
-    <t>2. Actual pupil numbers on roll in academic year 2024/25.</t>
-  </si>
-  <si>
-    <t>Local authority data provided through the School Capacity (SCAP) Collection 2024</t>
-  </si>
-  <si>
-    <t>Pupils in school provided through the January 2025 School Census</t>
-  </si>
-  <si>
-    <t>Local authority data provided through the School Capacity (SCAP) Collection 2022</t>
-  </si>
-  <si>
-    <t>1. Forecasts, submitted by local authorities for SCAP24 , at planning area level and aggregated to local authority level. Forecasts include pupils expected to be educated in new schools (or expanded schools) funded through Housing Developer Contributions (HDC) and Housing Infrastructure Fund (HIF) agreements.
-&lt;br&gt;2. Actual pupil numbers on roll for academic year 2024/25 are taken from the January school census and aggregated to local authority level. They include pupils in roll, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. &lt;br&gt;3. Forecast accuracy is calculated by  subtracting the years R-6 actual numbers from the years R-6 forecasts to give the absolute inaccuracy. Absolute inaccuracy is then divided by the R-6 actual number to give the relative percentage inaccuracy. The same is done for secondary using years 7-11. 
-&lt;br&gt;4.  Scorecard figures may differ to those published in SCAP due to the exclusion of years 12 to 14 in the pupil numbers and forecasts used in the scorecard.</t>
-  </si>
-  <si>
-    <r>
-      <t>1. Forecasts, submitted by local authorities</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>as part of the SCAP 2022, at planning area level and aggregated to local authority level. Forecasts include pupils expected to be educated in new schools (or expanded schools) funded through HDC and HIF agreements.
-&lt;br&gt;2. Actual pupil numbers on roll for academic year 2024/25 are taken from the January school census and aggregated to local authority level. They include pupils in roll, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. 	&lt;br&gt;3. Forecast accuracy is calculated by subtracting the years R-6 actual numbers from the years R-6 forecasts to give the absolute inaccuracy. Absolute inaccuracy is then divided by the R-6 actual number to give the relative percentage inaccuracy. The same is done for secondary using years 7-11. 
-&lt;br&gt;4.  Scorecard figures may differ to those published in SCAP due to the exclusion of years 12 to 14 in the pupil numbers and forecasts used in the scorecard.</t>
-    </r>
-  </si>
-  <si>
-    <t>School place offers by preference for September 2025 entry</t>
-  </si>
-  <si>
-    <t>The proportion of applicants who received an offer of a place in one of their top three preference schools for September 2025 on national offer day</t>
-  </si>
-  <si>
-    <t>Published School Applications and Offer data 2025/26 Academic Year</t>
-  </si>
-  <si>
-    <t>Quality of new school places created between academic year 2022/23 and 2023/24, based on Ofsted rating</t>
-  </si>
-  <si>
-    <t>The number of new places created between academic year 2022/23 and academic year 2023/24</t>
-  </si>
-  <si>
-    <t>Capacity of each school in May 2023</t>
-  </si>
-  <si>
-    <t>Capacity for each school in May 2024</t>
-  </si>
-  <si>
-    <t>Local authority data, provided through School Capacity collection 2024</t>
-  </si>
-  <si>
-    <t>Quality of school places created between academic year 2022/23 and academic year 2023/24, based on Ofsted rating. The quality of existing school places (places in 2023/24 which were also present in 2022/23) is shown for context.</t>
-  </si>
-  <si>
-    <t>1. Each school has been matched with the Ofsted judgement of 'Overall effectiveness: how good is the school." as at 31 August 2024 (published November 2024).
-&lt;br&gt;2. There are four Ofsted categories: 'Outstanding', 'Good', 'Requires improvement' and 'Inadequate'.
-&lt;br&gt;3. The calculation counts the number of existing and new places that have been created in schools of each category. &lt;br&gt;4. Note that many schools will have been inspected some time before August 2024, and some will have been inspected since this date. &lt;br&gt;5. There are school places with no rating, as the school has yet to be inspected so do not have an Ofsted judgement.</t>
-  </si>
-  <si>
-    <t>Percentage of new places created in good and outstanding schools between academic year 2022/23 and academic year 2023/24.</t>
-  </si>
-  <si>
-    <t>The quality of school places created between academic year 2022/23 and academic year 2023/24, and the quality of existing school places. Based on key stage 2 progress measures</t>
-  </si>
-  <si>
-    <t>Quality of new school places created between academic year 2022/23 and 2023/24, based on key stage 2 progress measures</t>
-  </si>
-  <si>
-    <t>The quality of school places created between academic year 2022/23 and academic year 2023/24, and the quality of existing school places. Based on key stage 4 progress 8 measure</t>
-  </si>
-  <si>
-    <t>Quality of new school places created between academic year 2022/23 and 2023/24, based on key stage 4 progress 8 measure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Each school has been matched with the key stage 4 progress 8 measure across 8 key subjects, for academic year ending July 2024 (published February 2025).
+    <t xml:space="preserve">1. Each school has been matched with the key stage 4 progress 8 measure across 8 key subjects, for academic year ending July 2023 (published February 2024).
 2. This measure judges schools’ performance as 'well above average', 'above average', 'average', 'below average' or 'well below average'.
 3. The calculation counts the number of new school places that have been created in schools of each category; and the number of existing school places in each category.
 4. Note that middle schools will not have a key stage 4 measure, and that new schools may not have a key stage 4 measure until the first cohort of pupils reaches year 11.
@@ -428,41 +487,246 @@
 </t>
   </si>
   <si>
-    <t>Percentage of new places created in well above and above-average schools between academic year 2022/23 and academic year 2023/24.</t>
+    <t>Percentage of  new school places in well above and above-average schools- key stage 2 measures</t>
+  </si>
+  <si>
+    <t>Percentage of  new school places in well above and above-average schools- key stage 4 progress 8 measure</t>
+  </si>
+  <si>
+    <t>Quality of school places created between academic year 2021/22 and academic year 2022/23, based on Ofsted rating. The quality of existing school places (places in 2022/23 which were also present in 2021/22) is shown for context.</t>
+  </si>
+  <si>
+    <t>1. Each school has been matched with the Ofsted judgement of 'Overall effectiveness: how good is the school." as at 31 August 2023 (published November 2023).
+&lt;br&gt;2. There are four Ofsted categories: 'Outstanding', 'Good', 'Requires improvement' and 'Inadequate'.
+&lt;br&gt;3. The calculation counts the number of existing and new places that have been created in schools of each category. &lt;br&gt;4. Note that many schools will have been inspected some time before August 2023, and some will have been inspected since this date. &lt;br&gt;5. There are school places with no rating, as the school has yet to be inspected so do not have an Ofsted judgement.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The national average has been adjusted to the relevant region for each local authority, using the Building Cost Information Service (BCIS) March 2024 published regional location factors. The England national average has been multiplied by the relevant regional location factor:  East Midlands: 1.03, East of England 0.99, Inner London: 1.29, North East: 0.91, North West: 1, Outer London: 1.21, South East: 1.13, South West: 1.01, West Midlands: 0.96, Yorkshire &amp; the Humber: 0.91. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. The cost data used in the scorecard is the 2018 Capital Spend data as used in the 2018, 2019 and 2021 Scorecards. For the 2023 Scorecard, this data has been adjusted for inflation (rebased to 1st Quarter 2024 prices). National averages adjusted for 2023 regional location factors are shown. </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">You can use this data to establish developer contributions per school place, by adjusting for further inflation if needed </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(see examples below).
+&lt;br&gt;2. Projects which do not create additional mainstream places or where the project's additional place funding is zero are removed.
+&lt;br&gt;3. Projects were identified as primary  or secondary phase based on additional mainstream place year group breakdown. Where a project created places across both phases, it was assigned a phase corresponding to the phase of the school it affected (i.e. if its school was middle-deemed primary - the project was assigned to primary).
+&lt;br&gt;4. Average cost per place figures for all-through, middle-deemed primary and middle-deemed secondary schools have not been calculated separately due to low sample sizes for these project types. </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>To estimate average cost per place for middle-deemed primary schools, we recommend using primary average cost per place</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> as the middle school provides education equivalent to the education a primary school provides for all year groups. </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>To estimate average cost per place for middle-deemed secondary schools, we recommend using secondary average cost per place</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for the same reason. </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>For new middle schools or whole school expansions for middle schools not ‘deemed’ primary or secondary, we recommend taking a mid-point of the primary and secondary costs if the project covers both primary- and secondary-equivalent year groups equally</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (e.g. 2 classes per Year 5 &amp; 6 and 2 classes per Year 7 &amp; 8). </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If the project only covers certain year groups, we recommend using primary cost data if only primary-equivalent years groups are expanding</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (e.g. Years 5 &amp; 6) and </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>secondary data if only secondary-equivalent year groups are expanding</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (e.g. Years 7 &amp; 8).
+&lt;br&gt;5. The average cost does not include costs associated with land acquisition.
+&lt;br&gt;6. The average cost includes costs associated with maintenance and building condition or enhancement works.
+&lt;br&gt;7. The measure does not include places in special schools or units attached to mainstream schools, or new places which were funded through central programmes (including free schools). Where a project creates additional mainstream places and also creates SEN places or re-provides places, an adjustment has been applied to apportion out those costs. 
+&lt;br&gt;8. All costs have been normalised to a common UK average price level using regional location factors published by BCIS, March 2024, 1 is the base weight.
+&lt;br&gt;9. All costs have been adjusted for inflation using the latest BCIS All-In Tender Price of Index (TPI), published March 2024.  Costs have been rebased from the start of construction (or time of place provision if construction start date unavailable) to 1st Quarter (Jan – Mar) 2024 prices using this index (Q1 2024 index value = 390).
+10. </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>To adjust the national average to current or future prices, you need to uprate or downrate the prices in this scorecard relative to the change that has happened since Q1 2024</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.  If you have access to the BCIS indices via a subscription to BCIS Online (https://www.rics.org/uk/products/data-products/bcis-construction/bcis-online/) you can use the latest inflation index to re-base (weight to apply = latest index/390).  If not, you can apply a known change to the published cost (e.g. up or down x%).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Example: New primary school in Outer London Q3 (Jul - Sep) 2024.  
+National average for primary new school place = £23,865. 
+Outer London location factor = 1.21 (taken from published BCIS regional location factors March 2023)
+Inflation weight = 394/390 = 1.01 ( taken from BCIS All-In TPI published March 2023). 
+Average primary New School place cost that applies to Outer London in Q3 2023 prices = £23,192 x 1.21 x 1.01 = £29,200 (rounded to nearest £100).  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+If you do not have access the BCIS index, but sources say TPI inflation is set to increase by 4% per annum, then approximate inflation weight = 6% (18 months’ worth of inflation) = 1.06.
+11. Some additional but limited benchmark information for similar capital programme schemes carried out by the DfE is available in the National School Delivery Cost Benchmarking study: https://documents.hants.gov.uk/property-services/NationalSchoolDeliveryBenchmarkingreport.pdf</t>
+    </r>
+  </si>
+  <si>
+    <t>Publication</t>
+  </si>
+  <si>
+    <t>2022/23</t>
+  </si>
+  <si>
+    <t>1. The number of places that have been created since May 2010 in each local authority is taken as the difference between capacity as reported by local authorities, via SCAP, at May 2010 and May 2024.
+&lt;br&gt;2. The measure includes all primary and middle deemed primary school capacity in the primary phase, and all secondary, middle deemed secondary and all-through school capacity in the secondary phase.
+&lt;br&gt;3. The measure reports net increase in places only, if phase capacity in a local authority has reduced between May 2010 and May 2024, this is recorded as zero places created. Therefore the sum of the local authority-level figures will not equal the overall increase in places at national level.</t>
+  </si>
+  <si>
+    <t>2.Capacity at May 2024</t>
+  </si>
+  <si>
+    <t>Local authority data provided through School Capacity (SCAP) Survey 2024</t>
+  </si>
+  <si>
+    <t>1. Local authority plans for places to be created or removed between May 2024 and before the start of the 2026/27 academic year.</t>
   </si>
   <si>
     <t>Local authority data provided through the School Capacity (SCAP) Survey 2024.</t>
   </si>
   <si>
-    <t>The actual percentage change in pupil numbers between 2009/10, 2014/15 (for secondary), 2018/19 (for primary) and 2024/25; the anticipated percentage change in pupil numbers in primary or secondary state-funded mainstream provision between the 2024/25 and 2026/27 academic years.</t>
-  </si>
-  <si>
-    <t>School census Jan 2015 data</t>
-  </si>
-  <si>
-    <t>School census Jan 2019 data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Number of pupils in roll in January 2015, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Number of pupils in roll in January 2019, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. </t>
+    <t xml:space="preserve">1. Local authority data about new permanent additional places, new temporary bulge places (to accommodate large cohorts as they move through the school) and permanent places to remove  2024/25, 2025/26  and 2026/27 is aggregated to local authority level.
+&lt;br&gt;2. The data was provided by local authorities in May 2024, and only includes projects they were confident would proceed. Local authorities were asked to include the total places of any new provision, even if spaces would fill gradually. 
+&lt;br&gt;3. Local authorities were asked not to include places created through free schools unless they were providing the funding for additional places themselves. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Changes to school capacity (both increases and decreases) as a consequence of works delivered through the CIF, SRP, SSEF, VA between 2024/25 and 2026/27 inclusive, aggregated to local authority level. </t>
+  </si>
+  <si>
+    <t>3. Places from free schools opened in September 2024 and due to be opened in September 2025.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. The calculation mirrors the approach taken for basic need funding allocations published in March 2025. It includes mainstream primary and secondary free schools which opened in September 2024 and those with a high degree of certainty of opening in September 2025, and counts the total number of places which will be in use by September 2026.
+&lt;br&gt;2. The data does not include free schools which opened before September 2024, as they will already be included in SCAP24 and are therefore existing places. It does not include free schools which are planned to open in the academic year 2026/27 and beyond. </t>
+  </si>
+  <si>
+    <t>4. Reduction in places from free school and academy closures between May 2024 and January 2025 or identified/confirmed to close before August 2025.</t>
+  </si>
+  <si>
+    <t>1. Where an academy or free school closed after 1 May 2024 its capacity, as reported in the School Capacity data, is now no longer available. Their capacity has therefore been removed from the planned delivery total.</t>
   </si>
   <si>
     <t>5. Total number of planned places (sum of 1, 2, 3, and 4 above)</t>
   </si>
   <si>
-    <t>2. Pupil Numbers for the 2014/15 academic year taken from the pupil census in January 2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3. Pupil Numbers for the 2018/19 academic year taken from the pupil census in January 2019
-</t>
-  </si>
-  <si>
-    <t>4. Pupil Numbers for the 2024/25 academic year taken from the pupil census in January 2025</t>
-  </si>
-  <si>
-    <t>5. Forecast pupil numbers for the 2026/27 academic year</t>
+    <t xml:space="preserve">1. This measure reports planned increases in capacity only. If there is a total net planned reduction in capacity (e.g. due to a free school closure), this is shown as zero places planned. Therefore the sum of local authority-level figures will not equal the national planned places figure.
+&lt;br&gt;2. Most local authorities will have further developed their plans since this data was reported in Summer 2024, and so although it allows for comparisons between local authorities, the figure is likely to be an understatement of the current position. </t>
   </si>
   <si>
     <t>1.This relates to the academic year 2026/27 and is the difference between local authority pupil forecasts and future capacity, taking account of planned future additions and places to remove.
@@ -476,12 +740,167 @@
 &lt;br&gt;8. Estimates for spare places are presented as a percentage of total future capacity.</t>
   </si>
   <si>
-    <t>1. Number of new school places created
-2. Quality of new places created as judged by key stage 2 progress measures</t>
-  </si>
-  <si>
-    <t>1. Number of new school places created
-2. Quality of new places created as judged by key stage 4 progress 8 measure</t>
+    <t xml:space="preserve">1. This refers to the amount of basic need capital funding that the Department for Education (DfE) has allocated to each local authority to create new places from the 2011-12 financial year to the 2025-26 financial year. Basic Need funding for the 2025-26 financial year is intended to support the creation of mainstream places for pupils aged 5 to 16 for the 2026/27 academic year. &lt;br&gt;2. The figure includes formula-based funding allocations and funding provided through the Targeted Basic Need Programme. Basic Need formula-based funding allocations cover the whole period and are not ring-fenced (although they can only be used for capital purposes).  Targeted Basic Need funding was provided between 2013 and 2015 and had to be spent by agreed deadlines and on specific projects. Both types of allocations are published here. &lt;br&gt;3. The figure only includes funding allocated to local authorities and does not include centrally-funded capital programmes such as the free schools programme. &lt;br&gt;4. The England total will not match the sum of allocations for all local authorities in the scorecard because the England total includes allocations to predecessor local authorities.
+</t>
+  </si>
+  <si>
+    <t>2. Pupil Numbers for the 2014/15 academic year taken from the pupil census in January 2015</t>
+  </si>
+  <si>
+    <t>School census Jan 2015 data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Number of pupils in roll in January 2015, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Pupil Numbers for the 2018/19 academic year taken from the pupil census in January 2019
+</t>
+  </si>
+  <si>
+    <t>School census Jan 2019 data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Number of pupils in roll in January 2019, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. </t>
+  </si>
+  <si>
+    <t>4. Pupil Numbers for the 2024/25 academic year taken from the pupil census in January 2025</t>
+  </si>
+  <si>
+    <t>School census Jan 2025 data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Number of pupils in roll in January 2025, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. 							</t>
+  </si>
+  <si>
+    <t>5. Forecast pupil numbers for the 2026/27 academic year</t>
+  </si>
+  <si>
+    <t>Local authority data provided through the  School Capacity (SCAP) Collection 2024</t>
+  </si>
+  <si>
+    <t>1. This is the local authority's forecast of pupil numbers for the academic year 2026/27 as provided in SCAP 2024.
+2. These forecasts cover pupils that local authorities anticipate will attend primary schools (or primary provision in middle or all-through schools i.e. years R-6) and secondary schools (or secondary provision in middle or all-through schools i.e. years 7-11)
+3. These forecasts focus on local authorities expectations about new school places and do not include pupils who are expected to attend independent schools or special/non-mainstream provision.</t>
+  </si>
+  <si>
+    <t>Total places created between May 2010 and May 2024</t>
+  </si>
+  <si>
+    <t>Places planned to 2026/27</t>
+  </si>
+  <si>
+    <t>Number of new places planned for delivery between May 2024 and September 2026;
+&lt;br&gt;This contains: 
+&lt;br&gt;1) local authority firm plans for new permanent additional places , new temporary bulge places and the removal of places,
+&lt;br&gt;2) capacity changes through the Condition Improvement Fund (CIF), School Rebuilding Programme (SRP), Selective Schools Expansion Fund (SSEF), and Voluntary Aided Schools Fund (VA)
+&lt;br&gt;3) places from free schools opened in September 2024 and planned to open in September 2025
+&lt;br&gt;4) reduction in places from free school and academy closures.</t>
+  </si>
+  <si>
+    <t>Unfilled places in 2023/24</t>
+  </si>
+  <si>
+    <t>Additional places needed in 2026/27; spare places in 2026/27</t>
+  </si>
+  <si>
+    <t>Estimated number of additional places needed to meet demand in 2026/27; estimated percentage of spare places in 2026/27.</t>
+  </si>
+  <si>
+    <t>Total basic need funding 2011 to 2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total amount of basic need capital funding allocated to each local authority to support them to create new mainstream primary and secondary places from 2011 to 2026. </t>
+  </si>
+  <si>
+    <t>Change in pupil numbers
+2009/10 to 2024/25; Anticipated change in pupil numbers 2024/25 to 2026/27</t>
+  </si>
+  <si>
+    <t>The actual percentage change in pupil numbers between 2009/10, 2014/15 (for secondary), 2018/19 (for primary) and 2024/25; the anticipated percentage change in pupil numbers in primary or secondary state-funded mainstream provision between the 2024/25 and 2026/27 academic years.</t>
+  </si>
+  <si>
+    <t>2023/24</t>
+  </si>
+  <si>
+    <t>Forecast accuracy of pupil projections for 2024/25</t>
+  </si>
+  <si>
+    <t>The one year ahead local authority forecast accuracy. It compares actual numbers on roll in 2024/25 with forecasts of pupil numbers for 2024/25 made one year previously (in SCAP 2024)</t>
+  </si>
+  <si>
+    <t>1. Forecasts of academic year 2024/25 pupil numbers made in 2023/24.</t>
+  </si>
+  <si>
+    <t>Local authority data provided through the School Capacity (SCAP) Collection 2024</t>
+  </si>
+  <si>
+    <t>1. Forecasts, submitted by local authorities for SCAP24 , at planning area level and aggregated to local authority level. Forecasts include pupils expected to be educated in new schools (or expanded schools) funded through Housing Developer Contributions (HDC) and Housing Infrastructure Fund (HIF) agreements.
+&lt;br&gt;2. Actual pupil numbers on roll for academic year 2024/25 are taken from the January school census and aggregated to local authority level. They include pupils in roll, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. &lt;br&gt;3. Forecast accuracy is calculated by  subtracting the years R-6 actual numbers from the years R-6 forecasts to give the absolute inaccuracy. Absolute inaccuracy is then divided by the R-6 actual number to give the relative percentage inaccuracy. The same is done for secondary using years 7-11. 
+&lt;br&gt;4.  Scorecard figures may differ to those published in SCAP due to the exclusion of years 12 to 14 in the pupil numbers and forecasts used in the scorecard.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Actual pupil numbers on roll in academic year 2024/25.
+</t>
+  </si>
+  <si>
+    <t>Pupils in school provided through the January 2025 School Census</t>
+  </si>
+  <si>
+    <t>The three year ahead forecast accuracy compares actual pupil numbers on roll with forecasts of pupil numbers for 2024/25 made three years previously (in SCAP 2022) by local authority).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Forecasts of academic year 2024/25 pupil numbers made in 2021/22.
+</t>
+  </si>
+  <si>
+    <t>Local authority data provided through the School Capacity (SCAP) Collection 2022</t>
+  </si>
+  <si>
+    <r>
+      <t>1. Forecasts, submitted by local authorities</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>as part of the SCAP 2022, at planning area level and aggregated to local authority level. Forecasts include pupils expected to be educated in new schools (or expanded schools) funded through HDC and HIF agreements.
+&lt;br&gt;2. Actual pupil numbers on roll for academic year 2024/25 are taken from the January school census and aggregated to local authority level. They include pupils in roll, including dual registrations, in reception to year 11 in the following types of schools: Academy converter, Academy sponsor led, City technology college. Community school, Foundation school, Free schools, Studio schools, University technical college, Voluntary aided school, Voluntary controlled school. 	&lt;br&gt;3. Forecast accuracy is calculated by subtracting the years R-6 actual numbers from the years R-6 forecasts to give the absolute inaccuracy. Absolute inaccuracy is then divided by the R-6 actual number to give the relative percentage inaccuracy. The same is done for secondary using years 7-11. 
+&lt;br&gt;4.  Scorecard figures may differ to those published in SCAP due to the exclusion of years 12 to 14 in the pupil numbers and forecasts used in the scorecard.</t>
+    </r>
+  </si>
+  <si>
+    <t>2. Actual pupil numbers on roll in academic year 2024/25.</t>
+  </si>
+  <si>
+    <t>School place offers by preference for September 2025 entry</t>
+  </si>
+  <si>
+    <t>The proportion of applicants who received an offer of a place in one of their top three preference schools for September 2025 on national offer day</t>
+  </si>
+  <si>
+    <t>Published School Applications and Offer data 2025/26 Academic Year</t>
+  </si>
+  <si>
+    <t>Quality of new school places created between academic year 2022/23 and 2023/24, based on Ofsted rating</t>
+  </si>
+  <si>
+    <t>The number of new places created between academic year 2022/23 and academic year 2023/24</t>
+  </si>
+  <si>
+    <t>Capacity of each school in May 2023</t>
   </si>
   <si>
     <t>1. The following school types, identified using Get Information About Schools, have been excluded:
@@ -500,11 +919,60 @@
 &lt;br&gt;10. The quality measures represent the window in time when places were added and this is not necessarily the same quality outcome as when the decision to add places was taken.</t>
   </si>
   <si>
+    <t>Capacity for each school in May 2024</t>
+  </si>
+  <si>
+    <t>Local authority data, provided through School Capacity collection 2024</t>
+  </si>
+  <si>
+    <t>Quality of school places created between academic year 2022/23 and academic year 2023/24, based on Ofsted rating. The quality of existing school places (places in 2023/24 which were also present in 2022/23) is shown for context.</t>
+  </si>
+  <si>
+    <t>1. Each school has been matched with the Ofsted judgement of 'Overall effectiveness: how good is the school." as at 31 August 2024 (published November 2024).
+&lt;br&gt;2. There are four Ofsted categories: 'Outstanding', 'Good', 'Requires improvement' and 'Inadequate'.
+&lt;br&gt;3. The calculation counts the number of existing and new places that have been created in schools of each category. &lt;br&gt;4. Note that many schools will have been inspected some time before August 2024, and some will have been inspected since this date. &lt;br&gt;5. There are school places with no rating, as the school has yet to be inspected so do not have an Ofsted judgement.</t>
+  </si>
+  <si>
+    <t>Percentage of new places created in good and outstanding schools between academic year 2022/23 and academic year 2023/24.</t>
+  </si>
+  <si>
+    <t>The quality of school places created between academic year 2022/23 and academic year 2023/24, and the quality of existing school places. Based on key stage 2 progress measures</t>
+  </si>
+  <si>
+    <t>Quality of new school places created between academic year 2022/23 and 2023/24, based on key stage 2 progress measures</t>
+  </si>
+  <si>
     <t xml:space="preserve">1. Each school has been matched with the key stage 2 progress measure for reading and maths, for academic year ending July 2023 (published December 2023). It was not be possible to calculate KS1-KS2 progress measures for the 2023/24 academic year, because there is no relevant KS1 data required to calculate KS1-KS2 progress measures for these cohorts, as primary tests and assessments were cancelled in academic years 2019/20 and 2020/21 due to COVID-19 disruption.
 2. This measure judges schools’ performance as 'well above average', 'above average', 'average', 'below average' or 'well below average'.
 3. The calculation counts the number of new school places that have been created in schools of each category; and the number of existing school places in each category.
 4. Middle schools may not have a key stage 2 measure and if they do, due to the age range of pupils at middle schools, pupils will have only attended a middle school for a short time before they take their key stage 2 tests and will still have a number of years left at the school. This should be taken into account when comparing their results to schools which start educating their pupils from the beginning of key stage 1.  New schools may not have a key stage 2 measure until the first cohort of pupils reaches year 6.
 5. For further information on key stage 2 progress measures please use the following url: https://www.gov.uk/government/collections/school-performance-tables-about-the-data </t>
+  </si>
+  <si>
+    <t>The quality of school places created between academic year 2022/23 and academic year 2023/24, and the quality of existing school places. Based on key stage 4 progress 8 measure</t>
+  </si>
+  <si>
+    <t>Quality of new school places created between academic year 2022/23 and 2023/24, based on key stage 4 progress 8 measure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Each school has been matched with the key stage 4 progress 8 measure across 8 key subjects, for academic year ending July 2024 (published February 2025).
+2. This measure judges schools’ performance as 'well above average', 'above average', 'average', 'below average' or 'well below average'.
+3. The calculation counts the number of new school places that have been created in schools of each category; and the number of existing school places in each category.
+4. Note that middle schools will not have a key stage 4 measure, and that new schools may not have a key stage 4 measure until the first cohort of pupils reaches year 11.
+5. Note that this progress 8 measure is not a strict measure of the effectiveness of the entire school as a school may add value before pupils take the key stage tests. 
+6. For further information on progress 8 measure please use the following url: https://www.gov.uk/government/collections/school-performance-tables-about-the-data 
+</t>
+  </si>
+  <si>
+    <t>Percentage of new places created in well above and above-average schools between academic year 2022/23 and academic year 2023/24.</t>
+  </si>
+  <si>
+    <t>1. Number of new school places created
+2. Quality of new places created as judged by key stage 2 progress measures</t>
+  </si>
+  <si>
+    <t>1. Number of new school places created
+2. Quality of new places created as judged by key stage 4 progress 8 measure</t>
   </si>
   <si>
     <t xml:space="preserve">The national average has been adjusted to the relevant region for each local authority, using the Building Cost Information Service (BCIS) March 2023 published regional location factors. The England national average has been multiplied by the relevant regional location factor:  East Midlands: 1.03, East of England 0.99, Inner London: 1.29, North East: 0.91, North West: 1, Outer London: 1.21, South East: 1.13, South West: 1.01, West Midlands: 0.96, Yorkshire &amp; the Humber: 0.91. </t>
@@ -983,9 +1451,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF104F75"/>
-      </left>
+      <left/>
       <right style="dotted">
         <color auto="1"/>
       </right>
@@ -996,13 +1462,13 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="dotted">
-        <color auto="1"/>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
       </right>
-      <top style="dotted">
-        <color auto="1"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -1011,7 +1477,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1035,6 +1501,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1062,15 +1531,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1080,7 +1549,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
@@ -1131,9 +1606,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1149,28 +1621,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1488,10 +1964,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8372DA64-5E2C-41C1-8CF4-85BC1C2AFF86}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView topLeftCell="C11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1503,7 +1979,7 @@
     <col min="5" max="5" width="87.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1519,13 +1995,16 @@
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F1" s="51" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="42" t="s">
-        <v>38</v>
+      <c r="B2" s="44" t="s">
+        <v>34</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>2</v>
@@ -1533,211 +2012,483 @@
       <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="44" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
-      <c r="B3" s="43"/>
+      <c r="B3" s="45"/>
       <c r="C3" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="43"/>
-    </row>
-    <row r="4" spans="1:5" ht="138" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="45"/>
+      <c r="F3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="138" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
-      <c r="B5" s="46"/>
+      <c r="B5" s="48"/>
       <c r="C5" s="6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="E5" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="12" t="s">
+      <c r="B6" s="48"/>
+      <c r="C6" s="13" t="s">
         <v>44</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="E6" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="12" t="s">
+      <c r="B7" s="48"/>
+      <c r="C7" s="13" t="s">
         <v>45</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="22"/>
+      <c r="D9" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="375" x14ac:dyDescent="0.25">
+      <c r="A10" s="32" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="12" t="s">
+      <c r="B10" s="13" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="375" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>54</v>
       </c>
       <c r="C10" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="22" t="s">
-        <v>35</v>
+      <c r="D10" s="23" t="s">
+        <v>99</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="F10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" s="13"/>
+        <v>52</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="14"/>
       <c r="D11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="11" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="50" t="s">
+      <c r="D13" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="47" t="s">
-        <v>93</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="10" t="s">
+      <c r="E13" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="46" t="s">
+        <v>110</v>
+      </c>
+      <c r="F15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E16" s="45"/>
+      <c r="F16" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B17" s="47" t="s">
+        <v>139</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="F17" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="51"/>
-      <c r="B13" s="48"/>
-      <c r="C13" s="10" t="s">
+      <c r="D18" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="F18" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="F19" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="F20" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="8"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="F21" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B22" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="22"/>
+      <c r="D22" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="375" x14ac:dyDescent="0.25">
+      <c r="A23" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="D13" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="51"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="51"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="52"/>
-      <c r="B16" s="49"/>
-      <c r="C16" s="27" t="s">
-        <v>102</v>
-      </c>
-      <c r="D16" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" s="27" t="s">
-        <v>62</v>
+      <c r="E23" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="F23" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="C24" s="14"/>
+      <c r="D24" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="F24" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="52" t="s">
+        <v>145</v>
+      </c>
+      <c r="B25" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="54"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="F26" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="54"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="F27" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="54"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="F28" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="56"/>
+      <c r="B29" s="57"/>
+      <c r="C29" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="E29" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="F29" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="B25:B29"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="B4:B8"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="E15:E16"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <hyperlinks>
@@ -1745,131 +2496,229 @@
     <hyperlink ref="D10" r:id="rId2" display=" 2021/22 school place planning published underlying data. " xr:uid="{093B09C6-85AC-4B03-8BE4-078C82660B4C}"/>
     <hyperlink ref="D2" r:id="rId3" xr:uid="{8150C38D-D188-4C8E-86C3-B5575B8FFEE8}"/>
     <hyperlink ref="D11" r:id="rId4" xr:uid="{84C17436-4B87-48EB-BAE5-31DBACCBDB31}"/>
-    <hyperlink ref="D15" r:id="rId5" display="School census Jan 2023 data" xr:uid="{B4335ED1-45C2-43A8-BAE4-D6C4C7E179D0}"/>
+    <hyperlink ref="D13" r:id="rId5" display="School census Jan 2023 data" xr:uid="{B4335ED1-45C2-43A8-BAE4-D6C4C7E179D0}"/>
     <hyperlink ref="D12" r:id="rId6" xr:uid="{CCB6838D-DD36-44DD-BC08-5E652C942FA3}"/>
     <hyperlink ref="D9" r:id="rId7" display="Local authority data provided through School Capacity (SCAP) Survey 2021" xr:uid="{F7517439-C801-46CD-8DC3-B6DD58F4289A}"/>
-    <hyperlink ref="D16" r:id="rId8" display="Local authority data provided through the  School Capacity (SCAP) Collection 2022" xr:uid="{2257ADC3-56E0-46AA-984A-65A14B6B91D4}"/>
-    <hyperlink ref="D13" r:id="rId9" xr:uid="{79AE5929-1652-4611-9E48-29269254E396}"/>
-    <hyperlink ref="D14" r:id="rId10" xr:uid="{4D3E4206-3C34-46F2-94BA-63E9C87A86E9}"/>
+    <hyperlink ref="D14" r:id="rId8" display="Local authority data provided through the  School Capacity (SCAP) Collection 2022" xr:uid="{2257ADC3-56E0-46AA-984A-65A14B6B91D4}"/>
+    <hyperlink ref="D17" r:id="rId9" display="Local authority data provided through the School Capacity (SCAP) Survey 2022." xr:uid="{D140B5FC-6CE2-48F1-BF21-C9EC2586782D}"/>
+    <hyperlink ref="D23" r:id="rId10" display=" 2021/22 school place planning published underlying data. " xr:uid="{168FA84B-11B4-4C80-A7A5-597B690A65BF}"/>
+    <hyperlink ref="D15" r:id="rId11" xr:uid="{D7EB4574-CB25-42A9-B4C2-3913F62B5513}"/>
+    <hyperlink ref="D24" r:id="rId12" xr:uid="{3D41CC56-05BA-471B-ABB1-3CB74AC2778A}"/>
+    <hyperlink ref="D28" r:id="rId13" display="School census Jan 2023 data" xr:uid="{F0889FF8-A60B-411C-A004-D5DA89758A71}"/>
+    <hyperlink ref="D25" r:id="rId14" xr:uid="{57A1343E-B39E-429E-94B0-FD3C6471C21E}"/>
+    <hyperlink ref="D22" r:id="rId15" display="Local authority data provided through School Capacity (SCAP) Survey 2021" xr:uid="{4E4AE6EF-3D53-4105-97A1-065AADC66650}"/>
+    <hyperlink ref="D29" r:id="rId16" display="Local authority data provided through the  School Capacity (SCAP) Collection 2022" xr:uid="{712DF8AA-676E-41AB-BBBE-2AB832B676D0}"/>
+    <hyperlink ref="D26" r:id="rId17" xr:uid="{506A2691-ED47-412F-A8C0-7648AE09BFD7}"/>
+    <hyperlink ref="D27" r:id="rId18" xr:uid="{CC0BA90D-BAE6-4C2F-9262-0D1CAD7283ED}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C67D23D-5B13-4F00-9F83-043839CEFFD1}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="55.42578125" style="31"/>
+    <col min="1" max="16384" width="55.42578125" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="31" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="F1" s="31" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="32"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D3" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="50"/>
+      <c r="F3" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="32"/>
+      <c r="B4" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="45" t="s">
+      <c r="C4" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="47" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="300.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="54"/>
-      <c r="C3" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="E3" s="54"/>
-    </row>
-    <row r="4" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="29"/>
-      <c r="B4" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="12" t="s">
+      <c r="F4" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="39"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="E4" s="45" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="272.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="36"/>
-      <c r="B5" s="53"/>
-      <c r="C5" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="D5" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="E5" s="53"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="E6" s="47" t="s">
+        <v>152</v>
+      </c>
+      <c r="F6" s="34" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="32"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="D7" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="E7" s="50"/>
+      <c r="F7" s="34" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="32"/>
+      <c r="B8" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" s="38" t="s">
+        <v>157</v>
+      </c>
+      <c r="E8" s="47" t="s">
+        <v>158</v>
+      </c>
+      <c r="F8" s="34" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="39"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="D9" s="40" t="s">
+        <v>154</v>
+      </c>
+      <c r="E9" s="49"/>
+      <c r="F9" s="34" t="s">
+        <v>147</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="E8:E9"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="E2:E3"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="E6:E7"/>
   </mergeCells>
+  <phoneticPr fontId="9" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="Local authority data provided through the School Capacity (SCAP) Collection 2022" xr:uid="{D14A8E59-0240-4725-B7AC-4582058C6B59}"/>
-    <hyperlink ref="D4" r:id="rId2" display="Local authority data provided through the School Capacity (SCAP) Collection 2021" xr:uid="{586F3224-6D8F-4AF9-899D-550CFDC0058F}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{586F3224-6D8F-4AF9-899D-550CFDC0058F}"/>
     <hyperlink ref="D3" r:id="rId3" display="Pupils in school provided through the January 2023 School Census" xr:uid="{17405BAA-EC5B-41A8-9F2F-BBE920A0B9BB}"/>
     <hyperlink ref="D5" r:id="rId4" display="Pupils in school provided through the January 2023 School Census" xr:uid="{54B0E578-7E98-4CE5-8BEB-25623CA0296D}"/>
+    <hyperlink ref="D6" r:id="rId5" display="Local authority data provided through the School Capacity (SCAP) Collection 2022" xr:uid="{F94E27B9-93F2-492F-B022-03D1BF2ED50B}"/>
+    <hyperlink ref="D8" r:id="rId6" display="Local authority data provided through the School Capacity (SCAP) Collection 2021" xr:uid="{DB6C9518-4974-4D88-A3FD-A0D73E1156DA}"/>
+    <hyperlink ref="D7" r:id="rId7" display="Pupils in school provided through the January 2023 School Census" xr:uid="{D4EB79EF-B53B-4F30-A202-85F4FBDCA5DB}"/>
+    <hyperlink ref="D9" r:id="rId8" display="Pupils in school provided through the January 2023 School Census" xr:uid="{A8F94BE9-CA43-4F91-A3C7-D2BD25322736}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3163888B-9214-4218-82C5-5CD72F2D39D0}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="48.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1885,41 +2734,88 @@
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="197.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="F1" s="31" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="E2" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="C3" s="13"/>
+      <c r="D3" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>16</v>
+      <c r="E3" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="58" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="58" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="Published School Applications and Offer data 2022/23 Academic Year" xr:uid="{65C563AA-E96A-4DA3-9BD3-0A919A6BB712}"/>
     <hyperlink ref="D3" r:id="rId2" display="Published School Applications and Offer data 2022/23 Academic Year" xr:uid="{73E1A89E-78ED-4859-B41E-1AE6B97802E3}"/>
+    <hyperlink ref="D4" r:id="rId3" display="Published School Applications and Offer data 2022/23 Academic Year" xr:uid="{DEAC6B57-4AAA-46A4-8F99-7C21A4EAB388}"/>
+    <hyperlink ref="D5" r:id="rId4" display="Published School Applications and Offer data 2022/23 Academic Year" xr:uid="{1A8CD594-5A7A-4EBE-87C4-EDF4055AC3CF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1927,165 +2823,388 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{172A91E8-EE08-4774-802F-E9F4C78EAB63}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="37.28515625" style="31"/>
-    <col min="5" max="5" width="77.28515625" style="31" customWidth="1"/>
-    <col min="6" max="16384" width="37.28515625" style="31"/>
+    <col min="1" max="4" width="37.28515625" style="34"/>
+    <col min="5" max="5" width="77.28515625" style="34" customWidth="1"/>
+    <col min="6" max="16384" width="37.28515625" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="31" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="F1" s="31" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="C2" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="12" t="s">
+      <c r="F2" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="41"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="39"/>
-    </row>
-    <row r="4" spans="1:5" ht="150" x14ac:dyDescent="0.25">
-      <c r="A4" s="38"/>
-      <c r="B4" s="40" t="s">
+      <c r="E3" s="42"/>
+      <c r="F3" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A4" s="41"/>
+      <c r="B4" s="43" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="F4" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="255" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="240" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="F8" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="F10" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="D13" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="F13" s="34" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="41"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="D14" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="E14" s="42"/>
+      <c r="F14" s="34" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A15" s="41"/>
+      <c r="B15" s="43" t="s">
+        <v>169</v>
+      </c>
+      <c r="C15" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D15" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="12" t="s">
+      <c r="E15" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="F15" s="34" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="34" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="315" x14ac:dyDescent="0.25">
+      <c r="A17" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="315" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="240" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="12" t="s">
+      <c r="E17" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="F17" s="34" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="240" x14ac:dyDescent="0.25">
+      <c r="A18" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="C18" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="12" t="s">
-        <v>34</v>
+      <c r="D18" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="F18" s="34" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="D19" s="28"/>
+      <c r="E19" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F19" s="34" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="D20" s="28"/>
+      <c r="E20" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="F20" s="34" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="Local authority data, provided through School Capacity collection 2022" xr:uid="{6EE32724-1837-46BD-9FD6-A4EEFD1E0A4A}"/>
-    <hyperlink ref="D3" r:id="rId2" display="Local authority data, provided through School Capacity collection 2023" xr:uid="{F8935CE3-E46D-430A-A5BC-BAB4A254BDA2}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{6EE32724-1837-46BD-9FD6-A4EEFD1E0A4A}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{F8935CE3-E46D-430A-A5BC-BAB4A254BDA2}"/>
     <hyperlink ref="D4" r:id="rId3" xr:uid="{2FB89BF4-390E-4CD5-92FB-FD0FF31F028D}"/>
-    <hyperlink ref="D6" r:id="rId4" xr:uid="{4534F643-19C4-4655-8095-8044AC4B7902}"/>
-    <hyperlink ref="D7" r:id="rId5" xr:uid="{4889CA3C-1157-412C-ACB1-EE5DA00A90DF}"/>
+    <hyperlink ref="D7" r:id="rId4" xr:uid="{4534F643-19C4-4655-8095-8044AC4B7902}"/>
+    <hyperlink ref="D8" r:id="rId5" xr:uid="{4889CA3C-1157-412C-ACB1-EE5DA00A90DF}"/>
+    <hyperlink ref="D13" r:id="rId6" display="Local authority data, provided through School Capacity collection 2022" xr:uid="{73725C21-EC8E-495A-8521-6604BDCA9BF5}"/>
+    <hyperlink ref="D14" r:id="rId7" display="Local authority data, provided through School Capacity collection 2023" xr:uid="{3107590D-6B8F-4322-8365-F40271488FAC}"/>
+    <hyperlink ref="D15" r:id="rId8" xr:uid="{169006D7-2497-4BE8-90DB-4A1783604C5F}"/>
+    <hyperlink ref="D17" r:id="rId9" xr:uid="{6D9BDEC1-A85B-4BAE-B25C-DC97AE840965}"/>
+    <hyperlink ref="D18" r:id="rId10" xr:uid="{D90B4F41-BA2F-44BC-AA85-E0C3BEF1F585}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2093,94 +3212,115 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB73E146-A141-4797-B302-F0B3455C0C2E}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="57.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="57.5703125" style="31"/>
+    <col min="1" max="16384" width="57.5703125" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="31" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="14" t="s">
+      <c r="F1" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="14" t="s">
+    </row>
+    <row r="2" spans="1:6" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="34" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="41"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="18"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="17"/>
+    <row r="3" spans="1:6" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="18"/>
       <c r="C4" s="19"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="17"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="18"/>
       <c r="C5" s="19"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="17"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="18"/>
       <c r="C6" s="19"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="17"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="18"/>
       <c r="C7" s="19"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="17"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="18"/>
       <c r="C8" s="19"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="17"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="18"/>
       <c r="C9" s="19"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="17"/>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="18"/>
       <c r="C10" s="19"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="17"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="18"/>
       <c r="C11" s="19"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="17"/>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="18"/>
       <c r="C12" s="19"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="17"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="18"/>
       <c r="C13" s="19"/>
     </row>
   </sheetData>
@@ -2190,6 +3330,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="ec07c698-60f5-424f-b9af-f4c59398b511" ContentTypeId="0x010100545E941595ED5448BA61900FDDAFF313" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Official Document" ma:contentTypeID="0x010100545E941595ED5448BA61900FDDAFF31300C0D9F77D091A79449828113EF8250EF5" ma:contentTypeVersion="9" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="3acf8af8f3f036fb6d934619e757bc96">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8c566321-f672-4e06-a901-b5e72b4c4357" xmlns:ns3="2a6436df-3f7a-48ac-8ea6-44b411e24bbc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="926947be84ee9a0228ce6a037c6848ba" ns2:_="" ns3:_="">
     <xsd:import namespace="8c566321-f672-4e06-a901-b5e72b4c4357"/>
@@ -2395,7 +3540,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="8c566321-f672-4e06-a901-b5e72b4c4357">
@@ -2440,7 +3585,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2449,7 +3594,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -2499,12 +3644,15 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="ec07c698-60f5-424f-b9af-f4c59398b511" ContentTypeId="0x010100545E941595ED5448BA61900FDDAFF313" PreviousValue="false"/>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D00F0DC4-2D9F-43FC-8616-EC131ED26B7D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1E94FF3-D2F7-4169-BE5C-5ED202BAA024}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2523,24 +3671,24 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{334E8BC2-6B82-4EDA-BE50-EFE4767E8CD2}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="8c566321-f672-4e06-a901-b5e72b4c4357"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8c566321-f672-4e06-a901-b5e72b4c4357"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="2a6436df-3f7a-48ac-8ea6-44b411e24bbc"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{035EEA42-582A-4724-B162-C22729062C2B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -2548,18 +3696,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9C56A4F-6917-41AA-BBE5-DA7C75896563}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D00F0DC4-2D9F-43FC-8616-EC131ED26B7D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>